<commit_message>
code change for View 100
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55651C\Documents\UiPath\P0002_090_PayCyleAfternoon_Performer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55651C\Documents\GitHub\P0002_090_PayCyleAfternoon_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9536B7E-20F3-4C63-A5AD-B2A999AA6853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605338B5-595E-4CE4-8F70-04AE3B499915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="593">
   <si>
     <t>Name</t>
   </si>
@@ -99,11 +99,11 @@
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="20"/>
+    <phoneticPr fontId="21"/>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="20"/>
+    <phoneticPr fontId="21"/>
   </si>
   <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
@@ -1021,9 +1021,6 @@
     <t>PaycycleResultList</t>
   </si>
   <si>
-    <t>All Paycycle Result list items will be processed now.</t>
-  </si>
-  <si>
     <t>CompletedStatusDelay</t>
   </si>
   <si>
@@ -1426,15 +1423,9 @@
     <t>SharepointURL</t>
   </si>
   <si>
-    <t>https://officemgmtentserv.sharepoint.com/sites/ACOE_Automations</t>
-  </si>
-  <si>
     <t>SharepointSubFolder</t>
   </si>
   <si>
-    <t>P002_090_PayCyleAfternoon</t>
-  </si>
-  <si>
     <t>FolderNameYear</t>
   </si>
   <si>
@@ -1681,9 +1672,6 @@
     <t>StatusCreatedDidNotAppear</t>
   </si>
   <si>
-    <t>00:00:04</t>
-  </si>
-  <si>
     <t>DefaultExcelSheetName</t>
   </si>
   <si>
@@ -1730,12 +1718,6 @@
   </si>
   <si>
     <t>Hello RPA Support Team,&lt;br&gt;&lt;br&gt;This email notification was raised for process P002_090_PayCycleAfternoon. The process execution met a System exception, details for which can be found below:&lt;br&gt;&lt;br&gt;Exception Message: Excp_Message&lt;br&gt;&lt;br&gt; Thanks,&lt;br&gt;Automation Team</t>
-  </si>
-  <si>
-    <t>Workflow to Approve all records in paycycle has a business exception.</t>
-  </si>
-  <si>
-    <t>ApproveAllRecordsWorkflowBE</t>
   </si>
   <si>
     <t>StatusCompletedNotAppearedBE_1</t>
@@ -1773,6 +1755,69 @@
   </si>
   <si>
     <t>System Exception has occurred for the paycycle.</t>
+  </si>
+  <si>
+    <t>ApproveRecordsCheckCompletedStatusWorkflowStarted</t>
+  </si>
+  <si>
+    <t>ApproveRecordsCheckCompletedStatusWorkflowCompleted</t>
+  </si>
+  <si>
+    <t>ApproveRecordsCheckCompletedStatusWorkflowSE</t>
+  </si>
+  <si>
+    <t>ApproveRecordsCheckCompletedStatusWorkflowBE</t>
+  </si>
+  <si>
+    <t>ArrowButtonFound</t>
+  </si>
+  <si>
+    <t>ArrowButtonNotFound</t>
+  </si>
+  <si>
+    <t>ArrowButtonNotFoundSE</t>
+  </si>
+  <si>
+    <t>Arrow button for next page was found.</t>
+  </si>
+  <si>
+    <t>Arrow button for next page not found.</t>
+  </si>
+  <si>
+    <t>NonWorkingDaysErrorMessage</t>
+  </si>
+  <si>
+    <t>Non Working Days have not been defined in the calender.</t>
+  </si>
+  <si>
+    <t>Long delay for where ever needed</t>
+  </si>
+  <si>
+    <t>https://officemgmtentserv.sharepoint.com/sites/ACOE_Automations_DEV</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon</t>
+  </si>
+  <si>
+    <t>00:00:50</t>
+  </si>
+  <si>
+    <t>All Paycycle Result list items are processed now.</t>
+  </si>
+  <si>
+    <t>Workflow to Approve Records and Check Completed Status in paycycle is started.</t>
+  </si>
+  <si>
+    <t>Workflow to Approve Records and Check Completed Status in paycycle is completed successfully.</t>
+  </si>
+  <si>
+    <t>Workflow to Approve Records and Check Completed Status in paycycle has a system exception.</t>
+  </si>
+  <si>
+    <t>Workflow to Approve Records and Check Completed Status in paycycle has a business exception.</t>
+  </si>
+  <si>
+    <t>CompletedStatusRefreshButtonDelay</t>
   </si>
 </sst>
 </file>
@@ -1782,11 +1827,18 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2003,52 +2055,53 @@
   </borders>
   <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="4" fontId="25" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="4" fontId="26" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="1"/>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="1"/>
@@ -2394,10 +2447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z128"/>
+  <dimension ref="A1:Z129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -2458,7 +2511,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>29</v>
@@ -2469,7 +2522,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>21</v>
@@ -2488,57 +2541,57 @@
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
+        <v>413</v>
+      </c>
+      <c r="B6" t="s">
         <v>414</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="4" t="s">
         <v>415</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B7" t="s">
         <v>417</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="4" t="s">
         <v>418</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
+        <v>419</v>
+      </c>
+      <c r="B8" t="s">
         <v>420</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="4" t="s">
         <v>421</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B9" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B10" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -2623,7 +2676,7 @@
         <v>58</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="C18" t="s">
         <v>59</v>
@@ -2645,7 +2698,7 @@
         <v>63</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="C20" t="s">
         <v>64</v>
@@ -2667,7 +2720,7 @@
         <v>68</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="C22" t="s">
         <v>69</v>
@@ -2733,7 +2786,7 @@
         <v>85</v>
       </c>
       <c r="B28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C28" t="s">
         <v>86</v>
@@ -2788,7 +2841,7 @@
         <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C33" t="s">
         <v>99</v>
@@ -2796,7 +2849,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B34" t="s">
         <v>100</v>
@@ -2927,7 +2980,7 @@
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="21" t="s">
+      <c r="A46" s="23" t="s">
         <v>130</v>
       </c>
       <c r="B46">
@@ -2938,24 +2991,26 @@
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="20" t="s">
+      <c r="A47" s="19" t="s">
         <v>132</v>
       </c>
       <c r="B47">
         <v>2</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="22" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="19" t="s">
-        <v>456</v>
+      <c r="A48" s="24" t="s">
+        <v>455</v>
       </c>
       <c r="B48">
         <v>10</v>
       </c>
-      <c r="C48" s="5"/>
+      <c r="C48" s="22" t="s">
+        <v>583</v>
+      </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="5" t="s">
@@ -3024,7 +3079,7 @@
         <v>317</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>547</v>
+        <v>586</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -3032,7 +3087,7 @@
         <v>229</v>
       </c>
       <c r="B57">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -3053,7 +3108,7 @@
         <v>230</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -3062,7 +3117,7 @@
       </c>
       <c r="B61" t="str">
         <f ca="1">TEXT(TODAY(), "yyyy-mm-dd")</f>
-        <v>2024-01-12</v>
+        <v>2024-01-16</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -3099,7 +3154,7 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="14" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B66" t="s">
         <v>261</v>
@@ -3107,10 +3162,10 @@
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="14" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B67" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -3147,7 +3202,7 @@
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="14" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B72" t="s">
         <v>322</v>
@@ -3155,10 +3210,10 @@
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="14" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B73" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -3171,32 +3226,32 @@
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B75">
         <v>60</v>
       </c>
     </row>
     <row r="76" spans="1:2">
-      <c r="A76" t="s">
-        <v>342</v>
-      </c>
-      <c r="B76" t="str">
+      <c r="A76" s="24" t="s">
+        <v>592</v>
+      </c>
+      <c r="B76">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>341</v>
+      </c>
+      <c r="B77" t="str">
         <f ca="1">TEXT(TODAY(), "mm/dd/yyyy")</f>
-        <v>01/12/2024</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="12" t="s">
-        <v>348</v>
-      </c>
-      <c r="B77" t="s">
-        <v>351</v>
+        <v>01/16/2024</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B78" t="s">
         <v>350</v>
@@ -3204,403 +3259,411 @@
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="12" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B79" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="12" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B80" t="s">
-        <v>74</v>
+        <v>352</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="B81" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="12" t="s">
+        <v>354</v>
+      </c>
+      <c r="B82" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="20" t="s">
         <v>355</v>
       </c>
-      <c r="B81" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="22" t="s">
+      <c r="B83" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B84" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="12" t="s">
+    <row r="85" spans="1:2">
+      <c r="A85" s="20" t="s">
         <v>357</v>
-      </c>
-      <c r="B83" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="22" t="s">
-        <v>358</v>
-      </c>
-      <c r="B84" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="23" t="s">
-        <v>576</v>
       </c>
       <c r="B85" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="86" spans="1:2">
-      <c r="A86" s="22" t="s">
+      <c r="A86" s="21" t="s">
         <v>570</v>
       </c>
       <c r="B86" t="s">
-        <v>577</v>
+        <v>360</v>
       </c>
     </row>
     <row r="87" spans="1:2">
-      <c r="A87" s="15" t="s">
-        <v>370</v>
+      <c r="A87" s="20" t="s">
+        <v>564</v>
       </c>
       <c r="B87" t="s">
-        <v>385</v>
+        <v>571</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="15" t="s">
+        <v>369</v>
+      </c>
+      <c r="B88" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="15" t="s">
+        <v>370</v>
+      </c>
+      <c r="B89" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="43.5">
+      <c r="A90" s="15" t="s">
         <v>371</v>
       </c>
-      <c r="B88" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="43.5">
-      <c r="A89" s="15" t="s">
-        <v>372</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" s="15" t="s">
-        <v>373</v>
-      </c>
-      <c r="B90" t="s">
-        <v>138</v>
+      <c r="B90" s="3" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="15" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B91" t="s">
-        <v>528</v>
+        <v>138</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="15" t="s">
+        <v>373</v>
+      </c>
+      <c r="B92" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="15" t="s">
+        <v>374</v>
+      </c>
+      <c r="B93" t="s">
         <v>375</v>
       </c>
-      <c r="B92" t="s">
+    </row>
+    <row r="94" spans="1:2" ht="29">
+      <c r="A94" s="15" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" ht="29">
-      <c r="A93" s="15" t="s">
-        <v>377</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" s="15" t="s">
-        <v>378</v>
-      </c>
-      <c r="B94" t="s">
-        <v>138</v>
+      <c r="B94" s="3" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="15" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B95" t="s">
-        <v>528</v>
+        <v>138</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="B96" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="15" t="s">
+        <v>379</v>
+      </c>
+      <c r="B97" t="s">
         <v>380</v>
       </c>
-      <c r="B96" t="s">
+    </row>
+    <row r="98" spans="1:2" ht="58">
+      <c r="A98" s="15" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" ht="58">
-      <c r="A97" s="15" t="s">
-        <v>382</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
-      <c r="A98" s="15" t="s">
-        <v>383</v>
-      </c>
-      <c r="B98" t="s">
-        <v>138</v>
+      <c r="B98" s="3" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="15" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B99" t="s">
-        <v>528</v>
+        <v>138</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="15" t="s">
+        <v>383</v>
+      </c>
+      <c r="B100" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="15" t="s">
+        <v>386</v>
+      </c>
+      <c r="B101" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="58">
+      <c r="A102" s="15" t="s">
         <v>387</v>
       </c>
-      <c r="B100" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="58">
-      <c r="A101" s="15" t="s">
-        <v>388</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2">
-      <c r="A102" s="15" t="s">
-        <v>389</v>
-      </c>
-      <c r="B102" t="s">
-        <v>138</v>
+      <c r="B102" s="3" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="15" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B103" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="104" spans="1:2">
-      <c r="A104" s="16" t="s">
-        <v>402</v>
+      <c r="A104" s="15" t="s">
+        <v>389</v>
       </c>
       <c r="B104" t="s">
-        <v>403</v>
+        <v>138</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" s="16" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B105" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" s="16" t="s">
+        <v>403</v>
+      </c>
+      <c r="B106" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="16" t="s">
+        <v>405</v>
+      </c>
+      <c r="B107" t="s">
         <v>406</v>
-      </c>
-      <c r="B106" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2">
-      <c r="A107" t="s">
-        <v>408</v>
-      </c>
-      <c r="B107" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B108" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B109" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>433</v>
+        <v>411</v>
       </c>
       <c r="B110" t="s">
-        <v>138</v>
+        <v>412</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B111" t="s">
-        <v>435</v>
+        <v>138</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>436</v>
-      </c>
-      <c r="B112" t="b">
-        <v>0</v>
+        <v>433</v>
+      </c>
+      <c r="B112" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>437</v>
+        <v>435</v>
+      </c>
+      <c r="B113" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>438</v>
-      </c>
-      <c r="B114">
-        <v>2</v>
+        <v>436</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
+        <v>437</v>
+      </c>
+      <c r="B115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="17" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="116" spans="1:3">
-      <c r="A116" s="17" t="s">
-        <v>440</v>
-      </c>
-      <c r="B116" t="b">
+      <c r="B117" t="b">
         <v>1</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3">
-      <c r="A117" t="s">
-        <v>455</v>
-      </c>
-      <c r="B117">
-        <v>10</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>461</v>
-      </c>
-      <c r="B118" t="s">
-        <v>462</v>
+        <v>454</v>
+      </c>
+      <c r="B118">
+        <v>10</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B119" t="s">
-        <v>464</v>
+        <v>584</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>465</v>
-      </c>
-      <c r="B120">
+        <v>461</v>
+      </c>
+      <c r="B120" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" t="s">
+        <v>462</v>
+      </c>
+      <c r="B121">
         <f ca="1">YEAR(TODAY())</f>
         <v>2024</v>
       </c>
     </row>
-    <row r="121" spans="1:3">
-      <c r="A121" t="s">
-        <v>466</v>
-      </c>
-      <c r="B121" t="s">
-        <v>516</v>
-      </c>
-      <c r="C121" t="str">
+    <row r="122" spans="1:3">
+      <c r="A122" t="s">
+        <v>463</v>
+      </c>
+      <c r="B122" t="s">
+        <v>513</v>
+      </c>
+      <c r="C122" t="str">
         <f ca="1">TEXT(MONTH(NOW()),"mmmm")</f>
         <v>January</v>
       </c>
     </row>
-    <row r="122" spans="1:3">
-      <c r="A122" t="s">
-        <v>503</v>
-      </c>
-      <c r="C122" t="str">
-        <f ca="1">TEXT(NOW(),"mm-dd hhmm")</f>
-        <v>01-12 1729</v>
-      </c>
-    </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>514</v>
-      </c>
-      <c r="B123" t="s">
-        <v>515</v>
+        <v>500</v>
+      </c>
+      <c r="C123" t="str">
+        <f ca="1">TEXT(NOW(),"mm-dd hhmm")</f>
+        <v>01-16 1935</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>521</v>
+        <v>511</v>
+      </c>
+      <c r="B124" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>530</v>
-      </c>
-      <c r="B125">
-        <v>90</v>
+        <v>518</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>543</v>
-      </c>
-      <c r="B126" t="s">
-        <v>544</v>
+        <v>527</v>
+      </c>
+      <c r="B126">
+        <v>90</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="B127" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>557</v>
+        <v>544</v>
       </c>
       <c r="B128" t="s">
-        <v>515</v>
+        <v>545</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" t="s">
+        <v>553</v>
+      </c>
+      <c r="B129" t="s">
+        <v>512</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="20"/>
+  <phoneticPr fontId="21"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3611,7 +3674,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -4764,7 +4827,7 @@
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="20"/>
+  <phoneticPr fontId="21"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4830,17 +4893,17 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="20"/>
+  <phoneticPr fontId="21"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D9DC59-3960-42CB-B3EC-EFF452A90D4F}">
-  <dimension ref="A1:Z158"/>
+  <dimension ref="A1:Z165"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4902,42 +4965,42 @@
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
+        <v>397</v>
+      </c>
+      <c r="B4" t="s">
         <v>398</v>
-      </c>
-      <c r="B4" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
+        <v>399</v>
+      </c>
+      <c r="B5" t="s">
         <v>400</v>
-      </c>
-      <c r="B5" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
+        <v>426</v>
+      </c>
+      <c r="B6" t="s">
         <v>427</v>
-      </c>
-      <c r="B6" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" t="s">
+        <v>428</v>
+      </c>
+      <c r="B7" t="s">
         <v>429</v>
-      </c>
-      <c r="B7" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
+        <v>430</v>
+      </c>
+      <c r="B8" t="s">
         <v>431</v>
-      </c>
-      <c r="B8" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -5094,23 +5157,23 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>238</v>
+        <v>581</v>
       </c>
       <c r="B28" t="s">
-        <v>237</v>
+        <v>582</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B29" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B30" t="s">
         <v>240</v>
@@ -5118,23 +5181,23 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B31" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B32" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B33" t="s">
         <v>244</v>
@@ -5142,255 +5205,255 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B34" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B35" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B36" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>225</v>
+        <v>249</v>
       </c>
       <c r="B37" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B38" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B39" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>258</v>
+        <v>227</v>
       </c>
       <c r="B40" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>448</v>
+        <v>258</v>
       </c>
       <c r="B41" t="s">
-        <v>449</v>
+        <v>257</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="B42" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B43" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B44" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B45" t="s">
-        <v>532</v>
+        <v>451</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B46" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>264</v>
+        <v>446</v>
       </c>
       <c r="B47" t="s">
-        <v>453</v>
+        <v>529</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B48" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="B49" t="s">
-        <v>266</v>
+        <v>452</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B50" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="B51" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B52" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B53" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B54" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B55" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="B56" t="s">
-        <v>454</v>
+        <v>274</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>457</v>
+        <v>287</v>
       </c>
       <c r="B57" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>568</v>
+        <v>456</v>
       </c>
       <c r="B58" t="s">
-        <v>569</v>
+        <v>458</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>458</v>
+        <v>562</v>
       </c>
       <c r="B59" t="s">
-        <v>460</v>
+        <v>563</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>269</v>
+        <v>457</v>
       </c>
       <c r="B60" t="s">
-        <v>272</v>
+        <v>459</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B61" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="B62" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B63" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B64" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B65" t="s">
         <v>288</v>
@@ -5398,39 +5461,39 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B66" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>546</v>
+        <v>292</v>
       </c>
       <c r="B67" t="s">
-        <v>545</v>
+        <v>291</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>294</v>
+        <v>543</v>
       </c>
       <c r="B68" t="s">
-        <v>297</v>
+        <v>542</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B69" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B70" t="s">
         <v>293</v>
@@ -5438,23 +5501,23 @@
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B71" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B72" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B73" t="s">
         <v>302</v>
@@ -5462,682 +5525,738 @@
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="B74" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B75" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B76" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>520</v>
+        <v>310</v>
       </c>
       <c r="B77" t="s">
-        <v>519</v>
+        <v>311</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>303</v>
+        <v>517</v>
       </c>
       <c r="B78" t="s">
-        <v>305</v>
+        <v>516</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B79" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="B80" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>319</v>
+        <v>572</v>
       </c>
       <c r="B81" t="s">
-        <v>318</v>
+        <v>588</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B82" t="s">
-        <v>572</v>
+        <v>318</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>574</v>
+        <v>320</v>
       </c>
       <c r="B83" t="s">
-        <v>575</v>
+        <v>566</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B84" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>533</v>
+        <v>565</v>
       </c>
       <c r="B85" t="s">
-        <v>450</v>
+        <v>567</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>534</v>
+        <v>329</v>
       </c>
       <c r="B86" t="s">
-        <v>451</v>
+        <v>328</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>535</v>
+        <v>331</v>
       </c>
       <c r="B87" t="s">
-        <v>452</v>
+        <v>330</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>536</v>
+        <v>560</v>
       </c>
       <c r="B88" t="s">
-        <v>532</v>
+        <v>330</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>537</v>
+        <v>573</v>
       </c>
       <c r="B89" t="s">
-        <v>532</v>
+        <v>589</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>538</v>
+        <v>574</v>
       </c>
       <c r="B90" t="s">
-        <v>541</v>
+        <v>590</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>539</v>
+        <v>575</v>
       </c>
       <c r="B91" t="s">
-        <v>542</v>
+        <v>591</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>540</v>
+        <v>334</v>
       </c>
       <c r="B92" t="s">
-        <v>542</v>
+        <v>337</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>326</v>
+        <v>343</v>
       </c>
       <c r="B93" t="s">
-        <v>327</v>
+        <v>342</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="B94" t="s">
-        <v>329</v>
+        <v>548</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>332</v>
+        <v>547</v>
       </c>
       <c r="B95" t="s">
-        <v>331</v>
+        <v>548</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>566</v>
+        <v>550</v>
       </c>
       <c r="B96" t="s">
-        <v>331</v>
+        <v>549</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>315</v>
+        <v>551</v>
       </c>
       <c r="B97" t="s">
-        <v>333</v>
+        <v>552</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>316</v>
+        <v>335</v>
       </c>
       <c r="B98" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>565</v>
+        <v>336</v>
       </c>
       <c r="B99" t="s">
-        <v>564</v>
+        <v>339</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>335</v>
+        <v>159</v>
       </c>
       <c r="B100" t="s">
-        <v>338</v>
+        <v>158</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>344</v>
+        <v>163</v>
       </c>
       <c r="B101" t="s">
-        <v>343</v>
+        <v>164</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>345</v>
+        <v>166</v>
       </c>
       <c r="B102" t="s">
-        <v>552</v>
+        <v>165</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>551</v>
+        <v>160</v>
       </c>
       <c r="B103" t="s">
-        <v>552</v>
+        <v>162</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>554</v>
+        <v>161</v>
       </c>
       <c r="B104" t="s">
-        <v>553</v>
+        <v>167</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>555</v>
+        <v>168</v>
       </c>
       <c r="B105" t="s">
-        <v>556</v>
+        <v>169</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>336</v>
+        <v>170</v>
       </c>
       <c r="B106" t="s">
-        <v>339</v>
+        <v>520</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>337</v>
+        <v>171</v>
       </c>
       <c r="B107" t="s">
-        <v>340</v>
+        <v>519</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="B108" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>163</v>
+        <v>440</v>
       </c>
       <c r="B109" t="s">
-        <v>164</v>
+        <v>441</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="B110" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>160</v>
+        <v>179</v>
       </c>
       <c r="B111" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
       <c r="B112" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="B113" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="B114" t="s">
-        <v>523</v>
+        <v>185</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="B115" t="s">
-        <v>522</v>
+        <v>186</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
       <c r="B116" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>441</v>
+        <v>174</v>
       </c>
       <c r="B117" t="s">
-        <v>442</v>
+        <v>346</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B118" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B119" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>180</v>
+        <v>391</v>
       </c>
       <c r="B120" t="s">
-        <v>181</v>
+        <v>392</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>182</v>
+        <v>521</v>
       </c>
       <c r="B121" t="s">
-        <v>183</v>
+        <v>523</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>184</v>
+        <v>522</v>
       </c>
       <c r="B122" t="s">
-        <v>185</v>
+        <v>524</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>187</v>
+        <v>393</v>
       </c>
       <c r="B123" t="s">
-        <v>186</v>
+        <v>394</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>188</v>
+        <v>395</v>
       </c>
       <c r="B124" t="s">
-        <v>186</v>
+        <v>396</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>174</v>
+        <v>464</v>
       </c>
       <c r="B125" t="s">
-        <v>347</v>
+        <v>471</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>175</v>
+        <v>467</v>
       </c>
       <c r="B126" t="s">
-        <v>190</v>
+        <v>475</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>176</v>
+        <v>468</v>
       </c>
       <c r="B127" t="s">
-        <v>189</v>
+        <v>474</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>392</v>
+        <v>469</v>
       </c>
       <c r="B128" t="s">
-        <v>393</v>
+        <v>478</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>524</v>
+        <v>470</v>
       </c>
       <c r="B129" t="s">
-        <v>526</v>
+        <v>477</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>525</v>
+        <v>476</v>
       </c>
       <c r="B130" t="s">
-        <v>527</v>
+        <v>477</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>394</v>
+        <v>465</v>
       </c>
       <c r="B131" t="s">
-        <v>395</v>
+        <v>472</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>396</v>
+        <v>466</v>
       </c>
       <c r="B132" t="s">
-        <v>397</v>
+        <v>473</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>467</v>
+        <v>479</v>
       </c>
       <c r="B133" t="s">
-        <v>474</v>
+        <v>480</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>470</v>
+        <v>485</v>
       </c>
       <c r="B134" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>471</v>
+        <v>486</v>
       </c>
       <c r="B135" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>472</v>
+        <v>487</v>
       </c>
       <c r="B136" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>473</v>
+        <v>483</v>
       </c>
       <c r="B137" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
       <c r="B138" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>468</v>
+        <v>488</v>
       </c>
       <c r="B139" t="s">
-        <v>475</v>
+        <v>491</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>469</v>
+        <v>494</v>
       </c>
       <c r="B140" t="s">
-        <v>476</v>
+        <v>496</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>482</v>
+        <v>495</v>
       </c>
       <c r="B141" t="s">
-        <v>483</v>
+        <v>498</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>488</v>
+        <v>497</v>
       </c>
       <c r="B142" t="s">
-        <v>478</v>
+        <v>499</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>489</v>
+        <v>501</v>
       </c>
       <c r="B143" t="s">
-        <v>477</v>
+        <v>503</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>490</v>
+        <v>502</v>
       </c>
       <c r="B144" t="s">
-        <v>480</v>
+        <v>504</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>486</v>
+        <v>505</v>
       </c>
       <c r="B145" t="s">
-        <v>484</v>
+        <v>507</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>487</v>
+        <v>506</v>
       </c>
       <c r="B146" t="s">
-        <v>485</v>
+        <v>508</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>491</v>
-      </c>
-      <c r="B147" t="s">
-        <v>494</v>
+        <v>509</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="148" spans="1:2">
-      <c r="A148" t="s">
-        <v>497</v>
-      </c>
-      <c r="B148" t="s">
-        <v>499</v>
+      <c r="A148" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
       <c r="B149" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>500</v>
+        <v>490</v>
       </c>
       <c r="B150" t="s">
-        <v>502</v>
+        <v>493</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>504</v>
+        <v>314</v>
       </c>
       <c r="B151" t="s">
-        <v>506</v>
+        <v>313</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>505</v>
+        <v>530</v>
       </c>
       <c r="B152" t="s">
-        <v>507</v>
+        <v>449</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>508</v>
+        <v>531</v>
       </c>
       <c r="B153" t="s">
-        <v>510</v>
+        <v>450</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>509</v>
+        <v>532</v>
       </c>
       <c r="B154" t="s">
-        <v>511</v>
+        <v>451</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>512</v>
-      </c>
-      <c r="B155" s="2" t="s">
-        <v>513</v>
+        <v>533</v>
+      </c>
+      <c r="B155" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="156" spans="1:2">
-      <c r="A156" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="B156" s="2" t="s">
-        <v>550</v>
+      <c r="A156" t="s">
+        <v>534</v>
+      </c>
+      <c r="B156" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>492</v>
+        <v>535</v>
       </c>
       <c r="B157" t="s">
-        <v>495</v>
+        <v>538</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>493</v>
+        <v>536</v>
       </c>
       <c r="B158" t="s">
-        <v>496</v>
+        <v>539</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159" t="s">
+        <v>537</v>
+      </c>
+      <c r="B159" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160" t="s">
+        <v>326</v>
+      </c>
+      <c r="B160" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" t="s">
+        <v>576</v>
+      </c>
+      <c r="B161" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
+      <c r="A162" t="s">
+        <v>577</v>
+      </c>
+      <c r="B162" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="A163" t="s">
+        <v>578</v>
+      </c>
+      <c r="B163" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="A164" t="s">
+        <v>315</v>
+      </c>
+      <c r="B164" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2">
+      <c r="A165" t="s">
+        <v>316</v>
+      </c>
+      <c r="B165" t="s">
+        <v>333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes to continue on error
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55651C\Documents\GitHub\P0002_090_PayCyleAfternoon_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605338B5-595E-4CE4-8F70-04AE3B499915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B585D6BA-3F1F-4CAC-A534-DBDB01874705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -2449,7 +2449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+    <sheetView topLeftCell="A69" workbookViewId="0">
       <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
@@ -3673,7 +3673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
changes to timeout and foldername
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55651C\Documents\GitHub\P0002_090_PayCyleAfternoon_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B585D6BA-3F1F-4CAC-A534-DBDB01874705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6B934D-B3B3-46F4-AB5D-00088824E641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="585">
   <si>
     <t>Name</t>
   </si>
@@ -301,15 +301,6 @@
     <t>Local Folder Path for Bot process folders</t>
   </si>
   <si>
-    <t>InputFolder</t>
-  </si>
-  <si>
-    <t>Input</t>
-  </si>
-  <si>
-    <t>Bot process Input folder name should be same locally and on the shared drive.</t>
-  </si>
-  <si>
     <t>OutputFolder</t>
   </si>
   <si>
@@ -319,24 +310,9 @@
     <t>Bot process Output folder name should be same locally and on the shared drive.</t>
   </si>
   <si>
-    <t>ExceptionFolder</t>
-  </si>
-  <si>
-    <t>Exception</t>
-  </si>
-  <si>
-    <t>Bot process Exception folder name should be same locally and on the shared drive.</t>
-  </si>
-  <si>
-    <t>SummaryFolder</t>
-  </si>
-  <si>
     <t>Summary</t>
   </si>
   <si>
-    <t>Bot process Summary folder name should be same locally and on the shared drive.</t>
-  </si>
-  <si>
     <t>Folder for placing exception screenshots.</t>
   </si>
   <si>
@@ -626,9 +602,6 @@
   </si>
   <si>
     <t>Asset</t>
-  </si>
-  <si>
-    <t>SharePointLink</t>
   </si>
   <si>
     <t>NavigateToPaycyclepageWorkflowStarted</t>
@@ -1818,6 +1791,9 @@
   </si>
   <si>
     <t>CompletedStatusRefreshButtonDelay</t>
+  </si>
+  <si>
+    <t>PSNT2</t>
   </si>
 </sst>
 </file>
@@ -2099,8 +2075,8 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="1"/>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="1"/>
@@ -2447,10 +2423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z129"/>
+  <dimension ref="A1:Z125"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -2497,10 +2473,10 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -2511,7 +2487,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>29</v>
@@ -2522,7 +2498,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>21</v>
@@ -2541,57 +2517,57 @@
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="B6" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="B7" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="B8" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="B9" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="B10" t="s">
-        <v>528</v>
+        <v>519</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -2599,7 +2575,7 @@
         <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C11" t="s">
         <v>45</v>
@@ -2610,7 +2586,7 @@
         <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C12" t="s">
         <v>47</v>
@@ -2621,7 +2597,7 @@
         <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C13" t="s">
         <v>49</v>
@@ -2632,7 +2608,7 @@
         <v>50</v>
       </c>
       <c r="B14" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C14" t="s">
         <v>51</v>
@@ -2643,7 +2619,7 @@
         <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C15" t="s">
         <v>53</v>
@@ -2654,7 +2630,7 @@
         <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C16" t="s">
         <v>55</v>
@@ -2665,7 +2641,7 @@
         <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C17" t="s">
         <v>57</v>
@@ -2676,7 +2652,7 @@
         <v>58</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>561</v>
+        <v>552</v>
       </c>
       <c r="C18" t="s">
         <v>59</v>
@@ -2698,7 +2674,7 @@
         <v>63</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>558</v>
+        <v>549</v>
       </c>
       <c r="C20" t="s">
         <v>64</v>
@@ -2720,7 +2696,7 @@
         <v>68</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>559</v>
+        <v>550</v>
       </c>
       <c r="C22" t="s">
         <v>69</v>
@@ -2786,7 +2762,7 @@
         <v>85</v>
       </c>
       <c r="B28" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="C28" t="s">
         <v>86</v>
@@ -2805,109 +2781,109 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>5</v>
       </c>
       <c r="B30" t="s">
+        <v>381</v>
+      </c>
+      <c r="C30" t="s">
         <v>91</v>
-      </c>
-      <c r="C30" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
+        <v>336</v>
+      </c>
+      <c r="B31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" t="s">
         <v>93</v>
-      </c>
-      <c r="B31" t="s">
-        <v>94</v>
-      </c>
-      <c r="C31" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B33" t="s">
         <v>96</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C33" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C32" t="s">
+      <c r="B34" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" t="s">
-        <v>390</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="C34" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>345</v>
-      </c>
-      <c r="B34" t="s">
+    <row r="35" spans="1:3">
+      <c r="A35" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C34" t="s">
+      <c r="B35" s="7" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
+      <c r="C35" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B35" t="s">
-        <v>97</v>
-      </c>
-      <c r="C35" t="s">
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="B36" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C36" t="s">
-        <v>140</v>
+      <c r="C36" s="5" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="7" t="s">
-        <v>105</v>
+      <c r="A37" s="5" t="s">
+        <v>106</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B38" s="7" t="s">
+      <c r="A38" s="5" t="s">
         <v>109</v>
       </c>
+      <c r="B38" s="5" t="s">
+        <v>110</v>
+      </c>
       <c r="C38" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>113</v>
@@ -2917,7 +2893,7 @@
       <c r="A40" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" t="s">
         <v>115</v>
       </c>
       <c r="C40" s="5" t="s">
@@ -2939,727 +2915,689 @@
       <c r="A42" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>97</v>
+      <c r="B42">
+        <v>5000</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43">
+        <v>5</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C43" s="5" t="s">
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="18" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="5" t="s">
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="B44" s="5" t="s">
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="23" t="s">
+        <v>446</v>
+      </c>
+      <c r="B45">
+        <v>10</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="B46" t="b">
+        <v>1</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="5" t="s">
+    <row r="47" spans="1:3">
+      <c r="A47" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B45">
-        <v>5000</v>
-      </c>
-      <c r="C45" s="5" t="s">
+      <c r="B47">
+        <v>20</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="B46">
+    <row r="48" spans="1:3">
+      <c r="A48" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B48">
         <v>5</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="B47">
-        <v>2</v>
-      </c>
-      <c r="C47" s="22" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="24" t="s">
-        <v>455</v>
-      </c>
-      <c r="B48">
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B50" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B51" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B52" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="B54">
         <v>10</v>
       </c>
-      <c r="C48" s="22" t="s">
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="B57" t="str">
+        <f ca="1">TEXT(TODAY(), "yyyy-mm-dd")</f>
+        <v>2024-01-17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="B58">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="B59">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="B60" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="B61" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="B62" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="B63" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="B64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="B65" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="B66" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="B67" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="B68" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="B69" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="B70" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="B71">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="23" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="B49" t="b">
-        <v>1</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B50">
-        <v>20</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="B51">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="B53" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B54" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B55" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="11" t="s">
-        <v>317</v>
-      </c>
-      <c r="B56" s="13" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="B57">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="B58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="9" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="B61" t="str">
-        <f ca="1">TEXT(TODAY(), "yyyy-mm-dd")</f>
-        <v>2024-01-16</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="B62">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="B63">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="B64" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="11" t="s">
-        <v>263</v>
-      </c>
-      <c r="B65" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="14" t="s">
-        <v>365</v>
-      </c>
-      <c r="B66" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="14" t="s">
-        <v>368</v>
-      </c>
-      <c r="B67" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="11" t="s">
-        <v>281</v>
-      </c>
-      <c r="B68" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="11" t="s">
-        <v>290</v>
-      </c>
-      <c r="B69" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="11" t="s">
-        <v>321</v>
-      </c>
-      <c r="B70" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71" s="11" t="s">
-        <v>323</v>
-      </c>
-      <c r="B71" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="14" t="s">
-        <v>366</v>
-      </c>
-      <c r="B72" t="s">
-        <v>322</v>
+      <c r="B72">
+        <v>30</v>
       </c>
     </row>
     <row r="73" spans="1:2">
-      <c r="A73" s="14" t="s">
-        <v>367</v>
-      </c>
-      <c r="B73" t="s">
-        <v>364</v>
+      <c r="A73" t="s">
+        <v>332</v>
+      </c>
+      <c r="B73" t="str">
+        <f ca="1">TEXT(TODAY(), "mm/dd/yyyy")</f>
+        <v>01/17/2024</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="11" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="B74" t="s">
-        <v>324</v>
+        <v>341</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="11" t="s">
-        <v>327</v>
-      </c>
-      <c r="B75">
-        <v>60</v>
+        <v>339</v>
+      </c>
+      <c r="B75" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="76" spans="1:2">
-      <c r="A76" s="24" t="s">
-        <v>592</v>
-      </c>
-      <c r="B76">
-        <v>30</v>
+      <c r="A76" s="11" t="s">
+        <v>342</v>
+      </c>
+      <c r="B76" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="77" spans="1:2">
-      <c r="A77" t="s">
-        <v>341</v>
-      </c>
-      <c r="B77" t="str">
-        <f ca="1">TEXT(TODAY(), "mm/dd/yyyy")</f>
-        <v>01/16/2024</v>
+      <c r="A77" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="B77" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="78" spans="1:2">
-      <c r="A78" s="12" t="s">
-        <v>347</v>
+      <c r="A78" s="11" t="s">
+        <v>345</v>
       </c>
       <c r="B78" t="s">
-        <v>350</v>
+        <v>115</v>
       </c>
     </row>
     <row r="79" spans="1:2">
-      <c r="A79" s="12" t="s">
-        <v>348</v>
+      <c r="A79" s="19" t="s">
+        <v>346</v>
       </c>
       <c r="B79" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="80" spans="1:2">
-      <c r="A80" s="12" t="s">
+      <c r="A80" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="B80" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="19" t="s">
+        <v>348</v>
+      </c>
+      <c r="B81" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="20" t="s">
+        <v>561</v>
+      </c>
+      <c r="B82" t="s">
         <v>351</v>
       </c>
-      <c r="B80" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="12" t="s">
-        <v>353</v>
-      </c>
-      <c r="B81" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="12" t="s">
-        <v>354</v>
-      </c>
-      <c r="B82" t="s">
-        <v>123</v>
-      </c>
     </row>
     <row r="83" spans="1:2">
-      <c r="A83" s="20" t="s">
-        <v>355</v>
+      <c r="A83" s="19" t="s">
+        <v>555</v>
       </c>
       <c r="B83" t="s">
-        <v>358</v>
+        <v>562</v>
       </c>
     </row>
     <row r="84" spans="1:2">
-      <c r="A84" s="12" t="s">
-        <v>356</v>
+      <c r="A84" s="14" t="s">
+        <v>360</v>
       </c>
       <c r="B84" t="s">
-        <v>359</v>
+        <v>375</v>
       </c>
     </row>
     <row r="85" spans="1:2">
-      <c r="A85" s="20" t="s">
-        <v>357</v>
+      <c r="A85" s="14" t="s">
+        <v>361</v>
       </c>
       <c r="B85" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" s="21" t="s">
-        <v>570</v>
-      </c>
-      <c r="B86" t="s">
-        <v>360</v>
+        <v>376</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="43.5">
+      <c r="A86" s="14" t="s">
+        <v>362</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="87" spans="1:2">
-      <c r="A87" s="20" t="s">
-        <v>564</v>
+      <c r="A87" s="14" t="s">
+        <v>363</v>
       </c>
       <c r="B87" t="s">
-        <v>571</v>
+        <v>130</v>
       </c>
     </row>
     <row r="88" spans="1:2">
-      <c r="A88" s="15" t="s">
+      <c r="A88" s="14" t="s">
+        <v>364</v>
+      </c>
+      <c r="B88" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="B89" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="29">
+      <c r="A90" s="14" t="s">
+        <v>367</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="B91" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="14" t="s">
         <v>369</v>
       </c>
-      <c r="B88" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" s="15" t="s">
+      <c r="B92" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="14" t="s">
         <v>370</v>
       </c>
-      <c r="B89" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="43.5">
-      <c r="A90" s="15" t="s">
+      <c r="B93" t="s">
         <v>371</v>
       </c>
-      <c r="B90" s="3" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" s="15" t="s">
+    </row>
+    <row r="94" spans="1:2" ht="58">
+      <c r="A94" s="14" t="s">
         <v>372</v>
       </c>
-      <c r="B91" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" s="15" t="s">
+      <c r="B94" s="3" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="14" t="s">
         <v>373</v>
       </c>
-      <c r="B92" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="15" t="s">
+      <c r="B95" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="14" t="s">
         <v>374</v>
       </c>
-      <c r="B93" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="29">
-      <c r="A94" s="15" t="s">
-        <v>376</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95" s="15" t="s">
+      <c r="B96" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="B95" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
-      <c r="A96" s="15" t="s">
+      <c r="B97" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="58">
+      <c r="A98" s="14" t="s">
         <v>378</v>
       </c>
-      <c r="B96" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
-      <c r="A97" s="15" t="s">
+      <c r="B98" s="3" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="14" t="s">
         <v>379</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B99" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="14" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" ht="58">
-      <c r="A98" s="15" t="s">
-        <v>381</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2">
-      <c r="A99" s="15" t="s">
-        <v>382</v>
-      </c>
-      <c r="B99" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
-      <c r="A100" s="15" t="s">
-        <v>383</v>
-      </c>
       <c r="B100" t="s">
-        <v>525</v>
+        <v>130</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="15" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="B101" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="58">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
       <c r="A102" s="15" t="s">
-        <v>387</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>557</v>
+        <v>394</v>
+      </c>
+      <c r="B102" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="15" t="s">
-        <v>388</v>
+        <v>396</v>
       </c>
       <c r="B103" t="s">
-        <v>138</v>
+        <v>397</v>
       </c>
     </row>
     <row r="104" spans="1:2">
-      <c r="A104" s="15" t="s">
-        <v>389</v>
+      <c r="A104" t="s">
+        <v>398</v>
       </c>
       <c r="B104" t="s">
-        <v>138</v>
+        <v>399</v>
       </c>
     </row>
     <row r="105" spans="1:2">
-      <c r="A105" s="16" t="s">
+      <c r="A105" t="s">
+        <v>400</v>
+      </c>
+      <c r="B105" t="s">
         <v>401</v>
       </c>
-      <c r="B105" t="s">
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="106" spans="1:2">
-      <c r="A106" s="16" t="s">
+      <c r="B106" t="s">
         <v>403</v>
       </c>
-      <c r="B106" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="107" spans="1:2">
-      <c r="A107" s="16" t="s">
-        <v>405</v>
+      <c r="A107" t="s">
+        <v>423</v>
       </c>
       <c r="B107" t="s">
-        <v>406</v>
+        <v>130</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>407</v>
+        <v>424</v>
       </c>
       <c r="B108" t="s">
-        <v>408</v>
+        <v>425</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>409</v>
-      </c>
-      <c r="B109" t="s">
-        <v>410</v>
+        <v>426</v>
+      </c>
+      <c r="B109" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>411</v>
-      </c>
-      <c r="B110" t="s">
-        <v>412</v>
+        <v>427</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>432</v>
-      </c>
-      <c r="B111" t="s">
-        <v>138</v>
+        <v>428</v>
+      </c>
+      <c r="B111">
+        <v>2</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>433</v>
-      </c>
-      <c r="B112" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
     </row>
     <row r="113" spans="1:3">
-      <c r="A113" t="s">
-        <v>435</v>
+      <c r="A113" s="16" t="s">
+        <v>430</v>
       </c>
       <c r="B113" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>436</v>
+        <v>445</v>
+      </c>
+      <c r="B114">
+        <v>10</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>437</v>
-      </c>
-      <c r="B115">
-        <v>2</v>
+        <v>451</v>
+      </c>
+      <c r="B115" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>438</v>
+        <v>452</v>
+      </c>
+      <c r="B116" t="s">
+        <v>576</v>
       </c>
     </row>
     <row r="117" spans="1:3">
-      <c r="A117" s="17" t="s">
-        <v>439</v>
-      </c>
-      <c r="B117" t="b">
-        <v>1</v>
+      <c r="A117" t="s">
+        <v>453</v>
+      </c>
+      <c r="B117">
+        <f ca="1">YEAR(TODAY())</f>
+        <v>2024</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
         <v>454</v>
       </c>
-      <c r="B118">
-        <v>10</v>
+      <c r="B118" t="s">
+        <v>504</v>
+      </c>
+      <c r="C118" t="str">
+        <f ca="1">TEXT(MONTH(NOW()),"mmmm")</f>
+        <v>January</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>460</v>
-      </c>
-      <c r="B119" t="s">
-        <v>584</v>
+        <v>491</v>
+      </c>
+      <c r="C119" t="str">
+        <f ca="1">TEXT(NOW(),"mm-dd hhmm")</f>
+        <v>01-17 1953</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>461</v>
+        <v>502</v>
       </c>
       <c r="B120" t="s">
-        <v>585</v>
+        <v>503</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>462</v>
-      </c>
-      <c r="B121">
-        <f ca="1">YEAR(TODAY())</f>
-        <v>2024</v>
+        <v>509</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>463</v>
-      </c>
-      <c r="B122" t="s">
-        <v>513</v>
-      </c>
-      <c r="C122" t="str">
-        <f ca="1">TEXT(MONTH(NOW()),"mmmm")</f>
-        <v>January</v>
+        <v>518</v>
+      </c>
+      <c r="B122">
+        <v>90</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>500</v>
-      </c>
-      <c r="C123" t="str">
-        <f ca="1">TEXT(NOW(),"mm-dd hhmm")</f>
-        <v>01-16 1935</v>
+        <v>531</v>
+      </c>
+      <c r="B123" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>511</v>
+        <v>535</v>
       </c>
       <c r="B124" t="s">
-        <v>512</v>
+        <v>536</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3">
-      <c r="A126" t="s">
-        <v>527</v>
-      </c>
-      <c r="B126">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3">
-      <c r="A127" t="s">
-        <v>540</v>
-      </c>
-      <c r="B127" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3">
-      <c r="A128" t="s">
         <v>544</v>
       </c>
-      <c r="B128" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2">
-      <c r="A129" t="s">
-        <v>553</v>
-      </c>
-      <c r="B129" t="s">
-        <v>512</v>
+      <c r="B125" t="s">
+        <v>503</v>
       </c>
     </row>
   </sheetData>
@@ -3673,7 +3611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -4853,7 +4791,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>27</v>
@@ -4886,10 +4824,10 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="B2" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -4949,1314 +4887,1314 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B3" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="B4" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="B5" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
       <c r="B6" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
       <c r="B7" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="B8" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B9" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B10" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B11" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B12" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="B13" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B14" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="B15" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:26">
       <c r="A16" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="B16" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="B17" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B18" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="B19" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="B20" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B21" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="B22" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="B23" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B24" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="B25" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B26" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="B27" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>581</v>
+        <v>572</v>
       </c>
       <c r="B28" t="s">
-        <v>582</v>
+        <v>573</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="B29" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="B30" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="B31" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="B32" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="B33" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="B34" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="B35" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B36" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="B37" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="B38" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="B39" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="B40" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B41" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
       <c r="B42" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="B43" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="B44" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="B45" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="B46" t="s">
-        <v>529</v>
+        <v>520</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
       <c r="B47" t="s">
-        <v>529</v>
+        <v>520</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="B48" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="B49" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B50" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B51" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="B52" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B53" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B54" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="B55" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="B56" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="B57" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="B58" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>562</v>
+        <v>553</v>
       </c>
       <c r="B59" t="s">
-        <v>563</v>
+        <v>554</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="B60" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="B61" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="B62" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="B63" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="B64" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="B65" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="B66" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="B67" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>543</v>
+        <v>534</v>
       </c>
       <c r="B68" t="s">
-        <v>542</v>
+        <v>533</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B69" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="B70" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="B71" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="B72" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="B73" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="B74" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="B75" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="B76" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="B77" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>517</v>
+        <v>508</v>
       </c>
       <c r="B78" t="s">
-        <v>516</v>
+        <v>507</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B79" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="B80" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>572</v>
+        <v>563</v>
       </c>
       <c r="B81" t="s">
-        <v>588</v>
+        <v>579</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="B82" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="B83" t="s">
-        <v>566</v>
+        <v>557</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>568</v>
+        <v>559</v>
       </c>
       <c r="B84" t="s">
-        <v>569</v>
+        <v>560</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>565</v>
+        <v>556</v>
       </c>
       <c r="B85" t="s">
-        <v>567</v>
+        <v>558</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="B86" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="B87" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>560</v>
+        <v>551</v>
       </c>
       <c r="B88" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>573</v>
+        <v>564</v>
       </c>
       <c r="B89" t="s">
-        <v>589</v>
+        <v>580</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>574</v>
+        <v>565</v>
       </c>
       <c r="B90" t="s">
-        <v>590</v>
+        <v>581</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>575</v>
+        <v>566</v>
       </c>
       <c r="B91" t="s">
-        <v>591</v>
+        <v>582</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="B92" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="B93" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="B94" t="s">
-        <v>548</v>
+        <v>539</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>547</v>
+        <v>538</v>
       </c>
       <c r="B95" t="s">
-        <v>548</v>
+        <v>539</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>550</v>
+        <v>541</v>
       </c>
       <c r="B96" t="s">
-        <v>549</v>
+        <v>540</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>551</v>
+        <v>542</v>
       </c>
       <c r="B97" t="s">
-        <v>552</v>
+        <v>543</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="B98" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="B99" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B100" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B101" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B102" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B103" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B104" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B105" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B106" t="s">
-        <v>520</v>
+        <v>511</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="B107" t="s">
-        <v>519</v>
+        <v>510</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B108" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="B109" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="B110" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B111" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="B112" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B113" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B114" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B115" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="B116" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B117" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="B118" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B119" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="B120" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>521</v>
+        <v>512</v>
       </c>
       <c r="B121" t="s">
-        <v>523</v>
+        <v>514</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>522</v>
+        <v>513</v>
       </c>
       <c r="B122" t="s">
-        <v>524</v>
+        <v>515</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="B123" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="B124" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
       <c r="B125" t="s">
-        <v>471</v>
+        <v>462</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="B126" t="s">
-        <v>475</v>
+        <v>466</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
       <c r="B127" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
+        <v>460</v>
+      </c>
+      <c r="B128" t="s">
         <v>469</v>
-      </c>
-      <c r="B128" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
       <c r="B129" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>476</v>
+        <v>467</v>
       </c>
       <c r="B130" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="B131" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
       <c r="B132" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
       <c r="B133" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
       <c r="B134" t="s">
-        <v>475</v>
+        <v>466</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
       <c r="B135" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
       <c r="B136" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="B137" t="s">
-        <v>481</v>
+        <v>472</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
       <c r="B138" t="s">
-        <v>482</v>
+        <v>473</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
       <c r="B139" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>494</v>
+        <v>485</v>
       </c>
       <c r="B140" t="s">
-        <v>496</v>
+        <v>487</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>495</v>
+        <v>486</v>
       </c>
       <c r="B141" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>497</v>
+        <v>488</v>
       </c>
       <c r="B142" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
       <c r="B143" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>502</v>
+        <v>493</v>
       </c>
       <c r="B144" t="s">
-        <v>504</v>
+        <v>495</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>505</v>
+        <v>496</v>
       </c>
       <c r="B145" t="s">
-        <v>507</v>
+        <v>498</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="B146" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>510</v>
+        <v>501</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="2" t="s">
-        <v>514</v>
+        <v>505</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>546</v>
+        <v>537</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
       <c r="B149" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>490</v>
+        <v>481</v>
       </c>
       <c r="B150" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="B151" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>530</v>
+        <v>521</v>
       </c>
       <c r="B152" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>531</v>
+        <v>522</v>
       </c>
       <c r="B153" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>532</v>
+        <v>523</v>
       </c>
       <c r="B154" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>533</v>
+        <v>524</v>
       </c>
       <c r="B155" t="s">
-        <v>529</v>
+        <v>520</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>534</v>
+        <v>525</v>
       </c>
       <c r="B156" t="s">
-        <v>529</v>
+        <v>520</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>535</v>
+        <v>526</v>
       </c>
       <c r="B157" t="s">
-        <v>538</v>
+        <v>529</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>536</v>
+        <v>527</v>
       </c>
       <c r="B158" t="s">
-        <v>539</v>
+        <v>530</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>537</v>
+        <v>528</v>
       </c>
       <c r="B159" t="s">
-        <v>539</v>
+        <v>530</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="B160" t="s">
-        <v>587</v>
+        <v>578</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>576</v>
+        <v>567</v>
       </c>
       <c r="B161" t="s">
-        <v>579</v>
+        <v>570</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>577</v>
+        <v>568</v>
       </c>
       <c r="B162" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>578</v>
+        <v>569</v>
       </c>
       <c r="B163" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="B164" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="B165" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to Asset and Config files
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55651C\Documents\GitHub\P0002_090_PayCyleAfternoon_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6B934D-B3B3-46F4-AB5D-00088824E641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D868411B-71AE-4F78-8DCC-B13DB39B5D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="546">
   <si>
     <t>Name</t>
   </si>
@@ -99,11 +99,11 @@
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="21"/>
+    <phoneticPr fontId="20"/>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="21"/>
+    <phoneticPr fontId="20"/>
   </si>
   <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
@@ -163,12 +163,6 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>https://soklfpub-tst.opc.oracleoutsourcing.com/psp/SOKLFTSTNSS/?cmd=login&amp;languageCd=ENG&amp;</t>
-  </si>
-  <si>
-    <t>PeopleSoft URL for lauching the web application.</t>
-  </si>
-  <si>
     <t>PeopleSoft_LoginURL</t>
   </si>
   <si>
@@ -181,39 +175,15 @@
     <t>RecipientEmailAddress</t>
   </si>
   <si>
-    <t>Email ID for recipients for Success Email</t>
-  </si>
-  <si>
     <t>CcRecipientEmailAddress</t>
   </si>
   <si>
-    <t>Email ID for CC recipients for Success Email</t>
-  </si>
-  <si>
-    <t>RecipientEmailAddressBE</t>
-  </si>
-  <si>
-    <t>Email ID for recipients for Business Exception Email</t>
-  </si>
-  <si>
-    <t>CcRecipientEmailAddressBE</t>
-  </si>
-  <si>
-    <t>Email ID for CC recipients for Business Exception Email</t>
-  </si>
-  <si>
     <t>RecipientEmailAddressSE</t>
   </si>
   <si>
-    <t>Email ID for recipients for System Exception Email</t>
-  </si>
-  <si>
     <t>CcRecipientEmailAddressSE</t>
   </si>
   <si>
-    <t>Email ID for CC recipients for System Exception Email</t>
-  </si>
-  <si>
     <t>EmailBody</t>
   </si>
   <si>
@@ -229,21 +199,6 @@
     <t>Success Email Subject</t>
   </si>
   <si>
-    <t>EmailBodyBE</t>
-  </si>
-  <si>
-    <t>Business Exception Email Body</t>
-  </si>
-  <si>
-    <t>EmailSubjectBE</t>
-  </si>
-  <si>
-    <t>Process Business Exception</t>
-  </si>
-  <si>
-    <t>Business Exception Email Subject</t>
-  </si>
-  <si>
     <t>EmailBodySE</t>
   </si>
   <si>
@@ -277,45 +232,12 @@
     <t>mail type is failure</t>
   </si>
   <si>
-    <t>ErrorTypeBE</t>
-  </si>
-  <si>
-    <t>Business</t>
-  </si>
-  <si>
-    <t>Error type is business exception</t>
-  </si>
-  <si>
-    <t>ErrorTypeSE</t>
-  </si>
-  <si>
-    <t>System</t>
-  </si>
-  <si>
-    <t>Error type is system exception</t>
-  </si>
-  <si>
-    <t>LocalFolderPath</t>
-  </si>
-  <si>
     <t>Local Folder Path for Bot process folders</t>
   </si>
   <si>
-    <t>OutputFolder</t>
-  </si>
-  <si>
-    <t>Output</t>
-  </si>
-  <si>
-    <t>Bot process Output folder name should be same locally and on the shared drive.</t>
-  </si>
-  <si>
     <t>Summary</t>
   </si>
   <si>
-    <t>Folder for placing exception screenshots.</t>
-  </si>
-  <si>
     <t>Summary_Report.xlsx</t>
   </si>
   <si>
@@ -358,48 +280,9 @@
     <t>Outlook exe name to kill instance</t>
   </si>
   <si>
-    <t>UpdateReportBusinessExceptionType</t>
-  </si>
-  <si>
-    <t>Business Exception</t>
-  </si>
-  <si>
-    <t>Exception type to be updated in exception report , if business.</t>
-  </si>
-  <si>
-    <t>UpdateReportSystemExceptionType</t>
-  </si>
-  <si>
-    <t>System Exception</t>
-  </si>
-  <si>
-    <t>Exception type to be updated in exception report , if system.</t>
-  </si>
-  <si>
-    <t>UpdateReportTypeSummary</t>
-  </si>
-  <si>
-    <t>If summary report needs to be updated.</t>
-  </si>
-  <si>
-    <t>UpdateReportExceptionStatus</t>
-  </si>
-  <si>
     <t>Failed</t>
   </si>
   <si>
-    <t>If a transaction is failed.</t>
-  </si>
-  <si>
-    <t>UpdateReportSuccessStatus</t>
-  </si>
-  <si>
-    <t>Completed</t>
-  </si>
-  <si>
-    <t>If a transaction completes successfully.</t>
-  </si>
-  <si>
     <t>CloseApplicationTimeout</t>
   </si>
   <si>
@@ -430,9 +313,6 @@
     <t>Number of queue items to be checked before adding, please add is input items are more than 20.</t>
   </si>
   <si>
-    <t>Udbhav.Agarwal.CTR@omes.ok.gov</t>
-  </si>
-  <si>
     <t>PeoplsoftLoginSuccessResult</t>
   </si>
   <si>
@@ -592,12 +472,6 @@
     <t>ReturnButtonCounterSelector</t>
   </si>
   <si>
-    <t>P002_090_PayCycleAfternoon_PayCycleValues</t>
-  </si>
-  <si>
-    <t>PayCycleDataAddedToQueue</t>
-  </si>
-  <si>
     <t>P002_090_PayCycleAfternoon_Queue</t>
   </si>
   <si>
@@ -697,18 +571,12 @@
     <t>CheckPaycycleandValidateDateWorkflowBE</t>
   </si>
   <si>
-    <t>UAGARWAL</t>
-  </si>
-  <si>
     <t>RunningPaycycleRetries</t>
   </si>
   <si>
     <t>CalenderNameOrchestrator</t>
   </si>
   <si>
-    <t>DateForCalender</t>
-  </si>
-  <si>
     <t>Invalid Calendar Name Found.</t>
   </si>
   <si>
@@ -1033,12 +901,6 @@
     <t>Workflow to Update Summary Report has a system exception.</t>
   </si>
   <si>
-    <t>C:\PaycycleAfternoon</t>
-  </si>
-  <si>
-    <t>QueueReference</t>
-  </si>
-  <si>
     <t>Summary file was found, bot will now update it.</t>
   </si>
   <si>
@@ -1060,12 +922,6 @@
     <t>InstanceNumberStatusProcessing</t>
   </si>
   <si>
-    <t>Processing</t>
-  </si>
-  <si>
-    <t>Queued</t>
-  </si>
-  <si>
     <t>InstanceNumberProcessName</t>
   </si>
   <si>
@@ -1123,18 +979,6 @@
     <t>MailsWithCustomMessages</t>
   </si>
   <si>
-    <t>BE_1Subject</t>
-  </si>
-  <si>
-    <t>BE_1Body</t>
-  </si>
-  <si>
-    <t>BE_1RecipientEmailAddress</t>
-  </si>
-  <si>
-    <t>BE_1CCEmailAddress</t>
-  </si>
-  <si>
     <t>SE_1Subject</t>
   </si>
   <si>
@@ -1165,9 +1009,6 @@
     <t>SE_2CCEmailAddress</t>
   </si>
   <si>
-    <t>BE_1,SE_1,SE_2,SE_3</t>
-  </si>
-  <si>
     <t>Status not changing to completed</t>
   </si>
   <si>
@@ -1183,9 +1024,6 @@
     <t>SE_3CCEmailAddress</t>
   </si>
   <si>
-    <t>C:\Users\55651C\Documents\UiPath\P002_090_PayCycleAfternoon_Performer\Exceptions_Screenshots</t>
-  </si>
-  <si>
     <t>GetMailDetailsWorkflowStarted</t>
   </si>
   <si>
@@ -1204,18 +1042,6 @@
     <t>Workflow to Get Mail Details has a System Exception.</t>
   </si>
   <si>
-    <t>PeoplesoftLoginCredentialsSE_2</t>
-  </si>
-  <si>
-    <t>SE_2: Credentials Error.</t>
-  </si>
-  <si>
-    <t>PeoplesoftLoginPageUnavailableSE_1</t>
-  </si>
-  <si>
-    <t>SE_1: Peoplesoft Unavailable.</t>
-  </si>
-  <si>
     <t>PeopleSoftLoginErrorKeyword1</t>
   </si>
   <si>
@@ -1252,45 +1078,6 @@
     <t>Shared_O365ApplicationID</t>
   </si>
   <si>
-    <t>PeopleSoft_HomepageURL</t>
-  </si>
-  <si>
-    <t>https://soklfpub-tst.opc.oracleoutsourcing.com/psc/SOKLFTSTNSS/EMPLOYEE/ERP/c/NUI_FRAMEWORK.PT_LANDINGPAGE.GBL</t>
-  </si>
-  <si>
-    <t>URL for homepage after login.</t>
-  </si>
-  <si>
-    <t>PeopleSoft_ProcessMonitorURL</t>
-  </si>
-  <si>
-    <t>https://soklfpub-tst.opc.oracleoutsourcing.com/psp/SOKLFTSTNSS/EMPLOYEE/ERP/c/PROCESSMONITOR.PROCESSMONITOR.GBL</t>
-  </si>
-  <si>
-    <t>URL for Process Monitor Page.</t>
-  </si>
-  <si>
-    <t>PeopleSoft_PaymentSelectionCriteriaURL</t>
-  </si>
-  <si>
-    <t>https://soklfpub-tst.opc.oracleoutsourcing.com/psp/SOKLFTSTNSS_6/EMPLOYEE/ERP/c/CREATE_PAYMENTS.PYCYCL_DEFN.GBL</t>
-  </si>
-  <si>
-    <t>URL for Payment Selection Criteria page.</t>
-  </si>
-  <si>
-    <t>URL for Paycycle Manager page.</t>
-  </si>
-  <si>
-    <t>URL for Paycycle Approval page.</t>
-  </si>
-  <si>
-    <t>PeopleSoft_PaycycleApprovalURL</t>
-  </si>
-  <si>
-    <t>PeopleSoft_PaycycleManagerURL</t>
-  </si>
-  <si>
     <t>PeoplesoftLoginPageNotFoundSE</t>
   </si>
   <si>
@@ -1318,9 +1105,6 @@
     <t>DEV</t>
   </si>
   <si>
-    <t>MarkEmailAsRead</t>
-  </si>
-  <si>
     <t>BotPeoplesoftUserID</t>
   </si>
   <si>
@@ -1501,18 +1285,9 @@
     <t>LocalFolderNotPresent</t>
   </si>
   <si>
-    <t>Local Output Folder Present.</t>
-  </si>
-  <si>
     <t>LocalFolderNotPresentSE</t>
   </si>
   <si>
-    <t xml:space="preserve">Local Output Folder Not Present. Path: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Local Output Folder Not Found. Path: </t>
-  </si>
-  <si>
     <t>FolderNameDay</t>
   </si>
   <si>
@@ -1552,21 +1327,9 @@
     <t>A1</t>
   </si>
   <si>
-    <t>January</t>
-  </si>
-  <si>
     <t>SummaryFileNotPresent</t>
   </si>
   <si>
-    <t>PaycycleAfternoonTest</t>
-  </si>
-  <si>
-    <t>SE_3: Paycycle was not approved as the correct status not found even after retries.</t>
-  </si>
-  <si>
-    <t>PaycycleStatusNotChangedSE_3</t>
-  </si>
-  <si>
     <t>InstanceNumber</t>
   </si>
   <si>
@@ -1588,18 +1351,12 @@
     <t>Mail does not have a custom exception.</t>
   </si>
   <si>
-    <t>deepali.chaudhry@ey.com</t>
-  </si>
-  <si>
     <t>Pay Cycle &lt;PayCycle_Name&gt; running more than 20 mins</t>
   </si>
   <si>
     <t>TargetAppearWaitLong</t>
   </si>
   <si>
-    <t>https://soklfpub-tst.opc.oracleoutsourcing.com/psp/SOKLFTSTNSS_6/EMPLOYEE/ERP/c/CREATE_PAYMENTS.PYCYCL_MGR.GBL</t>
-  </si>
-  <si>
     <t>No value in Server Dropdown was found.</t>
   </si>
   <si>
@@ -1687,13 +1444,7 @@
     <t xml:space="preserve">Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;The &lt;PayCycle_Name&gt; Pay Cycle has run for over 20 minutes, hindering subsequent processes for the bot. Please manually complete the &lt;PayCycle_Name&gt; Pay Cycle today. Once done, send an email notification to support team to prompt the remaining pay cycle bot processes.&lt;br&gt;&lt;br&gt;Thanks,&lt;br&gt;Automation Team               </t>
   </si>
   <si>
-    <t>Hello RPA Support Team,&lt;br&gt;&lt;br&gt;This email notification was raised for process P002_090_PayCycleAfternoon. The process execution met a business exception for Pay cycle &lt;PC&gt;  , details for which can be found below:&lt;br&gt;&lt;br&gt;Exception Message: Excp_Message&lt;br&gt;&lt;br&gt; Thanks,&lt;br&gt;Automation Team</t>
-  </si>
-  <si>
     <t>Hello RPA Support Team,&lt;br&gt;&lt;br&gt;This email notification was raised for process P002_090_PayCycleAfternoon. The process execution met a System exception, details for which can be found below:&lt;br&gt;&lt;br&gt;Exception Message: Excp_Message&lt;br&gt;&lt;br&gt; Thanks,&lt;br&gt;Automation Team</t>
-  </si>
-  <si>
-    <t>StatusCompletedNotAppearedBE_1</t>
   </si>
   <si>
     <t>Hello Team,&lt;br&gt;&lt;br&gt;This email notification was raised for P002_090_PayCycleAfternoon process
@@ -1766,15 +1517,6 @@
     <t>Long delay for where ever needed</t>
   </si>
   <si>
-    <t>https://officemgmtentserv.sharepoint.com/sites/ACOE_Automations_DEV</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon</t>
-  </si>
-  <si>
-    <t>00:00:50</t>
-  </si>
-  <si>
     <t>All Paycycle Result list items are processed now.</t>
   </si>
   <si>
@@ -1794,6 +1536,147 @@
   </si>
   <si>
     <t>PSNT2</t>
+  </si>
+  <si>
+    <t>PeopleSoftLoginCredentailsFolderName</t>
+  </si>
+  <si>
+    <t>DEV/P002_PayCycleAfternoon</t>
+  </si>
+  <si>
+    <t>ProcessFolderName</t>
+  </si>
+  <si>
+    <t>PaycycleAfternoon_Performer</t>
+  </si>
+  <si>
+    <t>00:02:00</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_PeopleSoftLoginURL</t>
+  </si>
+  <si>
+    <t>PeopleSoft_NavigationURL</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_PeopleSoftNavigationURL</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_CcRecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_RecipientEmailAddressSE</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_CcRecipientEmailAddressSE</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SenderEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_2RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_2CCEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_3RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_3CCEmailAddress</t>
+  </si>
+  <si>
+    <t>LocalRootFolderPath</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_LocalRootFolderPath</t>
+  </si>
+  <si>
+    <t>PeoplesoftLoginCredentialsSE_3</t>
+  </si>
+  <si>
+    <t>PeoplesoftLoginPageUnavailableSE_2</t>
+  </si>
+  <si>
+    <t>SE_3: Credentials Error.</t>
+  </si>
+  <si>
+    <t>SE_2: Peoplesoft Unavailable.</t>
+  </si>
+  <si>
+    <t>PaycycleStatusNotChangedSE_1</t>
+  </si>
+  <si>
+    <t>SE_1: Paycycle was not approved as the correct status not found even after retries.</t>
+  </si>
+  <si>
+    <t>StatusCompletedNotAppearedBE_4</t>
+  </si>
+  <si>
+    <t>BE_4: Status is not completed , so the record will be marked as an exception.</t>
+  </si>
+  <si>
+    <t>BE_4Subject</t>
+  </si>
+  <si>
+    <t>BE_4Body</t>
+  </si>
+  <si>
+    <t>BE_4RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>BE_4CCEmailAddress</t>
+  </si>
+  <si>
+    <t>BE_4,SE_1,SE_2,SE_3</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_BE_4RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_BE_4CCEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_1RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_1CCEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SharepointURL</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SharepointSubFolder</t>
+  </si>
+  <si>
+    <t>QUEUED</t>
+  </si>
+  <si>
+    <t>PROCESSING</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_RefreshMonitorBotUserID</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_CalenderNameOrchestrator</t>
+  </si>
+  <si>
+    <t>Local Root Folder Present.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Local Root Folder Not Present. Path: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Local Root Folder Not Found. Path: </t>
+  </si>
+  <si>
+    <t>LocalRootFolderPresent</t>
+  </si>
+  <si>
+    <t>Local Process Folder Present.</t>
   </si>
 </sst>
 </file>
@@ -1803,18 +1686,11 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1992,7 +1868,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2002,6 +1878,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -2031,52 +1913,51 @@
   </borders>
   <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="4" fontId="26" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="4" fontId="25" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="20"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="20"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="1"/>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="1"/>
@@ -2088,6 +1969,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="22">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{DA952E48-534A-4104-8A72-2BE892964A18}"/>
@@ -2423,10 +2306,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z125"/>
+  <dimension ref="A1:Z87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -2473,21 +2356,21 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
-        <v>149</v>
+        <v>109</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>186</v>
+        <v>144</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.5">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="24" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>29</v>
@@ -2498,7 +2381,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>21</v>
@@ -2506,1102 +2389,724 @@
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" t="s">
         <v>43</v>
       </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" t="s">
-        <v>404</v>
+      <c r="A6" s="25" t="s">
+        <v>499</v>
       </c>
       <c r="B6" t="s">
-        <v>405</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="72.5">
       <c r="A7" t="s">
-        <v>407</v>
-      </c>
-      <c r="B7" t="s">
-        <v>408</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>409</v>
+        <v>48</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
-        <v>410</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>411</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="58">
       <c r="A9" t="s">
-        <v>416</v>
-      </c>
-      <c r="B9" t="s">
-        <v>411</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>413</v>
+        <v>53</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="C9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>415</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>519</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>414</v>
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>133</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>130</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>501</v>
       </c>
       <c r="B13" t="s">
-        <v>130</v>
+        <v>502</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>290</v>
       </c>
       <c r="B14" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B15" t="s">
-        <v>130</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:26">
-      <c r="A16" t="s">
-        <v>54</v>
+      <c r="A16" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="B16" t="s">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" t="s">
-        <v>130</v>
-      </c>
-      <c r="C17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="72.5">
-      <c r="A18" t="s">
-        <v>58</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>552</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="A17" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20">
+        <v>5000</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="22" t="s">
+        <v>374</v>
+      </c>
+      <c r="B23">
+        <v>10</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" t="b">
+        <v>1</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25">
+        <v>20</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B34">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="B35" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="B36" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="B37" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="B38" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="B39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="B40" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B41" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="B42" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="B43" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="B44" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="B45" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="B46">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="22" t="s">
+        <v>497</v>
+      </c>
+      <c r="B47">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="B48" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="B49" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="B50" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="B51" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="58">
-      <c r="A20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>549</v>
-      </c>
-      <c r="C20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="58">
-      <c r="A22" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>550</v>
-      </c>
-      <c r="C22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>70</v>
-      </c>
-      <c r="B23" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>73</v>
-      </c>
-      <c r="B24" t="s">
-        <v>74</v>
-      </c>
-      <c r="C24" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" t="s">
-        <v>77</v>
-      </c>
-      <c r="C25" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="52" spans="1:2">
+      <c r="A52" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="B52" t="s">
         <v>80</v>
       </c>
-      <c r="C26" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>82</v>
-      </c>
-      <c r="B27" t="s">
-        <v>83</v>
-      </c>
-      <c r="C27" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>85</v>
-      </c>
-      <c r="B28" t="s">
-        <v>331</v>
-      </c>
-      <c r="C28" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>87</v>
-      </c>
-      <c r="B29" t="s">
-        <v>88</v>
-      </c>
-      <c r="C29" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" t="s">
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="B53" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="B54" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="18" t="s">
+        <v>300</v>
+      </c>
+      <c r="B55" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="19" t="s">
+        <v>478</v>
+      </c>
+      <c r="B56" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="18" t="s">
+        <v>472</v>
+      </c>
+      <c r="B57" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="B58" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="23" t="s">
+        <v>526</v>
+      </c>
+      <c r="B59" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="43.5">
+      <c r="A60" s="23" t="s">
+        <v>527</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="23" t="s">
+        <v>318</v>
+      </c>
+      <c r="B61" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="29">
+      <c r="A62" s="23" t="s">
+        <v>320</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="23" t="s">
+        <v>324</v>
+      </c>
+      <c r="B63" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="58">
+      <c r="A64" s="23" t="s">
+        <v>325</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="23" t="s">
+        <v>313</v>
+      </c>
+      <c r="B65" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="58">
+      <c r="A66" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="15" t="s">
+        <v>334</v>
+      </c>
+      <c r="B67" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="15" t="s">
+        <v>336</v>
+      </c>
+      <c r="B68" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="15" t="s">
+        <v>338</v>
+      </c>
+      <c r="B69" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>340</v>
+      </c>
+      <c r="B70" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>342</v>
+      </c>
+      <c r="B71" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>344</v>
+      </c>
+      <c r="B72" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="25" t="s">
+        <v>353</v>
+      </c>
+      <c r="B73" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>356</v>
+      </c>
+      <c r="B75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="16" t="s">
+        <v>358</v>
+      </c>
+      <c r="B77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>373</v>
+      </c>
+      <c r="B78">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
         <v>381</v>
       </c>
-      <c r="C30" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>336</v>
-      </c>
-      <c r="B31" t="s">
-        <v>92</v>
-      </c>
-      <c r="C31" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>94</v>
-      </c>
-      <c r="B32" t="s">
-        <v>90</v>
-      </c>
-      <c r="C32" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B33" t="s">
-        <v>96</v>
-      </c>
-      <c r="C33" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B40" t="s">
-        <v>115</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B42">
-        <v>5000</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="B43">
-        <v>5</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="B44">
-        <v>2</v>
-      </c>
-      <c r="C44" s="21" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="23" t="s">
-        <v>446</v>
-      </c>
-      <c r="B45">
-        <v>10</v>
-      </c>
-      <c r="C45" s="21" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B46" t="b">
-        <v>1</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B47">
-        <v>20</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B48">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="B50" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="B51" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="B52" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="10" t="s">
-        <v>308</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="B54">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="B55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="24" t="s">
-        <v>222</v>
-      </c>
-      <c r="B57" t="str">
-        <f ca="1">TEXT(TODAY(), "yyyy-mm-dd")</f>
-        <v>2024-01-17</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="B58">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="B59">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="B60" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="B61" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="13" t="s">
-        <v>356</v>
-      </c>
-      <c r="B62" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="13" t="s">
-        <v>359</v>
-      </c>
-      <c r="B63" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="B64" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="B65" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="10" t="s">
-        <v>312</v>
-      </c>
-      <c r="B66" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="B67" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="13" t="s">
-        <v>357</v>
-      </c>
-      <c r="B68" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="B69" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="B70" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="B71">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="23" t="s">
-        <v>583</v>
-      </c>
-      <c r="B72">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73" t="s">
-        <v>332</v>
-      </c>
-      <c r="B73" t="str">
-        <f ca="1">TEXT(TODAY(), "mm/dd/yyyy")</f>
-        <v>01/17/2024</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="11" t="s">
-        <v>338</v>
-      </c>
-      <c r="B74" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="11" t="s">
-        <v>339</v>
-      </c>
-      <c r="B75" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76" s="11" t="s">
-        <v>342</v>
-      </c>
-      <c r="B76" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="B77" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="11" t="s">
-        <v>345</v>
-      </c>
-      <c r="B78" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="19" t="s">
-        <v>346</v>
-      </c>
-      <c r="B79" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
-      <c r="A80" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="B80" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="19" t="s">
-        <v>348</v>
-      </c>
-      <c r="B81" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="20" t="s">
-        <v>561</v>
-      </c>
-      <c r="B82" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="19" t="s">
-        <v>555</v>
-      </c>
-      <c r="B83" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="14" t="s">
-        <v>360</v>
-      </c>
-      <c r="B84" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="14" t="s">
-        <v>361</v>
-      </c>
-      <c r="B85" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="43.5">
-      <c r="A86" s="14" t="s">
-        <v>362</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" s="14" t="s">
-        <v>363</v>
-      </c>
-      <c r="B87" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2">
-      <c r="A88" s="14" t="s">
-        <v>364</v>
-      </c>
-      <c r="B88" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" s="14" t="s">
-        <v>365</v>
-      </c>
-      <c r="B89" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="29">
-      <c r="A90" s="14" t="s">
-        <v>367</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" s="14" t="s">
-        <v>368</v>
-      </c>
-      <c r="B91" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" s="14" t="s">
-        <v>369</v>
-      </c>
-      <c r="B92" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="14" t="s">
-        <v>370</v>
-      </c>
-      <c r="B93" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="58">
-      <c r="A94" s="14" t="s">
-        <v>372</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95" s="14" t="s">
-        <v>373</v>
-      </c>
-      <c r="B95" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
-      <c r="A96" s="14" t="s">
-        <v>374</v>
-      </c>
-      <c r="B96" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
-      <c r="A97" s="14" t="s">
-        <v>377</v>
-      </c>
-      <c r="B97" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="58">
-      <c r="A98" s="14" t="s">
-        <v>378</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2">
-      <c r="A99" s="14" t="s">
-        <v>379</v>
-      </c>
-      <c r="B99" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
-      <c r="A100" s="14" t="s">
-        <v>380</v>
-      </c>
-      <c r="B100" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2">
-      <c r="A101" s="15" t="s">
-        <v>392</v>
-      </c>
-      <c r="B101" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2">
-      <c r="A102" s="15" t="s">
-        <v>394</v>
-      </c>
-      <c r="B102" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2">
-      <c r="A103" s="15" t="s">
-        <v>396</v>
-      </c>
-      <c r="B103" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2">
-      <c r="A104" t="s">
-        <v>398</v>
-      </c>
-      <c r="B104" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2">
-      <c r="A105" t="s">
-        <v>400</v>
-      </c>
-      <c r="B105" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2">
-      <c r="A106" t="s">
-        <v>402</v>
-      </c>
-      <c r="B106" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2">
-      <c r="A107" t="s">
-        <v>423</v>
-      </c>
-      <c r="B107" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2">
-      <c r="A108" t="s">
-        <v>424</v>
-      </c>
-      <c r="B108" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2">
-      <c r="A109" t="s">
-        <v>426</v>
-      </c>
-      <c r="B109" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2">
-      <c r="A110" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2">
-      <c r="A111" t="s">
-        <v>428</v>
-      </c>
-      <c r="B111">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2">
-      <c r="A112" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3">
-      <c r="A113" s="16" t="s">
-        <v>430</v>
-      </c>
-      <c r="B113" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3">
-      <c r="A114" t="s">
-        <v>445</v>
-      </c>
-      <c r="B114">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3">
-      <c r="A115" t="s">
-        <v>451</v>
-      </c>
-      <c r="B115" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3">
-      <c r="A116" t="s">
-        <v>452</v>
-      </c>
-      <c r="B116" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3">
-      <c r="A117" t="s">
-        <v>453</v>
-      </c>
-      <c r="B117">
+      <c r="B79">
         <f ca="1">YEAR(TODAY())</f>
         <v>2024</v>
       </c>
     </row>
-    <row r="118" spans="1:3">
-      <c r="A118" t="s">
-        <v>454</v>
-      </c>
-      <c r="B118" t="s">
-        <v>504</v>
-      </c>
-      <c r="C118" t="str">
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>382</v>
+      </c>
+      <c r="C80" t="str">
         <f ca="1">TEXT(MONTH(NOW()),"mmmm")</f>
         <v>January</v>
       </c>
     </row>
-    <row r="119" spans="1:3">
-      <c r="A119" t="s">
-        <v>491</v>
-      </c>
-      <c r="C119" t="str">
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>416</v>
+      </c>
+      <c r="C81" t="str">
         <f ca="1">TEXT(NOW(),"mm-dd hhmm")</f>
-        <v>01-17 1953</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
-      <c r="A120" t="s">
-        <v>502</v>
-      </c>
-      <c r="B120" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3">
-      <c r="A121" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3">
-      <c r="A122" t="s">
-        <v>518</v>
-      </c>
-      <c r="B122">
+        <v>01-18 2235</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>427</v>
+      </c>
+      <c r="B82" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>438</v>
+      </c>
+      <c r="B84">
         <v>90</v>
       </c>
     </row>
-    <row r="123" spans="1:3">
-      <c r="A123" t="s">
-        <v>531</v>
-      </c>
-      <c r="B123" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3">
-      <c r="A124" t="s">
-        <v>535</v>
-      </c>
-      <c r="B124" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3">
-      <c r="A125" t="s">
-        <v>544</v>
-      </c>
-      <c r="B125" t="s">
-        <v>503</v>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>450</v>
+      </c>
+      <c r="B85" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>454</v>
+      </c>
+      <c r="B86" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>463</v>
+      </c>
+      <c r="B87" t="s">
+        <v>428</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="21"/>
+  <phoneticPr fontId="20"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3611,15 +3116,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="1" max="1" width="33.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4765,23 +4270,23 @@
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="21"/>
+  <phoneticPr fontId="20"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:Z21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="31.90625" customWidth="1"/>
-    <col min="2" max="2" width="39.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.36328125" customWidth="1"/>
     <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
@@ -4791,7 +4296,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>187</v>
+        <v>145</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>27</v>
@@ -4824,24 +4329,236 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>185</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>184</v>
+        <v>504</v>
+      </c>
+      <c r="C2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="A3" t="s">
+        <v>505</v>
+      </c>
+      <c r="B3" t="s">
+        <v>506</v>
+      </c>
+      <c r="C3" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>507</v>
+      </c>
+      <c r="C4" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>508</v>
+      </c>
+      <c r="C5" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>509</v>
+      </c>
+      <c r="C6" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>510</v>
+      </c>
+      <c r="C7" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
+      <c r="A8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" t="s">
+        <v>539</v>
+      </c>
+      <c r="C8" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
+      <c r="A9" t="s">
+        <v>352</v>
+      </c>
+      <c r="B9" t="s">
+        <v>511</v>
+      </c>
+      <c r="C9" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="A10" s="23" t="s">
+        <v>528</v>
+      </c>
+      <c r="B10" t="s">
+        <v>531</v>
+      </c>
+      <c r="C10" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="A11" s="23" t="s">
+        <v>529</v>
+      </c>
+      <c r="B11" t="s">
+        <v>532</v>
+      </c>
+      <c r="C11" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
+      <c r="A12" s="23" t="s">
+        <v>321</v>
+      </c>
+      <c r="B12" t="s">
+        <v>512</v>
+      </c>
+      <c r="C12" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
+      <c r="A13" s="23" t="s">
+        <v>322</v>
+      </c>
+      <c r="B13" t="s">
+        <v>513</v>
+      </c>
+      <c r="C13" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="A14" s="23" t="s">
+        <v>326</v>
+      </c>
+      <c r="B14" t="s">
+        <v>514</v>
+      </c>
+      <c r="C14" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" s="23" t="s">
+        <v>327</v>
+      </c>
+      <c r="B15" t="s">
+        <v>515</v>
+      </c>
+      <c r="C15" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16" s="23" t="s">
+        <v>316</v>
+      </c>
+      <c r="B16" t="s">
+        <v>533</v>
+      </c>
+      <c r="C16" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="B17" t="s">
+        <v>534</v>
+      </c>
+      <c r="C17" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="23" t="s">
+        <v>516</v>
+      </c>
+      <c r="B18" t="s">
+        <v>517</v>
+      </c>
+      <c r="C18" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>379</v>
+      </c>
+      <c r="B19" t="s">
+        <v>535</v>
+      </c>
+      <c r="C19" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="23" t="s">
+        <v>380</v>
+      </c>
+      <c r="B20" t="s">
+        <v>536</v>
+      </c>
+      <c r="C20" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="B21" t="s">
+        <v>540</v>
+      </c>
+      <c r="C21" t="s">
+        <v>500</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="21"/>
+  <phoneticPr fontId="20"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D9DC59-3960-42CB-B3EC-EFF452A90D4F}">
-  <dimension ref="A1:Z165"/>
+  <dimension ref="A1:Z166"/>
   <sheetViews>
-    <sheetView topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="B144" sqref="B144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4887,1314 +4604,1322 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>388</v>
+        <v>518</v>
       </c>
       <c r="B4" t="s">
-        <v>389</v>
+        <v>520</v>
       </c>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
-        <v>390</v>
+        <v>519</v>
       </c>
       <c r="B5" t="s">
-        <v>391</v>
+        <v>521</v>
       </c>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
-        <v>417</v>
+        <v>346</v>
       </c>
       <c r="B6" t="s">
-        <v>418</v>
+        <v>347</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" t="s">
-        <v>419</v>
+        <v>348</v>
       </c>
       <c r="B7" t="s">
-        <v>420</v>
+        <v>349</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
-        <v>421</v>
+        <v>350</v>
       </c>
       <c r="B8" t="s">
-        <v>422</v>
+        <v>351</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
       <c r="B9" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>97</v>
       </c>
       <c r="B10" t="s">
-        <v>141</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" t="s">
-        <v>188</v>
+        <v>146</v>
       </c>
       <c r="B11" t="s">
-        <v>191</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" t="s">
-        <v>193</v>
+        <v>151</v>
       </c>
       <c r="B12" t="s">
-        <v>199</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" t="s">
-        <v>194</v>
+        <v>152</v>
       </c>
       <c r="B13" t="s">
-        <v>198</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" t="s">
-        <v>195</v>
+        <v>153</v>
       </c>
       <c r="B14" t="s">
-        <v>198</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" t="s">
-        <v>196</v>
+        <v>154</v>
       </c>
       <c r="B15" t="s">
-        <v>200</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:26">
       <c r="A16" t="s">
-        <v>197</v>
+        <v>155</v>
       </c>
       <c r="B16" t="s">
-        <v>201</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>189</v>
+        <v>147</v>
       </c>
       <c r="B17" t="s">
-        <v>192</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>190</v>
+        <v>148</v>
       </c>
       <c r="B18" t="s">
-        <v>202</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>204</v>
+        <v>162</v>
       </c>
       <c r="B19" t="s">
-        <v>203</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>209</v>
+        <v>167</v>
       </c>
       <c r="B20" t="s">
-        <v>208</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>210</v>
+        <v>168</v>
       </c>
       <c r="B21" t="s">
-        <v>211</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>212</v>
+        <v>170</v>
       </c>
       <c r="B22" t="s">
-        <v>211</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>205</v>
+        <v>163</v>
       </c>
       <c r="B23" t="s">
-        <v>207</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>206</v>
+        <v>164</v>
       </c>
       <c r="B24" t="s">
-        <v>213</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>215</v>
+        <v>173</v>
       </c>
       <c r="B25" t="s">
-        <v>214</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>224</v>
+        <v>180</v>
       </c>
       <c r="B26" t="s">
-        <v>223</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>227</v>
+        <v>183</v>
       </c>
       <c r="B27" t="s">
-        <v>226</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>572</v>
+        <v>489</v>
       </c>
       <c r="B28" t="s">
-        <v>573</v>
+        <v>490</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>229</v>
+        <v>185</v>
       </c>
       <c r="B29" t="s">
-        <v>228</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>230</v>
+        <v>186</v>
       </c>
       <c r="B30" t="s">
-        <v>231</v>
+        <v>187</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>232</v>
+        <v>188</v>
       </c>
       <c r="B31" t="s">
-        <v>231</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>234</v>
+        <v>190</v>
       </c>
       <c r="B32" t="s">
-        <v>233</v>
+        <v>189</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>236</v>
+        <v>192</v>
       </c>
       <c r="B33" t="s">
-        <v>235</v>
+        <v>191</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>237</v>
+        <v>193</v>
       </c>
       <c r="B34" t="s">
-        <v>235</v>
+        <v>191</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>241</v>
+        <v>197</v>
       </c>
       <c r="B35" t="s">
-        <v>238</v>
+        <v>194</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>239</v>
+        <v>195</v>
       </c>
       <c r="B36" t="s">
-        <v>242</v>
+        <v>198</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>240</v>
+        <v>196</v>
       </c>
       <c r="B37" t="s">
-        <v>243</v>
+        <v>199</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>216</v>
+        <v>174</v>
       </c>
       <c r="B38" t="s">
-        <v>247</v>
+        <v>203</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>217</v>
+        <v>175</v>
       </c>
       <c r="B39" t="s">
-        <v>245</v>
+        <v>201</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>218</v>
+        <v>176</v>
       </c>
       <c r="B40" t="s">
-        <v>246</v>
+        <v>202</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>249</v>
+        <v>205</v>
       </c>
       <c r="B41" t="s">
-        <v>248</v>
+        <v>204</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>438</v>
+        <v>366</v>
       </c>
       <c r="B42" t="s">
-        <v>439</v>
+        <v>367</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>433</v>
+        <v>361</v>
       </c>
       <c r="B43" t="s">
-        <v>440</v>
+        <v>368</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>434</v>
+        <v>362</v>
       </c>
       <c r="B44" t="s">
-        <v>441</v>
+        <v>369</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>435</v>
+        <v>363</v>
       </c>
       <c r="B45" t="s">
-        <v>442</v>
+        <v>370</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>436</v>
+        <v>364</v>
       </c>
       <c r="B46" t="s">
-        <v>520</v>
+        <v>439</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>437</v>
+        <v>365</v>
       </c>
       <c r="B47" t="s">
-        <v>520</v>
+        <v>439</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>255</v>
+        <v>211</v>
       </c>
       <c r="B48" t="s">
-        <v>443</v>
+        <v>371</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>256</v>
+        <v>212</v>
       </c>
       <c r="B49" t="s">
-        <v>443</v>
+        <v>371</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>250</v>
+        <v>206</v>
       </c>
       <c r="B50" t="s">
-        <v>257</v>
+        <v>213</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>251</v>
+        <v>207</v>
       </c>
       <c r="B51" t="s">
-        <v>258</v>
+        <v>214</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>259</v>
+        <v>215</v>
       </c>
       <c r="B52" t="s">
-        <v>262</v>
+        <v>218</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>267</v>
+        <v>223</v>
       </c>
       <c r="B53" t="s">
-        <v>269</v>
+        <v>225</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>266</v>
+        <v>222</v>
       </c>
       <c r="B54" t="s">
-        <v>265</v>
+        <v>221</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>271</v>
+        <v>227</v>
       </c>
       <c r="B55" t="s">
-        <v>270</v>
+        <v>226</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>268</v>
+        <v>224</v>
       </c>
       <c r="B56" t="s">
-        <v>265</v>
+        <v>221</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>278</v>
+        <v>234</v>
       </c>
       <c r="B57" t="s">
-        <v>444</v>
+        <v>372</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>447</v>
+        <v>375</v>
       </c>
       <c r="B58" t="s">
-        <v>449</v>
+        <v>377</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>553</v>
+        <v>470</v>
       </c>
       <c r="B59" t="s">
-        <v>554</v>
+        <v>471</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>448</v>
+        <v>376</v>
       </c>
       <c r="B60" t="s">
-        <v>450</v>
+        <v>378</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>260</v>
+        <v>216</v>
       </c>
       <c r="B61" t="s">
-        <v>263</v>
+        <v>219</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>261</v>
+        <v>217</v>
       </c>
       <c r="B62" t="s">
-        <v>264</v>
+        <v>220</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>274</v>
+        <v>230</v>
       </c>
       <c r="B63" t="s">
-        <v>273</v>
+        <v>229</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>276</v>
+        <v>232</v>
       </c>
       <c r="B64" t="s">
-        <v>275</v>
+        <v>231</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>277</v>
+        <v>233</v>
       </c>
       <c r="B65" t="s">
-        <v>279</v>
+        <v>235</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>278</v>
+        <v>234</v>
       </c>
       <c r="B66" t="s">
-        <v>279</v>
+        <v>235</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>283</v>
+        <v>239</v>
       </c>
       <c r="B67" t="s">
-        <v>282</v>
+        <v>238</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>534</v>
+        <v>453</v>
       </c>
       <c r="B68" t="s">
-        <v>533</v>
+        <v>452</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>285</v>
+        <v>241</v>
       </c>
       <c r="B69" t="s">
-        <v>288</v>
+        <v>244</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>286</v>
+        <v>242</v>
       </c>
       <c r="B70" t="s">
-        <v>284</v>
+        <v>240</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>287</v>
+        <v>243</v>
       </c>
       <c r="B71" t="s">
-        <v>284</v>
+        <v>240</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>289</v>
+        <v>245</v>
       </c>
       <c r="B72" t="s">
-        <v>292</v>
+        <v>248</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>290</v>
+        <v>246</v>
       </c>
       <c r="B73" t="s">
-        <v>293</v>
+        <v>249</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>291</v>
+        <v>247</v>
       </c>
       <c r="B74" t="s">
-        <v>293</v>
+        <v>249</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>297</v>
+        <v>253</v>
       </c>
       <c r="B75" t="s">
-        <v>298</v>
+        <v>254</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="B76" t="s">
-        <v>299</v>
+        <v>255</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>301</v>
+        <v>257</v>
       </c>
       <c r="B77" t="s">
-        <v>302</v>
+        <v>258</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>508</v>
+        <v>522</v>
       </c>
       <c r="B78" t="s">
-        <v>507</v>
+        <v>523</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>294</v>
+        <v>250</v>
       </c>
       <c r="B79" t="s">
-        <v>296</v>
+        <v>252</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>295</v>
+        <v>251</v>
       </c>
       <c r="B80" t="s">
-        <v>303</v>
+        <v>259</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>563</v>
+        <v>480</v>
       </c>
       <c r="B81" t="s">
-        <v>579</v>
+        <v>493</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>310</v>
+        <v>266</v>
       </c>
       <c r="B82" t="s">
-        <v>309</v>
+        <v>265</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>311</v>
+        <v>267</v>
       </c>
       <c r="B83" t="s">
-        <v>557</v>
+        <v>474</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>559</v>
+        <v>476</v>
       </c>
       <c r="B84" t="s">
-        <v>560</v>
+        <v>477</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>556</v>
+        <v>473</v>
       </c>
       <c r="B85" t="s">
-        <v>558</v>
+        <v>475</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>320</v>
+        <v>276</v>
       </c>
       <c r="B86" t="s">
-        <v>319</v>
+        <v>275</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>322</v>
+        <v>278</v>
       </c>
       <c r="B87" t="s">
-        <v>321</v>
+        <v>277</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>551</v>
+        <v>524</v>
       </c>
       <c r="B88" t="s">
-        <v>321</v>
+        <v>525</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>564</v>
+        <v>481</v>
       </c>
       <c r="B89" t="s">
-        <v>580</v>
+        <v>494</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>565</v>
+        <v>482</v>
       </c>
       <c r="B90" t="s">
-        <v>581</v>
+        <v>495</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>566</v>
+        <v>483</v>
       </c>
       <c r="B91" t="s">
-        <v>582</v>
+        <v>496</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>325</v>
+        <v>281</v>
       </c>
       <c r="B92" t="s">
-        <v>328</v>
+        <v>284</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>334</v>
+        <v>288</v>
       </c>
       <c r="B93" t="s">
-        <v>333</v>
+        <v>287</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>335</v>
+        <v>289</v>
       </c>
       <c r="B94" t="s">
-        <v>539</v>
+        <v>458</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>538</v>
+        <v>457</v>
       </c>
       <c r="B95" t="s">
-        <v>539</v>
+        <v>458</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>541</v>
+        <v>460</v>
       </c>
       <c r="B96" t="s">
-        <v>540</v>
+        <v>459</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>542</v>
+        <v>461</v>
       </c>
       <c r="B97" t="s">
-        <v>543</v>
+        <v>462</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>326</v>
+        <v>282</v>
       </c>
       <c r="B98" t="s">
-        <v>329</v>
+        <v>285</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>327</v>
+        <v>283</v>
       </c>
       <c r="B99" t="s">
-        <v>330</v>
+        <v>286</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>151</v>
+        <v>111</v>
       </c>
       <c r="B100" t="s">
-        <v>150</v>
+        <v>110</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>155</v>
+        <v>115</v>
       </c>
       <c r="B101" t="s">
-        <v>156</v>
+        <v>116</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>158</v>
+        <v>118</v>
       </c>
       <c r="B102" t="s">
-        <v>157</v>
+        <v>117</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>152</v>
+        <v>112</v>
       </c>
       <c r="B103" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>153</v>
+        <v>113</v>
       </c>
       <c r="B104" t="s">
-        <v>159</v>
+        <v>119</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="B105" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>162</v>
+        <v>122</v>
       </c>
       <c r="B106" t="s">
-        <v>511</v>
+        <v>432</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>163</v>
+        <v>123</v>
       </c>
       <c r="B107" t="s">
-        <v>510</v>
+        <v>431</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>165</v>
+        <v>125</v>
       </c>
       <c r="B108" t="s">
-        <v>164</v>
+        <v>124</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>431</v>
+        <v>359</v>
       </c>
       <c r="B109" t="s">
-        <v>432</v>
+        <v>360</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>169</v>
+        <v>129</v>
       </c>
       <c r="B110" t="s">
-        <v>170</v>
+        <v>130</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>171</v>
+        <v>131</v>
       </c>
       <c r="B111" t="s">
-        <v>170</v>
+        <v>130</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>172</v>
+        <v>132</v>
       </c>
       <c r="B112" t="s">
-        <v>173</v>
+        <v>133</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>174</v>
+        <v>134</v>
       </c>
       <c r="B113" t="s">
-        <v>175</v>
+        <v>135</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>176</v>
+        <v>136</v>
       </c>
       <c r="B114" t="s">
-        <v>177</v>
+        <v>137</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>179</v>
+        <v>139</v>
       </c>
       <c r="B115" t="s">
-        <v>178</v>
+        <v>138</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="B116" t="s">
-        <v>178</v>
+        <v>138</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>166</v>
+        <v>126</v>
       </c>
       <c r="B117" t="s">
-        <v>337</v>
+        <v>291</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>167</v>
+        <v>127</v>
       </c>
       <c r="B118" t="s">
-        <v>182</v>
+        <v>142</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>168</v>
+        <v>128</v>
       </c>
       <c r="B119" t="s">
-        <v>181</v>
+        <v>141</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>382</v>
+        <v>328</v>
       </c>
       <c r="B120" t="s">
-        <v>383</v>
+        <v>329</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>512</v>
+        <v>433</v>
       </c>
       <c r="B121" t="s">
-        <v>514</v>
+        <v>435</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>513</v>
+        <v>434</v>
       </c>
       <c r="B122" t="s">
-        <v>515</v>
+        <v>436</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>384</v>
+        <v>330</v>
       </c>
       <c r="B123" t="s">
-        <v>385</v>
+        <v>331</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>386</v>
+        <v>332</v>
       </c>
       <c r="B124" t="s">
-        <v>387</v>
+        <v>333</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>455</v>
+        <v>383</v>
       </c>
       <c r="B125" t="s">
-        <v>462</v>
+        <v>390</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>458</v>
+        <v>386</v>
       </c>
       <c r="B126" t="s">
-        <v>466</v>
+        <v>394</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>459</v>
+        <v>387</v>
       </c>
       <c r="B127" t="s">
-        <v>465</v>
+        <v>393</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>460</v>
+        <v>388</v>
       </c>
       <c r="B128" t="s">
-        <v>469</v>
+        <v>397</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>461</v>
+        <v>389</v>
       </c>
       <c r="B129" t="s">
-        <v>468</v>
+        <v>396</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>467</v>
+        <v>395</v>
       </c>
       <c r="B130" t="s">
-        <v>468</v>
+        <v>396</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>456</v>
+        <v>384</v>
       </c>
       <c r="B131" t="s">
-        <v>463</v>
+        <v>391</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>457</v>
+        <v>385</v>
       </c>
       <c r="B132" t="s">
-        <v>464</v>
+        <v>392</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>470</v>
+        <v>398</v>
       </c>
       <c r="B133" t="s">
-        <v>471</v>
+        <v>399</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>476</v>
+        <v>404</v>
       </c>
       <c r="B134" t="s">
-        <v>466</v>
+        <v>394</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>477</v>
+        <v>405</v>
       </c>
       <c r="B135" t="s">
-        <v>465</v>
+        <v>393</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>478</v>
+        <v>406</v>
       </c>
       <c r="B136" t="s">
-        <v>468</v>
+        <v>396</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>474</v>
+        <v>402</v>
       </c>
       <c r="B137" t="s">
-        <v>472</v>
+        <v>400</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>475</v>
+        <v>403</v>
       </c>
       <c r="B138" t="s">
-        <v>473</v>
+        <v>401</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>479</v>
+        <v>407</v>
       </c>
       <c r="B139" t="s">
-        <v>482</v>
+        <v>410</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>485</v>
+        <v>544</v>
       </c>
       <c r="B140" t="s">
-        <v>487</v>
+        <v>541</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>486</v>
+        <v>414</v>
       </c>
       <c r="B141" t="s">
-        <v>489</v>
+        <v>542</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>488</v>
+        <v>415</v>
       </c>
       <c r="B142" t="s">
-        <v>490</v>
+        <v>543</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>492</v>
+        <v>413</v>
       </c>
       <c r="B143" t="s">
-        <v>494</v>
+        <v>545</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>493</v>
+        <v>417</v>
       </c>
       <c r="B144" t="s">
-        <v>495</v>
+        <v>419</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>496</v>
+        <v>418</v>
       </c>
       <c r="B145" t="s">
-        <v>498</v>
+        <v>420</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>497</v>
+        <v>421</v>
       </c>
       <c r="B146" t="s">
-        <v>499</v>
+        <v>423</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>500</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>501</v>
+        <v>422</v>
+      </c>
+      <c r="B147" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="148" spans="1:2">
-      <c r="A148" s="2" t="s">
-        <v>505</v>
+      <c r="A148" t="s">
+        <v>425</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>537</v>
+        <v>426</v>
       </c>
     </row>
     <row r="149" spans="1:2">
-      <c r="A149" t="s">
-        <v>480</v>
-      </c>
-      <c r="B149" t="s">
-        <v>483</v>
+      <c r="A149" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>481</v>
+        <v>408</v>
       </c>
       <c r="B150" t="s">
-        <v>484</v>
+        <v>411</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>305</v>
+        <v>409</v>
       </c>
       <c r="B151" t="s">
-        <v>304</v>
+        <v>412</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>521</v>
+        <v>261</v>
       </c>
       <c r="B152" t="s">
-        <v>440</v>
+        <v>260</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>522</v>
+        <v>440</v>
       </c>
       <c r="B153" t="s">
-        <v>441</v>
+        <v>368</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>523</v>
+        <v>441</v>
       </c>
       <c r="B154" t="s">
-        <v>442</v>
+        <v>369</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>524</v>
+        <v>442</v>
       </c>
       <c r="B155" t="s">
-        <v>520</v>
+        <v>370</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>525</v>
+        <v>443</v>
       </c>
       <c r="B156" t="s">
-        <v>520</v>
+        <v>439</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>526</v>
+        <v>444</v>
       </c>
       <c r="B157" t="s">
-        <v>529</v>
+        <v>439</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>527</v>
+        <v>445</v>
       </c>
       <c r="B158" t="s">
-        <v>530</v>
+        <v>448</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>528</v>
+        <v>446</v>
       </c>
       <c r="B159" t="s">
-        <v>530</v>
+        <v>449</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>317</v>
+        <v>447</v>
       </c>
       <c r="B160" t="s">
-        <v>578</v>
+        <v>449</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>567</v>
+        <v>273</v>
       </c>
       <c r="B161" t="s">
-        <v>570</v>
+        <v>492</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>568</v>
+        <v>484</v>
       </c>
       <c r="B162" t="s">
-        <v>571</v>
+        <v>487</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>569</v>
+        <v>485</v>
       </c>
       <c r="B163" t="s">
-        <v>571</v>
+        <v>488</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>306</v>
+        <v>486</v>
       </c>
       <c r="B164" t="s">
-        <v>323</v>
+        <v>488</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>307</v>
+        <v>262</v>
       </c>
       <c r="B165" t="s">
-        <v>324</v>
+        <v>279</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2">
+      <c r="A166" t="s">
+        <v>263</v>
+      </c>
+      <c r="B166" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made changes to Graph Api combined library and Kill workflow
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55651C\Documents\GitHub\P0002_090_PayCyleAfternoon_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D868411B-71AE-4F78-8DCC-B13DB39B5D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814EE685-8A4A-4D38-9B61-1B7693E097D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="546">
   <si>
     <t>Name</t>
   </si>
@@ -99,11 +99,11 @@
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="20"/>
+    <phoneticPr fontId="21"/>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="20"/>
+    <phoneticPr fontId="21"/>
   </si>
   <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
@@ -256,27 +256,18 @@
     <t>Kill_excel</t>
   </si>
   <si>
-    <t>Excel.exe</t>
-  </si>
-  <si>
     <t>Excel exe name to kill excel instance</t>
   </si>
   <si>
     <t>Kill_msedge</t>
   </si>
   <si>
-    <t>msedge.exe</t>
-  </si>
-  <si>
     <t>Edge exe name to kill instance</t>
   </si>
   <si>
     <t>Kill_Outlook</t>
   </si>
   <si>
-    <t>outlook.exe</t>
-  </si>
-  <si>
     <t>Outlook exe name to kill instance</t>
   </si>
   <si>
@@ -955,9 +946,6 @@
     <t>Last step not showing as "complete"</t>
   </si>
   <si>
-    <t>udbhavagarwal's workspace</t>
-  </si>
-  <si>
     <t>P002_090_PayCycleAfternoon_Performer</t>
   </si>
   <si>
@@ -1100,9 +1088,6 @@
   </si>
   <si>
     <t>OrchestratorGraphAPIAssetsFolder</t>
-  </si>
-  <si>
-    <t>DEV</t>
   </si>
   <si>
     <t>BotPeoplesoftUserID</t>
@@ -1541,142 +1526,157 @@
     <t>PeopleSoftLoginCredentailsFolderName</t>
   </si>
   <si>
+    <t>ProcessFolderName</t>
+  </si>
+  <si>
+    <t>PaycycleAfternoon_Performer</t>
+  </si>
+  <si>
+    <t>00:02:00</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_PeopleSoftLoginURL</t>
+  </si>
+  <si>
+    <t>PeopleSoft_NavigationURL</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_PeopleSoftNavigationURL</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_CcRecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_RecipientEmailAddressSE</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_CcRecipientEmailAddressSE</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SenderEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_2RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_2CCEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_3RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_3CCEmailAddress</t>
+  </si>
+  <si>
+    <t>LocalRootFolderPath</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_LocalRootFolderPath</t>
+  </si>
+  <si>
+    <t>PeoplesoftLoginCredentialsSE_3</t>
+  </si>
+  <si>
+    <t>PeoplesoftLoginPageUnavailableSE_2</t>
+  </si>
+  <si>
+    <t>SE_3: Credentials Error.</t>
+  </si>
+  <si>
+    <t>SE_2: Peoplesoft Unavailable.</t>
+  </si>
+  <si>
+    <t>PaycycleStatusNotChangedSE_1</t>
+  </si>
+  <si>
+    <t>SE_1: Paycycle was not approved as the correct status not found even after retries.</t>
+  </si>
+  <si>
+    <t>StatusCompletedNotAppearedBE_4</t>
+  </si>
+  <si>
+    <t>BE_4: Status is not completed , so the record will be marked as an exception.</t>
+  </si>
+  <si>
+    <t>BE_4Subject</t>
+  </si>
+  <si>
+    <t>BE_4Body</t>
+  </si>
+  <si>
+    <t>BE_4RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>BE_4CCEmailAddress</t>
+  </si>
+  <si>
+    <t>BE_4,SE_1,SE_2,SE_3</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_BE_4RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_BE_4CCEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_1RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_1CCEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SharepointURL</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SharepointSubFolder</t>
+  </si>
+  <si>
+    <t>QUEUED</t>
+  </si>
+  <si>
+    <t>PROCESSING</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_RefreshMonitorBotUserID</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_CalenderNameOrchestrator</t>
+  </si>
+  <si>
+    <t>Local Root Folder Present.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Local Root Folder Not Present. Path: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Local Root Folder Not Found. Path: </t>
+  </si>
+  <si>
+    <t>LocalRootFolderPresent</t>
+  </si>
+  <si>
+    <t>Local Process Folder Present.</t>
+  </si>
+  <si>
+    <t>PROD/P002_090_PayCycleAfternoon</t>
+  </si>
+  <si>
     <t>DEV/P002_PayCycleAfternoon</t>
   </si>
   <si>
-    <t>ProcessFolderName</t>
-  </si>
-  <si>
-    <t>PaycycleAfternoon_Performer</t>
-  </si>
-  <si>
-    <t>00:02:00</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_PeopleSoftLoginURL</t>
-  </si>
-  <si>
-    <t>PeopleSoft_NavigationURL</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_PeopleSoftNavigationURL</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_RecipientEmailAddress</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_CcRecipientEmailAddress</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_RecipientEmailAddressSE</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_CcRecipientEmailAddressSE</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_SenderEmailAddress</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_SE_2RecipientEmailAddress</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_SE_2CCEmailAddress</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_SE_3RecipientEmailAddress</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_SE_3CCEmailAddress</t>
-  </si>
-  <si>
-    <t>LocalRootFolderPath</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_LocalRootFolderPath</t>
-  </si>
-  <si>
-    <t>PeoplesoftLoginCredentialsSE_3</t>
-  </si>
-  <si>
-    <t>PeoplesoftLoginPageUnavailableSE_2</t>
-  </si>
-  <si>
-    <t>SE_3: Credentials Error.</t>
-  </si>
-  <si>
-    <t>SE_2: Peoplesoft Unavailable.</t>
-  </si>
-  <si>
-    <t>PaycycleStatusNotChangedSE_1</t>
-  </si>
-  <si>
-    <t>SE_1: Paycycle was not approved as the correct status not found even after retries.</t>
-  </si>
-  <si>
-    <t>StatusCompletedNotAppearedBE_4</t>
-  </si>
-  <si>
-    <t>BE_4: Status is not completed , so the record will be marked as an exception.</t>
-  </si>
-  <si>
-    <t>BE_4Subject</t>
-  </si>
-  <si>
-    <t>BE_4Body</t>
-  </si>
-  <si>
-    <t>BE_4RecipientEmailAddress</t>
-  </si>
-  <si>
-    <t>BE_4CCEmailAddress</t>
-  </si>
-  <si>
-    <t>BE_4,SE_1,SE_2,SE_3</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_BE_4RecipientEmailAddress</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_BE_4CCEmailAddress</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_SE_1RecipientEmailAddress</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_SE_1CCEmailAddress</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_SharepointURL</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_SharepointSubFolder</t>
-  </si>
-  <si>
-    <t>QUEUED</t>
-  </si>
-  <si>
-    <t>PROCESSING</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_RefreshMonitorBotUserID</t>
-  </si>
-  <si>
-    <t>P002_090_PayCycleAfternoon_CalenderNameOrchestrator</t>
-  </si>
-  <si>
-    <t>Local Root Folder Present.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Local Root Folder Not Present. Path: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Local Root Folder Not Found. Path: </t>
-  </si>
-  <si>
-    <t>LocalRootFolderPresent</t>
-  </si>
-  <si>
-    <t>Local Process Folder Present.</t>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>excel</t>
+  </si>
+  <si>
+    <t>msedge</t>
+  </si>
+  <si>
+    <t>outlook</t>
   </si>
 </sst>
 </file>
@@ -1686,11 +1686,18 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1868,7 +1875,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1878,12 +1885,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="49"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1913,51 +1914,52 @@
   </borders>
   <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="4" fontId="25" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="4" fontId="26" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="1"/>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="1"/>
@@ -1969,8 +1971,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="20" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="22">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{DA952E48-534A-4104-8A72-2BE892964A18}"/>
@@ -2308,8 +2308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -2356,21 +2356,21 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.5">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>305</v>
+        <v>541</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>29</v>
@@ -2381,7 +2381,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>21</v>
@@ -2392,18 +2392,18 @@
         <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" s="25" t="s">
-        <v>499</v>
+      <c r="A6" t="s">
+        <v>494</v>
       </c>
       <c r="B6" t="s">
-        <v>500</v>
+        <v>541</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="72.5">
@@ -2411,7 +2411,7 @@
         <v>48</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="C7" t="s">
         <v>49</v>
@@ -2433,7 +2433,7 @@
         <v>53</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="C9" t="s">
         <v>54</v>
@@ -2474,10 +2474,10 @@
     </row>
     <row r="13" spans="1:26">
       <c r="A13" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="B13" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="C13" t="s">
         <v>64</v>
@@ -2485,7 +2485,7 @@
     </row>
     <row r="14" spans="1:26">
       <c r="A14" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B14" t="s">
         <v>66</v>
@@ -2507,117 +2507,117 @@
     </row>
     <row r="16" spans="1:26">
       <c r="A16" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B16" t="s">
         <v>70</v>
       </c>
       <c r="C16" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="23" t="s">
+        <v>543</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>544</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>545</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B20">
         <v>5000</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="21" t="s">
-        <v>83</v>
+      <c r="A21" s="24" t="s">
+        <v>80</v>
       </c>
       <c r="B21">
         <v>5</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="17" t="s">
-        <v>85</v>
+      <c r="A22" s="16" t="s">
+        <v>82</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
-      <c r="C22" s="20" t="s">
-        <v>86</v>
+      <c r="C22" s="19" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="22" t="s">
-        <v>374</v>
+      <c r="A23" s="20" t="s">
+        <v>369</v>
       </c>
       <c r="B23">
         <v>10</v>
       </c>
-      <c r="C23" s="20" t="s">
-        <v>491</v>
+      <c r="C23" s="19" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="5" t="s">
-        <v>87</v>
+      <c r="A24" s="24" t="s">
+        <v>84</v>
       </c>
       <c r="B24" t="b">
         <v>1</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B25">
         <v>20</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B26">
         <v>5</v>
@@ -2625,7 +2625,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -2633,31 +2633,31 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B28" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B29" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="10" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="10" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B31">
         <v>10</v>
@@ -2665,7 +2665,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -2673,7 +2673,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="9" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B33">
         <v>10</v>
@@ -2681,7 +2681,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="10" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B34">
         <v>90</v>
@@ -2689,39 +2689,39 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="13" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B35" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B36" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="13" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B37" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="13" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B38" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="10" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B39" t="b">
         <v>1</v>
@@ -2729,95 +2729,95 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="10" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B40" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="10" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B41" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B42" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="13" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B43" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="13" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B44" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="10" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B45" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="10" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B46">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="22" t="s">
-        <v>497</v>
+      <c r="A47" s="20" t="s">
+        <v>492</v>
       </c>
       <c r="B47">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="11" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B48" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="11" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B49" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="11" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B50" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="11" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B51" t="s">
         <v>59</v>
@@ -2825,188 +2825,188 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="11" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B52" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="18" t="s">
+      <c r="A53" s="17" t="s">
+        <v>295</v>
+      </c>
+      <c r="B53" t="s">
         <v>298</v>
-      </c>
-      <c r="B53" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="B54" t="s">
         <v>299</v>
       </c>
-      <c r="B54" t="s">
-        <v>302</v>
-      </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="18" t="s">
+      <c r="A55" s="17" t="s">
+        <v>297</v>
+      </c>
+      <c r="B55" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="18" t="s">
+        <v>473</v>
+      </c>
+      <c r="B56" t="s">
         <v>300</v>
       </c>
-      <c r="B55" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="19" t="s">
-        <v>478</v>
-      </c>
-      <c r="B56" t="s">
-        <v>303</v>
-      </c>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57" s="18" t="s">
-        <v>472</v>
+      <c r="A57" s="17" t="s">
+        <v>467</v>
       </c>
       <c r="B57" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58" s="14" t="s">
-        <v>312</v>
+      <c r="A58" s="22" t="s">
+        <v>308</v>
       </c>
       <c r="B58" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="23" t="s">
-        <v>526</v>
+      <c r="A59" s="21" t="s">
+        <v>520</v>
       </c>
       <c r="B59" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="43.5">
-      <c r="A60" s="23" t="s">
-        <v>527</v>
+      <c r="A60" s="21" t="s">
+        <v>521</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61" s="23" t="s">
-        <v>318</v>
+      <c r="A61" s="21" t="s">
+        <v>314</v>
       </c>
       <c r="B61" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="29">
-      <c r="A62" s="23" t="s">
+      <c r="A62" s="21" t="s">
+        <v>316</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="21" t="s">
         <v>320</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="23" t="s">
-        <v>324</v>
-      </c>
       <c r="B63" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="58">
-      <c r="A64" s="23" t="s">
-        <v>325</v>
+      <c r="A64" s="21" t="s">
+        <v>321</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="23" t="s">
-        <v>313</v>
+      <c r="A65" s="22" t="s">
+        <v>309</v>
       </c>
       <c r="B65" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="58">
-      <c r="A66" s="23" t="s">
-        <v>315</v>
+      <c r="A66" s="22" t="s">
+        <v>311</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="15" t="s">
+      <c r="A67" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="B67" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="B68" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="14" t="s">
         <v>334</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B69" t="s">
         <v>335</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="15" t="s">
-        <v>336</v>
-      </c>
-      <c r="B68" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="15" t="s">
-        <v>338</v>
-      </c>
-      <c r="B69" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B70" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B71" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B72" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="25" t="s">
-        <v>353</v>
+      <c r="A73" t="s">
+        <v>349</v>
       </c>
       <c r="B73" t="s">
-        <v>354</v>
+        <v>542</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="B75">
         <v>2</v>
@@ -3014,12 +3014,12 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="16" t="s">
-        <v>358</v>
+      <c r="A77" s="15" t="s">
+        <v>353</v>
       </c>
       <c r="B77" t="b">
         <v>1</v>
@@ -3027,7 +3027,7 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="B78">
         <v>10</v>
@@ -3035,7 +3035,7 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="B79">
         <f ca="1">YEAR(TODAY())</f>
@@ -3044,7 +3044,7 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="C80" t="str">
         <f ca="1">TEXT(MONTH(NOW()),"mmmm")</f>
@@ -3053,29 +3053,29 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="C81" t="str">
         <f ca="1">TEXT(NOW(),"mm-dd hhmm")</f>
-        <v>01-18 2235</v>
+        <v>02-06 2312</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="B82" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="B84">
         <v>90</v>
@@ -3083,30 +3083,30 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="B85" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="B86" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="B87" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="20"/>
+  <phoneticPr fontId="21"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3116,7 +3116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -3173,7 +3173,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="29">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -4270,7 +4270,7 @@
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="20"/>
+  <phoneticPr fontId="21"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4279,8 +4279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -4296,7 +4296,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>27</v>
@@ -4332,21 +4332,24 @@
         <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="C2" t="s">
-        <v>500</v>
+        <v>541</v>
+      </c>
+      <c r="D2" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="B3" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="C3" t="s">
-        <v>500</v>
+        <v>541</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -4354,10 +4357,10 @@
         <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="C4" t="s">
-        <v>500</v>
+        <v>541</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -4365,10 +4368,10 @@
         <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="C5" t="s">
-        <v>500</v>
+        <v>541</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -4376,10 +4379,10 @@
         <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="C6" t="s">
-        <v>500</v>
+        <v>541</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -4387,168 +4390,168 @@
         <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="C7" t="s">
-        <v>500</v>
+        <v>541</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B8" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="C8" t="s">
-        <v>500</v>
+        <v>541</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B9" t="s">
+        <v>505</v>
+      </c>
+      <c r="C9" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="A10" s="21" t="s">
+        <v>522</v>
+      </c>
+      <c r="B10" t="s">
+        <v>525</v>
+      </c>
+      <c r="C10" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="A11" s="21" t="s">
+        <v>523</v>
+      </c>
+      <c r="B11" t="s">
+        <v>526</v>
+      </c>
+      <c r="C11" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
+      <c r="A12" s="21" t="s">
+        <v>317</v>
+      </c>
+      <c r="B12" t="s">
+        <v>506</v>
+      </c>
+      <c r="C12" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
+      <c r="A13" s="21" t="s">
+        <v>318</v>
+      </c>
+      <c r="B13" t="s">
+        <v>507</v>
+      </c>
+      <c r="C13" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="A14" s="21" t="s">
+        <v>322</v>
+      </c>
+      <c r="B14" t="s">
+        <v>508</v>
+      </c>
+      <c r="C14" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" s="21" t="s">
+        <v>323</v>
+      </c>
+      <c r="B15" t="s">
+        <v>509</v>
+      </c>
+      <c r="C15" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16" s="21" t="s">
+        <v>312</v>
+      </c>
+      <c r="B16" t="s">
+        <v>527</v>
+      </c>
+      <c r="C16" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="21" t="s">
+        <v>313</v>
+      </c>
+      <c r="B17" t="s">
+        <v>528</v>
+      </c>
+      <c r="C17" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="21" t="s">
+        <v>510</v>
+      </c>
+      <c r="B18" t="s">
         <v>511</v>
       </c>
-      <c r="C9" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26">
-      <c r="A10" s="23" t="s">
-        <v>528</v>
-      </c>
-      <c r="B10" t="s">
-        <v>531</v>
-      </c>
-      <c r="C10" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26">
-      <c r="A11" s="23" t="s">
-        <v>529</v>
-      </c>
-      <c r="B11" t="s">
-        <v>532</v>
-      </c>
-      <c r="C11" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26">
-      <c r="A12" s="23" t="s">
-        <v>321</v>
-      </c>
-      <c r="B12" t="s">
-        <v>512</v>
-      </c>
-      <c r="C12" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26">
-      <c r="A13" s="23" t="s">
-        <v>322</v>
-      </c>
-      <c r="B13" t="s">
-        <v>513</v>
-      </c>
-      <c r="C13" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26">
-      <c r="A14" s="23" t="s">
-        <v>326</v>
-      </c>
-      <c r="B14" t="s">
-        <v>514</v>
-      </c>
-      <c r="C14" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26">
-      <c r="A15" s="23" t="s">
-        <v>327</v>
-      </c>
-      <c r="B15" t="s">
-        <v>515</v>
-      </c>
-      <c r="C15" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26">
-      <c r="A16" s="23" t="s">
-        <v>316</v>
-      </c>
-      <c r="B16" t="s">
-        <v>533</v>
-      </c>
-      <c r="C16" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="23" t="s">
-        <v>317</v>
-      </c>
-      <c r="B17" t="s">
-        <v>534</v>
-      </c>
-      <c r="C17" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="23" t="s">
-        <v>516</v>
-      </c>
-      <c r="B18" t="s">
-        <v>517</v>
-      </c>
       <c r="C18" t="s">
-        <v>500</v>
+        <v>541</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B19" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="C19" t="s">
-        <v>500</v>
+        <v>541</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="23" t="s">
-        <v>380</v>
+      <c r="A20" s="21" t="s">
+        <v>375</v>
       </c>
       <c r="B20" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="C20" t="s">
-        <v>500</v>
+        <v>541</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="23" t="s">
-        <v>178</v>
+      <c r="A21" s="21" t="s">
+        <v>175</v>
       </c>
       <c r="B21" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="C21" t="s">
-        <v>500</v>
+        <v>541</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="20"/>
+  <phoneticPr fontId="21"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4557,8 +4560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D9DC59-3960-42CB-B3EC-EFF452A90D4F}">
   <dimension ref="A1:Z166"/>
   <sheetViews>
-    <sheetView topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="B144" sqref="B144"/>
+    <sheetView topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="A166" sqref="A166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4604,1322 +4607,1322 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="B4" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="B5" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B6" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B7" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B8" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B9" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B11" t="s">
         <v>146</v>
-      </c>
-      <c r="B11" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B12" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B13" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B14" t="s">
         <v>153</v>
-      </c>
-      <c r="B14" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B15" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:26">
       <c r="A16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B16" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" t="s">
         <v>147</v>
-      </c>
-      <c r="B17" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B18" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B19" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B20" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B21" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B22" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B23" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B24" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B25" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B26" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B27" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="B28" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B29" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B30" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B31" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B32" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B33" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B34" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B35" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
+        <v>192</v>
+      </c>
+      <c r="B36" t="s">
         <v>195</v>
-      </c>
-      <c r="B36" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
+        <v>193</v>
+      </c>
+      <c r="B37" t="s">
         <v>196</v>
-      </c>
-      <c r="B37" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B38" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B39" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B40" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B41" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="B42" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="B43" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="B44" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="B45" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="B46" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="B47" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B48" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B49" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B50" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B51" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
+        <v>212</v>
+      </c>
+      <c r="B52" t="s">
         <v>215</v>
-      </c>
-      <c r="B52" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B53" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B54" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B55" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B56" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B57" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="B58" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="B59" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="B60" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
+        <v>213</v>
+      </c>
+      <c r="B61" t="s">
         <v>216</v>
-      </c>
-      <c r="B61" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
+        <v>214</v>
+      </c>
+      <c r="B62" t="s">
         <v>217</v>
-      </c>
-      <c r="B62" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B63" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B64" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B65" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B66" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B67" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="B68" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
+        <v>238</v>
+      </c>
+      <c r="B69" t="s">
         <v>241</v>
-      </c>
-      <c r="B69" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B70" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B71" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
+        <v>242</v>
+      </c>
+      <c r="B72" t="s">
         <v>245</v>
-      </c>
-      <c r="B72" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
+        <v>243</v>
+      </c>
+      <c r="B73" t="s">
         <v>246</v>
-      </c>
-      <c r="B73" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B74" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B75" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B76" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B77" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="B78" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B79" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B80" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="B81" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B82" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B83" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="B84" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="B85" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B86" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B87" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="B88" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="B89" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="B90" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="B91" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
+        <v>278</v>
+      </c>
+      <c r="B92" t="s">
         <v>281</v>
-      </c>
-      <c r="B92" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B93" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B94" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="B95" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="B96" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="B97" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
+        <v>279</v>
+      </c>
+      <c r="B98" t="s">
         <v>282</v>
-      </c>
-      <c r="B98" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
+        <v>280</v>
+      </c>
+      <c r="B99" t="s">
         <v>283</v>
-      </c>
-      <c r="B99" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B100" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B101" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B102" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B103" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B104" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B105" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B106" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B107" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B108" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="B109" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B110" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B111" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B112" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B113" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B114" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B115" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B116" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B117" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B118" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B119" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B120" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="B121" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B122" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B123" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B124" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="B125" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="B126" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="B127" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="B128" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B129" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="B130" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="B131" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="B132" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="B133" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B134" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="B135" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="B136" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="B137" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="B138" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="B139" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="B140" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="B141" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="B142" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="B143" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="B144" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="B145" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="B146" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="B147" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" s="2" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="B150" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="B151" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B152" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="B153" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="B154" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="B155" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="B156" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B157" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="B158" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="B159" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="B160" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B161" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="B162" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="B163" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="B164" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B165" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B166" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change to an activity to go back to home.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55651C\Documents\GitHub\P0002_090_PayCyleAfternoon_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC84C911-E7FF-4AB6-B55B-1326FBD7DA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25F6495-5093-4618-998F-B3163A02B5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="545">
   <si>
     <t>Name</t>
   </si>
@@ -2305,8 +2305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -2402,6 +2402,9 @@
       <c r="B6" t="s">
         <v>540</v>
       </c>
+      <c r="C6" t="s">
+        <v>540</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="72.5">
       <c r="A7" t="s">
@@ -2617,7 +2620,7 @@
         <v>99</v>
       </c>
       <c r="B26">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -3054,7 +3057,7 @@
       </c>
       <c r="C81" t="str">
         <f ca="1">TEXT(NOW(),"mm-dd hhmm")</f>
-        <v>02-07 1802</v>
+        <v>02-13 2022</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -3075,7 +3078,7 @@
         <v>433</v>
       </c>
       <c r="B84">
-        <v>90</v>
+        <v>300</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -4276,8 +4279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -4557,8 +4560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D9DC59-3960-42CB-B3EC-EFF452A90D4F}">
   <dimension ref="A1:Z166"/>
   <sheetViews>
-    <sheetView topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="A166" sqref="A166"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
made changes to table data extraction , Approve button and Sharepoint folder link in email
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55651C\Documents\GitHub\P0002_090_PayCyleAfternoon_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25F6495-5093-4618-998F-B3163A02B5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3205D536-0EA1-43B7-BDD4-C2CB93F296F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="571">
   <si>
     <t>Name</t>
   </si>
@@ -99,11 +99,11 @@
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="21"/>
+    <phoneticPr fontId="23"/>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="21"/>
+    <phoneticPr fontId="23"/>
   </si>
   <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
@@ -394,9 +394,6 @@
     <t>SetTransactionStatusSuccess</t>
   </si>
   <si>
-    <t>Data added to the queue successfully.</t>
-  </si>
-  <si>
     <t>SetTransactionStatusBE</t>
   </si>
   <si>
@@ -488,9 +485,6 @@
   </si>
   <si>
     <t>NavigateButtonNotPresent</t>
-  </si>
-  <si>
-    <t>NavigateButtonNotPresentBE</t>
   </si>
   <si>
     <t>PaymentSelectionPresent</t>
@@ -1671,6 +1665,90 @@
   </si>
   <si>
     <t>outlook</t>
+  </si>
+  <si>
+    <t>Instance Number Records from the table could not be extracted for paycycle.</t>
+  </si>
+  <si>
+    <t>TableInstanceRecordsExtracted</t>
+  </si>
+  <si>
+    <t>TableInstanceRecordsNotExtracted</t>
+  </si>
+  <si>
+    <t>TableInstanceRecordsNotExtractedSE</t>
+  </si>
+  <si>
+    <t>Instance Number Records from the table were extracted for paycycle.</t>
+  </si>
+  <si>
+    <t>DelayApproveButton</t>
+  </si>
+  <si>
+    <t>00:00:05</t>
+  </si>
+  <si>
+    <t>ApproveButtonRetries</t>
+  </si>
+  <si>
+    <t>ApproveButtonAttribute</t>
+  </si>
+  <si>
+    <t>aastate</t>
+  </si>
+  <si>
+    <t>ApproveButtonDesiredState</t>
+  </si>
+  <si>
+    <t>DISABLED</t>
+  </si>
+  <si>
+    <t>There was an error as Approve button was not disabled.</t>
+  </si>
+  <si>
+    <t>ApproveButtonRetryScopeError</t>
+  </si>
+  <si>
+    <t>ApproveButtonDisabled</t>
+  </si>
+  <si>
+    <t>ApproveButtonNotDisabled</t>
+  </si>
+  <si>
+    <t>ApproveButtonNotDisabledSE</t>
+  </si>
+  <si>
+    <t>Approve button was disabled on page Pay cycle approval, click Pay cycle Manager</t>
+  </si>
+  <si>
+    <t>Approve button was not disabled on page Pay cycle approval</t>
+  </si>
+  <si>
+    <t>HomeButtonPresent</t>
+  </si>
+  <si>
+    <t>HomeButtonNotPresent</t>
+  </si>
+  <si>
+    <t>HomeButtonNotPresentSE</t>
+  </si>
+  <si>
+    <t>NavigateButtonNotPresentSE</t>
+  </si>
+  <si>
+    <t>Home Button was found on homepage.</t>
+  </si>
+  <si>
+    <t>The Home button was not found in Peoplesoft page.</t>
+  </si>
+  <si>
+    <t>SharepointShareDocuments</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SharepointPath</t>
+  </si>
+  <si>
+    <t>Success Mail will be sent now before process completion.</t>
   </si>
   <si>
     <t>PROD</t>
@@ -1683,11 +1761,25 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1911,51 +2003,53 @@
   </borders>
   <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="4" fontId="26" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="4" fontId="28" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="1"/>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="1"/>
@@ -2303,10 +2397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z87"/>
+  <dimension ref="A1:Z91"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -2356,7 +2450,7 @@
         <v>106</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -2367,7 +2461,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>29</v>
@@ -2378,7 +2472,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>21</v>
@@ -2397,13 +2491,13 @@
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B6" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C6" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="72.5">
@@ -2411,7 +2505,7 @@
         <v>48</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C7" t="s">
         <v>49</v>
@@ -2433,7 +2527,7 @@
         <v>53</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C9" t="s">
         <v>54</v>
@@ -2474,10 +2568,10 @@
     </row>
     <row r="13" spans="1:26">
       <c r="A13" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B13" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C13" t="s">
         <v>64</v>
@@ -2485,7 +2579,7 @@
     </row>
     <row r="14" spans="1:26">
       <c r="A14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B14" t="s">
         <v>66</v>
@@ -2521,7 +2615,7 @@
         <v>71</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>72</v>
@@ -2532,7 +2626,7 @@
         <v>73</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>74</v>
@@ -2543,7 +2637,7 @@
         <v>75</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>76</v>
@@ -2584,17 +2678,17 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="20" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B23">
         <v>10</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="25" t="s">
         <v>84</v>
       </c>
       <c r="B24" t="b">
@@ -2620,7 +2714,7 @@
         <v>99</v>
       </c>
       <c r="B26">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2649,15 +2743,15 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="10" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B31">
         <v>10</v>
@@ -2665,7 +2759,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -2673,7 +2767,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B33">
         <v>10</v>
@@ -2681,7 +2775,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="10" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B34">
         <v>90</v>
@@ -2689,39 +2783,39 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="13" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B35" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B36" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="13" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B37" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="13" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B38" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B39" t="b">
         <v>1</v>
@@ -2729,55 +2823,55 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B40" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="10" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B41" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B42" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="13" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B43" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="13" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B44" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B45" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="10" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B46">
         <v>15</v>
@@ -2785,7 +2879,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="20" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B47">
         <v>45</v>
@@ -2793,31 +2887,31 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B48" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="11" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B49" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B50" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B51" t="s">
         <v>59</v>
@@ -2825,7 +2919,7 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="11" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B52" t="s">
         <v>77</v>
@@ -2833,180 +2927,180 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="17" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B53" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B54" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="17" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B55" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="18" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B56" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="17" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B57" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="22" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B58" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="21" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B59" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="43.5">
       <c r="A60" s="21" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="21" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B61" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="29">
       <c r="A62" s="21" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="21" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B63" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="58">
       <c r="A64" s="21" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="22" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B65" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="58">
       <c r="A66" s="22" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="14" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B67" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="14" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B68" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="14" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B69" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B70" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B71" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B72" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B73" t="s">
-        <v>544</v>
+        <v>570</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B75">
         <v>2</v>
@@ -3014,12 +3108,12 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="15" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B77" t="b">
         <v>1</v>
@@ -3027,7 +3121,7 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B78">
         <v>10</v>
@@ -3035,7 +3129,7 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B79">
         <f ca="1">YEAR(TODAY())</f>
@@ -3044,7 +3138,7 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C80" t="str">
         <f ca="1">TEXT(MONTH(NOW()),"mmmm")</f>
@@ -3053,29 +3147,29 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C81" t="str">
         <f ca="1">TEXT(NOW(),"mm-dd hhmm")</f>
-        <v>02-13 2022</v>
+        <v>02-14 2142</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B82" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B84">
         <v>300</v>
@@ -3083,30 +3177,62 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B85" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B86" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B87" t="s">
-        <v>423</v>
+        <v>421</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="25" t="s">
+        <v>547</v>
+      </c>
+      <c r="B88" s="12" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="25" t="s">
+        <v>549</v>
+      </c>
+      <c r="B89">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>550</v>
+      </c>
+      <c r="B90" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>552</v>
+      </c>
+      <c r="B91" t="s">
+        <v>553</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="21"/>
+  <phoneticPr fontId="23"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4270,17 +4396,17 @@
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="21"/>
+  <phoneticPr fontId="23"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z21"/>
+  <dimension ref="A1:Z22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -4296,7 +4422,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>27</v>
@@ -4332,24 +4458,24 @@
         <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C2" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D2" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B3" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C3" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -4357,10 +4483,10 @@
         <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C4" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -4368,10 +4494,10 @@
         <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C5" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -4379,10 +4505,10 @@
         <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C6" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -4390,10 +4516,10 @@
         <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C7" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -4401,167 +4527,178 @@
         <v>101</v>
       </c>
       <c r="B8" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C8" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B9" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C9" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" s="21" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B10" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C10" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" s="21" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B11" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C11" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" s="21" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B12" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C12" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" s="21" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B13" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C13" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" s="21" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B14" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C14" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" s="21" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B15" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C15" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="16" spans="1:26">
       <c r="A16" s="21" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B16" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C16" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="21" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B17" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C17" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="21" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B18" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C18" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B19" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C19" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="21" t="s">
-        <v>375</v>
+      <c r="A20" s="26" t="s">
+        <v>373</v>
       </c>
       <c r="B20" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C20" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="21" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B21" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C21" t="s">
-        <v>540</v>
+        <v>538</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="26" t="s">
+        <v>567</v>
+      </c>
+      <c r="B22" t="s">
+        <v>568</v>
+      </c>
+      <c r="C22" t="s">
+        <v>538</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="21"/>
+  <phoneticPr fontId="23"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D9DC59-3960-42CB-B3EC-EFF452A90D4F}">
-  <dimension ref="A1:Z166"/>
+  <dimension ref="A1:Z176"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="B129" sqref="B129"/>
+    <sheetView topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="B115" sqref="B115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4623,42 +4760,42 @@
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
+        <v>510</v>
+      </c>
+      <c r="B4" t="s">
         <v>512</v>
-      </c>
-      <c r="B4" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
+        <v>511</v>
+      </c>
+      <c r="B5" t="s">
         <v>513</v>
-      </c>
-      <c r="B5" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B8" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -4679,1250 +4816,1330 @@
     </row>
     <row r="11" spans="1:26">
       <c r="A11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>561</v>
       </c>
       <c r="B12" t="s">
-        <v>154</v>
+        <v>565</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" t="s">
-        <v>149</v>
+        <v>562</v>
       </c>
       <c r="B13" t="s">
-        <v>153</v>
+        <v>566</v>
       </c>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" t="s">
-        <v>150</v>
+        <v>563</v>
       </c>
       <c r="B14" t="s">
-        <v>153</v>
+        <v>566</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B15" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:26">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B16" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>144</v>
+        <v>564</v>
       </c>
       <c r="B17" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B18" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B19" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="B20" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="B21" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B22" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B24" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B25" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="B26" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="B27" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>484</v>
+        <v>168</v>
       </c>
       <c r="B28" t="s">
-        <v>485</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B29" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B30" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>185</v>
+        <v>482</v>
       </c>
       <c r="B31" t="s">
-        <v>184</v>
+        <v>483</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B32" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="B33" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B34" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B35" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B36" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B37" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="B38" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="B39" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="B40" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>202</v>
+        <v>169</v>
       </c>
       <c r="B41" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>361</v>
+        <v>170</v>
       </c>
       <c r="B42" t="s">
-        <v>362</v>
+        <v>196</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>356</v>
+        <v>171</v>
       </c>
       <c r="B43" t="s">
-        <v>363</v>
+        <v>197</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>357</v>
+        <v>200</v>
       </c>
       <c r="B44" t="s">
-        <v>364</v>
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B45" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="B46" t="s">
-        <v>434</v>
+        <v>361</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="B47" t="s">
-        <v>434</v>
+        <v>362</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>208</v>
+        <v>356</v>
       </c>
       <c r="B48" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>209</v>
+        <v>357</v>
       </c>
       <c r="B49" t="s">
-        <v>366</v>
+        <v>432</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>203</v>
+        <v>358</v>
       </c>
       <c r="B50" t="s">
-        <v>210</v>
+        <v>432</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B51" t="s">
-        <v>211</v>
+        <v>364</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B52" t="s">
-        <v>215</v>
+        <v>364</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="B53" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="B54" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="B55" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B56" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B57" t="s">
-        <v>367</v>
+        <v>216</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>370</v>
+        <v>222</v>
       </c>
       <c r="B58" t="s">
-        <v>372</v>
+        <v>221</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>465</v>
+        <v>219</v>
       </c>
       <c r="B59" t="s">
-        <v>466</v>
+        <v>216</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>371</v>
+        <v>229</v>
       </c>
       <c r="B60" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>213</v>
+        <v>544</v>
       </c>
       <c r="B61" t="s">
-        <v>216</v>
+        <v>542</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>214</v>
+        <v>545</v>
       </c>
       <c r="B62" t="s">
-        <v>217</v>
+        <v>542</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>227</v>
+        <v>543</v>
       </c>
       <c r="B63" t="s">
-        <v>226</v>
+        <v>546</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>229</v>
+        <v>368</v>
       </c>
       <c r="B64" t="s">
-        <v>228</v>
+        <v>370</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>230</v>
+        <v>463</v>
       </c>
       <c r="B65" t="s">
-        <v>232</v>
+        <v>464</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>231</v>
+        <v>369</v>
       </c>
       <c r="B66" t="s">
-        <v>232</v>
+        <v>371</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
       <c r="B67" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>448</v>
+        <v>212</v>
       </c>
       <c r="B68" t="s">
-        <v>447</v>
+        <v>215</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="B69" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="B70" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="B71" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="B72" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="B73" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>244</v>
+        <v>446</v>
       </c>
       <c r="B74" t="s">
-        <v>246</v>
+        <v>445</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="B75" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="B76" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="B77" t="s">
-        <v>255</v>
+        <v>235</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>516</v>
+        <v>240</v>
       </c>
       <c r="B78" t="s">
-        <v>517</v>
+        <v>243</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="B79" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B80" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>475</v>
+        <v>248</v>
       </c>
       <c r="B81" t="s">
-        <v>488</v>
+        <v>249</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>263</v>
+        <v>555</v>
       </c>
       <c r="B82" t="s">
-        <v>262</v>
+        <v>554</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="B83" t="s">
-        <v>469</v>
+        <v>250</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>471</v>
+        <v>252</v>
       </c>
       <c r="B84" t="s">
-        <v>472</v>
+        <v>253</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>468</v>
+        <v>514</v>
       </c>
       <c r="B85" t="s">
-        <v>470</v>
+        <v>515</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>273</v>
+        <v>556</v>
       </c>
       <c r="B86" t="s">
-        <v>272</v>
+        <v>559</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>275</v>
+        <v>557</v>
       </c>
       <c r="B87" t="s">
-        <v>274</v>
+        <v>560</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>518</v>
+        <v>558</v>
       </c>
       <c r="B88" t="s">
-        <v>519</v>
+        <v>560</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>476</v>
+        <v>245</v>
       </c>
       <c r="B89" t="s">
-        <v>489</v>
+        <v>247</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>477</v>
+        <v>246</v>
       </c>
       <c r="B90" t="s">
-        <v>490</v>
+        <v>254</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="B91" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="B92" t="s">
-        <v>281</v>
+        <v>260</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>285</v>
+        <v>262</v>
       </c>
       <c r="B93" t="s">
-        <v>284</v>
+        <v>467</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>286</v>
+        <v>469</v>
       </c>
       <c r="B94" t="s">
-        <v>453</v>
+        <v>470</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>452</v>
+        <v>466</v>
       </c>
       <c r="B95" t="s">
-        <v>453</v>
+        <v>468</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>455</v>
+        <v>271</v>
       </c>
       <c r="B96" t="s">
-        <v>454</v>
+        <v>270</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>456</v>
+        <v>273</v>
       </c>
       <c r="B97" t="s">
-        <v>457</v>
+        <v>272</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>279</v>
+        <v>516</v>
       </c>
       <c r="B98" t="s">
-        <v>282</v>
+        <v>517</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>280</v>
+        <v>474</v>
       </c>
       <c r="B99" t="s">
-        <v>283</v>
+        <v>487</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>108</v>
+        <v>475</v>
       </c>
       <c r="B100" t="s">
-        <v>107</v>
+        <v>488</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>112</v>
+        <v>476</v>
       </c>
       <c r="B101" t="s">
-        <v>113</v>
+        <v>489</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>115</v>
+        <v>276</v>
       </c>
       <c r="B102" t="s">
-        <v>114</v>
+        <v>279</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>109</v>
+        <v>283</v>
       </c>
       <c r="B103" t="s">
-        <v>111</v>
+        <v>282</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>110</v>
+        <v>284</v>
       </c>
       <c r="B104" t="s">
-        <v>116</v>
+        <v>451</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>117</v>
+        <v>450</v>
       </c>
       <c r="B105" t="s">
-        <v>118</v>
+        <v>451</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>119</v>
+        <v>453</v>
       </c>
       <c r="B106" t="s">
-        <v>427</v>
+        <v>452</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>120</v>
+        <v>454</v>
       </c>
       <c r="B107" t="s">
-        <v>426</v>
+        <v>455</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>122</v>
+        <v>277</v>
       </c>
       <c r="B108" t="s">
-        <v>121</v>
+        <v>280</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>354</v>
+        <v>278</v>
       </c>
       <c r="B109" t="s">
-        <v>355</v>
+        <v>281</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="B111" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="B112" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B113" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="B114" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="B115" t="s">
-        <v>135</v>
+        <v>569</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="B116" t="s">
-        <v>135</v>
+        <v>425</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B117" t="s">
-        <v>288</v>
+        <v>424</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B118" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>125</v>
+        <v>352</v>
       </c>
       <c r="B119" t="s">
-        <v>138</v>
+        <v>353</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>324</v>
+        <v>125</v>
       </c>
       <c r="B120" t="s">
-        <v>325</v>
+        <v>126</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>428</v>
+        <v>127</v>
       </c>
       <c r="B121" t="s">
-        <v>430</v>
+        <v>126</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>429</v>
+        <v>128</v>
       </c>
       <c r="B122" t="s">
-        <v>431</v>
+        <v>129</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>326</v>
+        <v>130</v>
       </c>
       <c r="B123" t="s">
-        <v>327</v>
+        <v>131</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>328</v>
+        <v>132</v>
       </c>
       <c r="B124" t="s">
-        <v>329</v>
+        <v>133</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>378</v>
+        <v>135</v>
       </c>
       <c r="B125" t="s">
-        <v>385</v>
+        <v>134</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>381</v>
+        <v>136</v>
       </c>
       <c r="B126" t="s">
-        <v>389</v>
+        <v>134</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>382</v>
+        <v>122</v>
       </c>
       <c r="B127" t="s">
-        <v>388</v>
+        <v>286</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>383</v>
+        <v>123</v>
       </c>
       <c r="B128" t="s">
-        <v>392</v>
+        <v>138</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>384</v>
+        <v>124</v>
       </c>
       <c r="B129" t="s">
-        <v>391</v>
+        <v>137</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>390</v>
+        <v>322</v>
       </c>
       <c r="B130" t="s">
-        <v>391</v>
+        <v>323</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>379</v>
+        <v>426</v>
       </c>
       <c r="B131" t="s">
-        <v>386</v>
+        <v>428</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>380</v>
+        <v>427</v>
       </c>
       <c r="B132" t="s">
-        <v>387</v>
+        <v>429</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>393</v>
+        <v>324</v>
       </c>
       <c r="B133" t="s">
-        <v>394</v>
+        <v>325</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>399</v>
+        <v>326</v>
       </c>
       <c r="B134" t="s">
-        <v>389</v>
+        <v>327</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>400</v>
+        <v>376</v>
       </c>
       <c r="B135" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>401</v>
+        <v>379</v>
       </c>
       <c r="B136" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>397</v>
+        <v>380</v>
       </c>
       <c r="B137" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>398</v>
+        <v>381</v>
       </c>
       <c r="B138" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="B139" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>538</v>
+        <v>388</v>
       </c>
       <c r="B140" t="s">
-        <v>535</v>
+        <v>389</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>409</v>
+        <v>377</v>
       </c>
       <c r="B141" t="s">
-        <v>536</v>
+        <v>384</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>410</v>
+        <v>378</v>
       </c>
       <c r="B142" t="s">
-        <v>537</v>
+        <v>385</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>408</v>
+        <v>391</v>
       </c>
       <c r="B143" t="s">
-        <v>539</v>
+        <v>392</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>412</v>
+        <v>397</v>
       </c>
       <c r="B144" t="s">
-        <v>414</v>
+        <v>387</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>413</v>
+        <v>398</v>
       </c>
       <c r="B145" t="s">
-        <v>415</v>
+        <v>386</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>416</v>
+        <v>399</v>
       </c>
       <c r="B146" t="s">
-        <v>418</v>
+        <v>389</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>417</v>
+        <v>395</v>
       </c>
       <c r="B147" t="s">
-        <v>419</v>
+        <v>393</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>420</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>421</v>
+        <v>396</v>
+      </c>
+      <c r="B148" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="149" spans="1:2">
-      <c r="A149" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>451</v>
+      <c r="A149" t="s">
+        <v>400</v>
+      </c>
+      <c r="B149" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>403</v>
+        <v>536</v>
       </c>
       <c r="B150" t="s">
-        <v>406</v>
+        <v>533</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="B151" t="s">
-        <v>407</v>
+        <v>534</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>258</v>
+        <v>408</v>
       </c>
       <c r="B152" t="s">
-        <v>257</v>
+        <v>535</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>435</v>
+        <v>406</v>
       </c>
       <c r="B153" t="s">
-        <v>363</v>
+        <v>537</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>436</v>
+        <v>410</v>
       </c>
       <c r="B154" t="s">
-        <v>364</v>
+        <v>412</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>437</v>
+        <v>411</v>
       </c>
       <c r="B155" t="s">
-        <v>365</v>
+        <v>413</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>438</v>
+        <v>414</v>
       </c>
       <c r="B156" t="s">
-        <v>434</v>
+        <v>416</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>439</v>
+        <v>415</v>
       </c>
       <c r="B157" t="s">
-        <v>434</v>
+        <v>417</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>440</v>
-      </c>
-      <c r="B158" t="s">
-        <v>443</v>
+        <v>418</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="159" spans="1:2">
-      <c r="A159" t="s">
-        <v>441</v>
-      </c>
-      <c r="B159" t="s">
-        <v>444</v>
+      <c r="A159" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>442</v>
+        <v>401</v>
       </c>
       <c r="B160" t="s">
-        <v>444</v>
+        <v>404</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>270</v>
+        <v>402</v>
       </c>
       <c r="B161" t="s">
-        <v>487</v>
+        <v>405</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>479</v>
+        <v>256</v>
       </c>
       <c r="B162" t="s">
-        <v>482</v>
+        <v>255</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>480</v>
+        <v>433</v>
       </c>
       <c r="B163" t="s">
-        <v>483</v>
+        <v>361</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>481</v>
+        <v>434</v>
       </c>
       <c r="B164" t="s">
-        <v>483</v>
+        <v>362</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>259</v>
+        <v>435</v>
       </c>
       <c r="B165" t="s">
-        <v>276</v>
+        <v>363</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>260</v>
+        <v>436</v>
       </c>
       <c r="B166" t="s">
-        <v>277</v>
+        <v>432</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2">
+      <c r="A167" t="s">
+        <v>437</v>
+      </c>
+      <c r="B167" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2">
+      <c r="A168" t="s">
+        <v>438</v>
+      </c>
+      <c r="B168" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2">
+      <c r="A169" t="s">
+        <v>439</v>
+      </c>
+      <c r="B169" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2">
+      <c r="A170" t="s">
+        <v>440</v>
+      </c>
+      <c r="B170" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2">
+      <c r="A171" t="s">
+        <v>268</v>
+      </c>
+      <c r="B171" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2">
+      <c r="A172" t="s">
+        <v>477</v>
+      </c>
+      <c r="B172" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2">
+      <c r="A173" t="s">
+        <v>478</v>
+      </c>
+      <c r="B173" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2">
+      <c r="A174" t="s">
+        <v>479</v>
+      </c>
+      <c r="B174" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2">
+      <c r="A175" t="s">
+        <v>257</v>
+      </c>
+      <c r="B175" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2">
+      <c r="A176" t="s">
+        <v>258</v>
+      </c>
+      <c r="B176" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made changes to the Peoplesoft login as password expiry exception added, also added some log messages and made sharepoint folder structure change.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55651C\Documents\GitHub\P0002_090_PayCyleAfternoon_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3205D536-0EA1-43B7-BDD4-C2CB93F296F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F245808E-D470-4657-8470-030A17647071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="588">
   <si>
     <t>Name</t>
   </si>
@@ -99,11 +99,11 @@
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="23"/>
+    <phoneticPr fontId="24"/>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="23"/>
+    <phoneticPr fontId="24"/>
   </si>
   <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
@@ -1607,9 +1607,6 @@
     <t>BE_4CCEmailAddress</t>
   </si>
   <si>
-    <t>BE_4,SE_1,SE_2,SE_3</t>
-  </si>
-  <si>
     <t>P002_090_PayCycleAfternoon_BE_4RecipientEmailAddress</t>
   </si>
   <si>
@@ -1749,6 +1746,60 @@
   </si>
   <si>
     <t>Success Mail will be sent now before process completion.</t>
+  </si>
+  <si>
+    <t>TotalRecordsToBeApproved</t>
+  </si>
+  <si>
+    <t>Total Number of records to be approved for this paycycle :</t>
+  </si>
+  <si>
+    <t>ProcessPaycycleRun</t>
+  </si>
+  <si>
+    <t>The pay cycle being processed now is :</t>
+  </si>
+  <si>
+    <t>ProcessEnvironmentRootFolder</t>
+  </si>
+  <si>
+    <t>SE_5Subject</t>
+  </si>
+  <si>
+    <t>Peoplesoft Credentials Expired for Pay Cycle Afternoon Process</t>
+  </si>
+  <si>
+    <t>SE_5Body</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;PeopleSoft credentials expired for user ID &lt;Bot_user_ID&gt;. &lt;br&gt;&lt;br&gt;Automation support team: Please confirm that the login credentials are valid / updated prior to the next Bot run&lt;br&gt; &lt;br&gt; Thanks,&lt;br&gt;Automation Team               </t>
+  </si>
+  <si>
+    <t>BE_4,SE_1,SE_2,SE_3,SE_5</t>
+  </si>
+  <si>
+    <t>SE_5RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_5RecipientEmailAddress</t>
+  </si>
+  <si>
+    <t>SE_5CCEmailAddress</t>
+  </si>
+  <si>
+    <t>P002_090_PayCycleAfternoon_SE_5CCEmailAddress</t>
+  </si>
+  <si>
+    <t>PeoplesoftCredentialsExpiredSE</t>
+  </si>
+  <si>
+    <t>People Soft Credenatials expired.</t>
+  </si>
+  <si>
+    <t>PeoplesoftCredentialsExpiredSE_5</t>
+  </si>
+  <si>
+    <t>SE_5: People Soft Credenatials have expired.</t>
   </si>
   <si>
     <t>PROD</t>
@@ -1761,11 +1812,18 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2003,51 +2061,52 @@
   </borders>
   <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="4" fontId="28" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="4" fontId="29" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="1"/>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="1"/>
@@ -2397,10 +2456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z91"/>
+  <dimension ref="A1:Z93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -2460,8 +2519,9 @@
       <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B3" t="s">
-        <v>538</v>
+      <c r="B3" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>29</v>
@@ -2493,11 +2553,12 @@
       <c r="A6" t="s">
         <v>492</v>
       </c>
-      <c r="B6" t="s">
-        <v>538</v>
+      <c r="B6" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
       <c r="C6" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="72.5">
@@ -2615,7 +2676,7 @@
         <v>71</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>72</v>
@@ -2626,7 +2687,7 @@
         <v>73</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>74</v>
@@ -2637,7 +2698,7 @@
         <v>75</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>76</v>
@@ -2890,7 +2951,7 @@
         <v>287</v>
       </c>
       <c r="B48" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -2898,7 +2959,7 @@
         <v>288</v>
       </c>
       <c r="B49" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -2970,7 +3031,7 @@
         <v>306</v>
       </c>
       <c r="B58" t="s">
-        <v>522</v>
+        <v>578</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -3021,7 +3082,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:2">
       <c r="A65" s="22" t="s">
         <v>307</v>
       </c>
@@ -3029,7 +3090,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="58">
+    <row r="66" spans="1:2" ht="58">
       <c r="A66" s="22" t="s">
         <v>309</v>
       </c>
@@ -3037,202 +3098,219 @@
         <v>460</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="14" t="s">
+    <row r="67" spans="1:2">
+      <c r="A67" s="27" t="s">
+        <v>574</v>
+      </c>
+      <c r="B67" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="43.5">
+      <c r="A68" s="27" t="s">
+        <v>576</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="14" t="s">
         <v>328</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B69" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="14" t="s">
+    <row r="70" spans="1:2">
+      <c r="A70" s="14" t="s">
         <v>330</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B70" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="14" t="s">
+    <row r="71" spans="1:2">
+      <c r="A71" s="14" t="s">
         <v>332</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B71" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
-      <c r="A70" t="s">
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
         <v>334</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B72" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
-      <c r="A71" t="s">
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
         <v>336</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B73" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
-      <c r="A72" t="s">
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
         <v>338</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B74" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
-      <c r="A73" t="s">
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
         <v>347</v>
       </c>
-      <c r="B73" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" t="s">
+      <c r="B75" t="str">
+        <f>Constants!$B$18</f>
+        <v>PROD</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
-      <c r="A75" t="s">
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
         <v>349</v>
       </c>
-      <c r="B75">
+      <c r="B77">
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
-      <c r="A76" t="s">
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="15" t="s">
+    <row r="79" spans="1:2">
+      <c r="A79" s="15" t="s">
         <v>351</v>
       </c>
-      <c r="B77" t="b">
+      <c r="B79" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
-      <c r="A78" t="s">
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
         <v>366</v>
       </c>
-      <c r="B78">
+      <c r="B80">
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
-      <c r="A79" t="s">
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
         <v>374</v>
       </c>
-      <c r="B79">
+      <c r="B81">
         <f ca="1">YEAR(TODAY())</f>
         <v>2024</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
-      <c r="A80" t="s">
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
         <v>375</v>
       </c>
-      <c r="C80" t="str">
+      <c r="C82" t="str">
         <f ca="1">TEXT(MONTH(NOW()),"mmmm")</f>
         <v>January</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
-      <c r="A81" t="s">
-        <v>409</v>
-      </c>
-      <c r="C81" t="str">
-        <f ca="1">TEXT(NOW(),"mm-dd hhmm")</f>
-        <v>02-14 2142</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" t="s">
-        <v>420</v>
-      </c>
-      <c r="B82" t="s">
-        <v>421</v>
-      </c>
-    </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>423</v>
+        <v>409</v>
+      </c>
+      <c r="C83" t="str">
+        <f ca="1">TEXT(NOW(),"mm-dd hhmm")</f>
+        <v>02-26 2128</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>431</v>
-      </c>
-      <c r="B84">
-        <v>300</v>
+        <v>420</v>
+      </c>
+      <c r="B84" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>443</v>
-      </c>
-      <c r="B85" t="s">
-        <v>444</v>
+        <v>423</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>447</v>
-      </c>
-      <c r="B86" t="s">
-        <v>448</v>
+        <v>431</v>
+      </c>
+      <c r="B86">
+        <v>300</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
+        <v>443</v>
+      </c>
+      <c r="B87" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>447</v>
+      </c>
+      <c r="B88" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
         <v>456</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B89" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
-      <c r="A88" s="25" t="s">
+    <row r="90" spans="1:3">
+      <c r="A90" s="25" t="s">
+        <v>546</v>
+      </c>
+      <c r="B90" s="12" t="s">
         <v>547</v>
       </c>
-      <c r="B88" s="12" t="s">
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="25" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89" s="25" t="s">
+      <c r="B91">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
         <v>549</v>
       </c>
-      <c r="B89">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90" t="s">
+      <c r="B92" t="s">
         <v>550</v>
       </c>
-      <c r="B90" t="s">
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91" t="s">
+      <c r="B93" t="s">
         <v>552</v>
       </c>
-      <c r="B91" t="s">
-        <v>553</v>
-      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="23"/>
+  <phoneticPr fontId="24"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3240,13 +3318,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z988"/>
+  <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="33.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60.81640625" bestFit="1" customWidth="1"/>
@@ -3254,7 +3332,7 @@
     <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.25" customHeight="1">
+    <row r="1" spans="1:26" ht="18.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3310,8 +3388,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+    <row r="5" spans="1:26">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -3322,8 +3399,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+    <row r="7" spans="1:26">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -3334,7 +3410,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+    <row r="8" spans="1:26">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -3345,7 +3421,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+    <row r="9" spans="1:26">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -3356,7 +3432,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+    <row r="10" spans="1:26">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -3367,7 +3443,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+    <row r="11" spans="1:26">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -3378,7 +3454,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+    <row r="12" spans="1:26">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -3389,8 +3465,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+    <row r="14" spans="1:26">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -3401,7 +3476,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+    <row r="15" spans="1:26">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -3412,7 +3487,6 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>37</v>
@@ -3424,989 +3498,26 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
-    <row r="101" ht="14.25" customHeight="1"/>
-    <row r="102" ht="14.25" customHeight="1"/>
-    <row r="103" ht="14.25" customHeight="1"/>
-    <row r="104" ht="14.25" customHeight="1"/>
-    <row r="105" ht="14.25" customHeight="1"/>
-    <row r="106" ht="14.25" customHeight="1"/>
-    <row r="107" ht="14.25" customHeight="1"/>
-    <row r="108" ht="14.25" customHeight="1"/>
-    <row r="109" ht="14.25" customHeight="1"/>
-    <row r="110" ht="14.25" customHeight="1"/>
-    <row r="111" ht="14.25" customHeight="1"/>
-    <row r="112" ht="14.25" customHeight="1"/>
-    <row r="113" ht="14.25" customHeight="1"/>
-    <row r="114" ht="14.25" customHeight="1"/>
-    <row r="115" ht="14.25" customHeight="1"/>
-    <row r="116" ht="14.25" customHeight="1"/>
-    <row r="117" ht="14.25" customHeight="1"/>
-    <row r="118" ht="14.25" customHeight="1"/>
-    <row r="119" ht="14.25" customHeight="1"/>
-    <row r="120" ht="14.25" customHeight="1"/>
-    <row r="121" ht="14.25" customHeight="1"/>
-    <row r="122" ht="14.25" customHeight="1"/>
-    <row r="123" ht="14.25" customHeight="1"/>
-    <row r="124" ht="14.25" customHeight="1"/>
-    <row r="125" ht="14.25" customHeight="1"/>
-    <row r="126" ht="14.25" customHeight="1"/>
-    <row r="127" ht="14.25" customHeight="1"/>
-    <row r="128" ht="14.25" customHeight="1"/>
-    <row r="129" ht="14.25" customHeight="1"/>
-    <row r="130" ht="14.25" customHeight="1"/>
-    <row r="131" ht="14.25" customHeight="1"/>
-    <row r="132" ht="14.25" customHeight="1"/>
-    <row r="133" ht="14.25" customHeight="1"/>
-    <row r="134" ht="14.25" customHeight="1"/>
-    <row r="135" ht="14.25" customHeight="1"/>
-    <row r="136" ht="14.25" customHeight="1"/>
-    <row r="137" ht="14.25" customHeight="1"/>
-    <row r="138" ht="14.25" customHeight="1"/>
-    <row r="139" ht="14.25" customHeight="1"/>
-    <row r="140" ht="14.25" customHeight="1"/>
-    <row r="141" ht="14.25" customHeight="1"/>
-    <row r="142" ht="14.25" customHeight="1"/>
-    <row r="143" ht="14.25" customHeight="1"/>
-    <row r="144" ht="14.25" customHeight="1"/>
-    <row r="145" ht="14.25" customHeight="1"/>
-    <row r="146" ht="14.25" customHeight="1"/>
-    <row r="147" ht="14.25" customHeight="1"/>
-    <row r="148" ht="14.25" customHeight="1"/>
-    <row r="149" ht="14.25" customHeight="1"/>
-    <row r="150" ht="14.25" customHeight="1"/>
-    <row r="151" ht="14.25" customHeight="1"/>
-    <row r="152" ht="14.25" customHeight="1"/>
-    <row r="153" ht="14.25" customHeight="1"/>
-    <row r="154" ht="14.25" customHeight="1"/>
-    <row r="155" ht="14.25" customHeight="1"/>
-    <row r="156" ht="14.25" customHeight="1"/>
-    <row r="157" ht="14.25" customHeight="1"/>
-    <row r="158" ht="14.25" customHeight="1"/>
-    <row r="159" ht="14.25" customHeight="1"/>
-    <row r="160" ht="14.25" customHeight="1"/>
-    <row r="161" ht="14.25" customHeight="1"/>
-    <row r="162" ht="14.25" customHeight="1"/>
-    <row r="163" ht="14.25" customHeight="1"/>
-    <row r="164" ht="14.25" customHeight="1"/>
-    <row r="165" ht="14.25" customHeight="1"/>
-    <row r="166" ht="14.25" customHeight="1"/>
-    <row r="167" ht="14.25" customHeight="1"/>
-    <row r="168" ht="14.25" customHeight="1"/>
-    <row r="169" ht="14.25" customHeight="1"/>
-    <row r="170" ht="14.25" customHeight="1"/>
-    <row r="171" ht="14.25" customHeight="1"/>
-    <row r="172" ht="14.25" customHeight="1"/>
-    <row r="173" ht="14.25" customHeight="1"/>
-    <row r="174" ht="14.25" customHeight="1"/>
-    <row r="175" ht="14.25" customHeight="1"/>
-    <row r="176" ht="14.25" customHeight="1"/>
-    <row r="177" ht="14.25" customHeight="1"/>
-    <row r="178" ht="14.25" customHeight="1"/>
-    <row r="179" ht="14.25" customHeight="1"/>
-    <row r="180" ht="14.25" customHeight="1"/>
-    <row r="181" ht="14.25" customHeight="1"/>
-    <row r="182" ht="14.25" customHeight="1"/>
-    <row r="183" ht="14.25" customHeight="1"/>
-    <row r="184" ht="14.25" customHeight="1"/>
-    <row r="185" ht="14.25" customHeight="1"/>
-    <row r="186" ht="14.25" customHeight="1"/>
-    <row r="187" ht="14.25" customHeight="1"/>
-    <row r="188" ht="14.25" customHeight="1"/>
-    <row r="189" ht="14.25" customHeight="1"/>
-    <row r="190" ht="14.25" customHeight="1"/>
-    <row r="191" ht="14.25" customHeight="1"/>
-    <row r="192" ht="14.25" customHeight="1"/>
-    <row r="193" ht="14.25" customHeight="1"/>
-    <row r="194" ht="14.25" customHeight="1"/>
-    <row r="195" ht="14.25" customHeight="1"/>
-    <row r="196" ht="14.25" customHeight="1"/>
-    <row r="197" ht="14.25" customHeight="1"/>
-    <row r="198" ht="14.25" customHeight="1"/>
-    <row r="199" ht="14.25" customHeight="1"/>
-    <row r="200" ht="14.25" customHeight="1"/>
-    <row r="201" ht="14.25" customHeight="1"/>
-    <row r="202" ht="14.25" customHeight="1"/>
-    <row r="203" ht="14.25" customHeight="1"/>
-    <row r="204" ht="14.25" customHeight="1"/>
-    <row r="205" ht="14.25" customHeight="1"/>
-    <row r="206" ht="14.25" customHeight="1"/>
-    <row r="207" ht="14.25" customHeight="1"/>
-    <row r="208" ht="14.25" customHeight="1"/>
-    <row r="209" ht="14.25" customHeight="1"/>
-    <row r="210" ht="14.25" customHeight="1"/>
-    <row r="211" ht="14.25" customHeight="1"/>
-    <row r="212" ht="14.25" customHeight="1"/>
-    <row r="213" ht="14.25" customHeight="1"/>
-    <row r="214" ht="14.25" customHeight="1"/>
-    <row r="215" ht="14.25" customHeight="1"/>
-    <row r="216" ht="14.25" customHeight="1"/>
-    <row r="217" ht="14.25" customHeight="1"/>
-    <row r="218" ht="14.25" customHeight="1"/>
-    <row r="219" ht="14.25" customHeight="1"/>
-    <row r="220" ht="14.25" customHeight="1"/>
-    <row r="221" ht="14.25" customHeight="1"/>
-    <row r="222" ht="14.25" customHeight="1"/>
-    <row r="223" ht="14.25" customHeight="1"/>
-    <row r="224" ht="14.25" customHeight="1"/>
-    <row r="225" ht="14.25" customHeight="1"/>
-    <row r="226" ht="14.25" customHeight="1"/>
-    <row r="227" ht="14.25" customHeight="1"/>
-    <row r="228" ht="14.25" customHeight="1"/>
-    <row r="229" ht="14.25" customHeight="1"/>
-    <row r="230" ht="14.25" customHeight="1"/>
-    <row r="231" ht="14.25" customHeight="1"/>
-    <row r="232" ht="14.25" customHeight="1"/>
-    <row r="233" ht="14.25" customHeight="1"/>
-    <row r="234" ht="14.25" customHeight="1"/>
-    <row r="235" ht="14.25" customHeight="1"/>
-    <row r="236" ht="14.25" customHeight="1"/>
-    <row r="237" ht="14.25" customHeight="1"/>
-    <row r="238" ht="14.25" customHeight="1"/>
-    <row r="239" ht="14.25" customHeight="1"/>
-    <row r="240" ht="14.25" customHeight="1"/>
-    <row r="241" ht="14.25" customHeight="1"/>
-    <row r="242" ht="14.25" customHeight="1"/>
-    <row r="243" ht="14.25" customHeight="1"/>
-    <row r="244" ht="14.25" customHeight="1"/>
-    <row r="245" ht="14.25" customHeight="1"/>
-    <row r="246" ht="14.25" customHeight="1"/>
-    <row r="247" ht="14.25" customHeight="1"/>
-    <row r="248" ht="14.25" customHeight="1"/>
-    <row r="249" ht="14.25" customHeight="1"/>
-    <row r="250" ht="14.25" customHeight="1"/>
-    <row r="251" ht="14.25" customHeight="1"/>
-    <row r="252" ht="14.25" customHeight="1"/>
-    <row r="253" ht="14.25" customHeight="1"/>
-    <row r="254" ht="14.25" customHeight="1"/>
-    <row r="255" ht="14.25" customHeight="1"/>
-    <row r="256" ht="14.25" customHeight="1"/>
-    <row r="257" ht="14.25" customHeight="1"/>
-    <row r="258" ht="14.25" customHeight="1"/>
-    <row r="259" ht="14.25" customHeight="1"/>
-    <row r="260" ht="14.25" customHeight="1"/>
-    <row r="261" ht="14.25" customHeight="1"/>
-    <row r="262" ht="14.25" customHeight="1"/>
-    <row r="263" ht="14.25" customHeight="1"/>
-    <row r="264" ht="14.25" customHeight="1"/>
-    <row r="265" ht="14.25" customHeight="1"/>
-    <row r="266" ht="14.25" customHeight="1"/>
-    <row r="267" ht="14.25" customHeight="1"/>
-    <row r="268" ht="14.25" customHeight="1"/>
-    <row r="269" ht="14.25" customHeight="1"/>
-    <row r="270" ht="14.25" customHeight="1"/>
-    <row r="271" ht="14.25" customHeight="1"/>
-    <row r="272" ht="14.25" customHeight="1"/>
-    <row r="273" ht="14.25" customHeight="1"/>
-    <row r="274" ht="14.25" customHeight="1"/>
-    <row r="275" ht="14.25" customHeight="1"/>
-    <row r="276" ht="14.25" customHeight="1"/>
-    <row r="277" ht="14.25" customHeight="1"/>
-    <row r="278" ht="14.25" customHeight="1"/>
-    <row r="279" ht="14.25" customHeight="1"/>
-    <row r="280" ht="14.25" customHeight="1"/>
-    <row r="281" ht="14.25" customHeight="1"/>
-    <row r="282" ht="14.25" customHeight="1"/>
-    <row r="283" ht="14.25" customHeight="1"/>
-    <row r="284" ht="14.25" customHeight="1"/>
-    <row r="285" ht="14.25" customHeight="1"/>
-    <row r="286" ht="14.25" customHeight="1"/>
-    <row r="287" ht="14.25" customHeight="1"/>
-    <row r="288" ht="14.25" customHeight="1"/>
-    <row r="289" ht="14.25" customHeight="1"/>
-    <row r="290" ht="14.25" customHeight="1"/>
-    <row r="291" ht="14.25" customHeight="1"/>
-    <row r="292" ht="14.25" customHeight="1"/>
-    <row r="293" ht="14.25" customHeight="1"/>
-    <row r="294" ht="14.25" customHeight="1"/>
-    <row r="295" ht="14.25" customHeight="1"/>
-    <row r="296" ht="14.25" customHeight="1"/>
-    <row r="297" ht="14.25" customHeight="1"/>
-    <row r="298" ht="14.25" customHeight="1"/>
-    <row r="299" ht="14.25" customHeight="1"/>
-    <row r="300" ht="14.25" customHeight="1"/>
-    <row r="301" ht="14.25" customHeight="1"/>
-    <row r="302" ht="14.25" customHeight="1"/>
-    <row r="303" ht="14.25" customHeight="1"/>
-    <row r="304" ht="14.25" customHeight="1"/>
-    <row r="305" ht="14.25" customHeight="1"/>
-    <row r="306" ht="14.25" customHeight="1"/>
-    <row r="307" ht="14.25" customHeight="1"/>
-    <row r="308" ht="14.25" customHeight="1"/>
-    <row r="309" ht="14.25" customHeight="1"/>
-    <row r="310" ht="14.25" customHeight="1"/>
-    <row r="311" ht="14.25" customHeight="1"/>
-    <row r="312" ht="14.25" customHeight="1"/>
-    <row r="313" ht="14.25" customHeight="1"/>
-    <row r="314" ht="14.25" customHeight="1"/>
-    <row r="315" ht="14.25" customHeight="1"/>
-    <row r="316" ht="14.25" customHeight="1"/>
-    <row r="317" ht="14.25" customHeight="1"/>
-    <row r="318" ht="14.25" customHeight="1"/>
-    <row r="319" ht="14.25" customHeight="1"/>
-    <row r="320" ht="14.25" customHeight="1"/>
-    <row r="321" ht="14.25" customHeight="1"/>
-    <row r="322" ht="14.25" customHeight="1"/>
-    <row r="323" ht="14.25" customHeight="1"/>
-    <row r="324" ht="14.25" customHeight="1"/>
-    <row r="325" ht="14.25" customHeight="1"/>
-    <row r="326" ht="14.25" customHeight="1"/>
-    <row r="327" ht="14.25" customHeight="1"/>
-    <row r="328" ht="14.25" customHeight="1"/>
-    <row r="329" ht="14.25" customHeight="1"/>
-    <row r="330" ht="14.25" customHeight="1"/>
-    <row r="331" ht="14.25" customHeight="1"/>
-    <row r="332" ht="14.25" customHeight="1"/>
-    <row r="333" ht="14.25" customHeight="1"/>
-    <row r="334" ht="14.25" customHeight="1"/>
-    <row r="335" ht="14.25" customHeight="1"/>
-    <row r="336" ht="14.25" customHeight="1"/>
-    <row r="337" ht="14.25" customHeight="1"/>
-    <row r="338" ht="14.25" customHeight="1"/>
-    <row r="339" ht="14.25" customHeight="1"/>
-    <row r="340" ht="14.25" customHeight="1"/>
-    <row r="341" ht="14.25" customHeight="1"/>
-    <row r="342" ht="14.25" customHeight="1"/>
-    <row r="343" ht="14.25" customHeight="1"/>
-    <row r="344" ht="14.25" customHeight="1"/>
-    <row r="345" ht="14.25" customHeight="1"/>
-    <row r="346" ht="14.25" customHeight="1"/>
-    <row r="347" ht="14.25" customHeight="1"/>
-    <row r="348" ht="14.25" customHeight="1"/>
-    <row r="349" ht="14.25" customHeight="1"/>
-    <row r="350" ht="14.25" customHeight="1"/>
-    <row r="351" ht="14.25" customHeight="1"/>
-    <row r="352" ht="14.25" customHeight="1"/>
-    <row r="353" ht="14.25" customHeight="1"/>
-    <row r="354" ht="14.25" customHeight="1"/>
-    <row r="355" ht="14.25" customHeight="1"/>
-    <row r="356" ht="14.25" customHeight="1"/>
-    <row r="357" ht="14.25" customHeight="1"/>
-    <row r="358" ht="14.25" customHeight="1"/>
-    <row r="359" ht="14.25" customHeight="1"/>
-    <row r="360" ht="14.25" customHeight="1"/>
-    <row r="361" ht="14.25" customHeight="1"/>
-    <row r="362" ht="14.25" customHeight="1"/>
-    <row r="363" ht="14.25" customHeight="1"/>
-    <row r="364" ht="14.25" customHeight="1"/>
-    <row r="365" ht="14.25" customHeight="1"/>
-    <row r="366" ht="14.25" customHeight="1"/>
-    <row r="367" ht="14.25" customHeight="1"/>
-    <row r="368" ht="14.25" customHeight="1"/>
-    <row r="369" ht="14.25" customHeight="1"/>
-    <row r="370" ht="14.25" customHeight="1"/>
-    <row r="371" ht="14.25" customHeight="1"/>
-    <row r="372" ht="14.25" customHeight="1"/>
-    <row r="373" ht="14.25" customHeight="1"/>
-    <row r="374" ht="14.25" customHeight="1"/>
-    <row r="375" ht="14.25" customHeight="1"/>
-    <row r="376" ht="14.25" customHeight="1"/>
-    <row r="377" ht="14.25" customHeight="1"/>
-    <row r="378" ht="14.25" customHeight="1"/>
-    <row r="379" ht="14.25" customHeight="1"/>
-    <row r="380" ht="14.25" customHeight="1"/>
-    <row r="381" ht="14.25" customHeight="1"/>
-    <row r="382" ht="14.25" customHeight="1"/>
-    <row r="383" ht="14.25" customHeight="1"/>
-    <row r="384" ht="14.25" customHeight="1"/>
-    <row r="385" ht="14.25" customHeight="1"/>
-    <row r="386" ht="14.25" customHeight="1"/>
-    <row r="387" ht="14.25" customHeight="1"/>
-    <row r="388" ht="14.25" customHeight="1"/>
-    <row r="389" ht="14.25" customHeight="1"/>
-    <row r="390" ht="14.25" customHeight="1"/>
-    <row r="391" ht="14.25" customHeight="1"/>
-    <row r="392" ht="14.25" customHeight="1"/>
-    <row r="393" ht="14.25" customHeight="1"/>
-    <row r="394" ht="14.25" customHeight="1"/>
-    <row r="395" ht="14.25" customHeight="1"/>
-    <row r="396" ht="14.25" customHeight="1"/>
-    <row r="397" ht="14.25" customHeight="1"/>
-    <row r="398" ht="14.25" customHeight="1"/>
-    <row r="399" ht="14.25" customHeight="1"/>
-    <row r="400" ht="14.25" customHeight="1"/>
-    <row r="401" ht="14.25" customHeight="1"/>
-    <row r="402" ht="14.25" customHeight="1"/>
-    <row r="403" ht="14.25" customHeight="1"/>
-    <row r="404" ht="14.25" customHeight="1"/>
-    <row r="405" ht="14.25" customHeight="1"/>
-    <row r="406" ht="14.25" customHeight="1"/>
-    <row r="407" ht="14.25" customHeight="1"/>
-    <row r="408" ht="14.25" customHeight="1"/>
-    <row r="409" ht="14.25" customHeight="1"/>
-    <row r="410" ht="14.25" customHeight="1"/>
-    <row r="411" ht="14.25" customHeight="1"/>
-    <row r="412" ht="14.25" customHeight="1"/>
-    <row r="413" ht="14.25" customHeight="1"/>
-    <row r="414" ht="14.25" customHeight="1"/>
-    <row r="415" ht="14.25" customHeight="1"/>
-    <row r="416" ht="14.25" customHeight="1"/>
-    <row r="417" ht="14.25" customHeight="1"/>
-    <row r="418" ht="14.25" customHeight="1"/>
-    <row r="419" ht="14.25" customHeight="1"/>
-    <row r="420" ht="14.25" customHeight="1"/>
-    <row r="421" ht="14.25" customHeight="1"/>
-    <row r="422" ht="14.25" customHeight="1"/>
-    <row r="423" ht="14.25" customHeight="1"/>
-    <row r="424" ht="14.25" customHeight="1"/>
-    <row r="425" ht="14.25" customHeight="1"/>
-    <row r="426" ht="14.25" customHeight="1"/>
-    <row r="427" ht="14.25" customHeight="1"/>
-    <row r="428" ht="14.25" customHeight="1"/>
-    <row r="429" ht="14.25" customHeight="1"/>
-    <row r="430" ht="14.25" customHeight="1"/>
-    <row r="431" ht="14.25" customHeight="1"/>
-    <row r="432" ht="14.25" customHeight="1"/>
-    <row r="433" ht="14.25" customHeight="1"/>
-    <row r="434" ht="14.25" customHeight="1"/>
-    <row r="435" ht="14.25" customHeight="1"/>
-    <row r="436" ht="14.25" customHeight="1"/>
-    <row r="437" ht="14.25" customHeight="1"/>
-    <row r="438" ht="14.25" customHeight="1"/>
-    <row r="439" ht="14.25" customHeight="1"/>
-    <row r="440" ht="14.25" customHeight="1"/>
-    <row r="441" ht="14.25" customHeight="1"/>
-    <row r="442" ht="14.25" customHeight="1"/>
-    <row r="443" ht="14.25" customHeight="1"/>
-    <row r="444" ht="14.25" customHeight="1"/>
-    <row r="445" ht="14.25" customHeight="1"/>
-    <row r="446" ht="14.25" customHeight="1"/>
-    <row r="447" ht="14.25" customHeight="1"/>
-    <row r="448" ht="14.25" customHeight="1"/>
-    <row r="449" ht="14.25" customHeight="1"/>
-    <row r="450" ht="14.25" customHeight="1"/>
-    <row r="451" ht="14.25" customHeight="1"/>
-    <row r="452" ht="14.25" customHeight="1"/>
-    <row r="453" ht="14.25" customHeight="1"/>
-    <row r="454" ht="14.25" customHeight="1"/>
-    <row r="455" ht="14.25" customHeight="1"/>
-    <row r="456" ht="14.25" customHeight="1"/>
-    <row r="457" ht="14.25" customHeight="1"/>
-    <row r="458" ht="14.25" customHeight="1"/>
-    <row r="459" ht="14.25" customHeight="1"/>
-    <row r="460" ht="14.25" customHeight="1"/>
-    <row r="461" ht="14.25" customHeight="1"/>
-    <row r="462" ht="14.25" customHeight="1"/>
-    <row r="463" ht="14.25" customHeight="1"/>
-    <row r="464" ht="14.25" customHeight="1"/>
-    <row r="465" ht="14.25" customHeight="1"/>
-    <row r="466" ht="14.25" customHeight="1"/>
-    <row r="467" ht="14.25" customHeight="1"/>
-    <row r="468" ht="14.25" customHeight="1"/>
-    <row r="469" ht="14.25" customHeight="1"/>
-    <row r="470" ht="14.25" customHeight="1"/>
-    <row r="471" ht="14.25" customHeight="1"/>
-    <row r="472" ht="14.25" customHeight="1"/>
-    <row r="473" ht="14.25" customHeight="1"/>
-    <row r="474" ht="14.25" customHeight="1"/>
-    <row r="475" ht="14.25" customHeight="1"/>
-    <row r="476" ht="14.25" customHeight="1"/>
-    <row r="477" ht="14.25" customHeight="1"/>
-    <row r="478" ht="14.25" customHeight="1"/>
-    <row r="479" ht="14.25" customHeight="1"/>
-    <row r="480" ht="14.25" customHeight="1"/>
-    <row r="481" ht="14.25" customHeight="1"/>
-    <row r="482" ht="14.25" customHeight="1"/>
-    <row r="483" ht="14.25" customHeight="1"/>
-    <row r="484" ht="14.25" customHeight="1"/>
-    <row r="485" ht="14.25" customHeight="1"/>
-    <row r="486" ht="14.25" customHeight="1"/>
-    <row r="487" ht="14.25" customHeight="1"/>
-    <row r="488" ht="14.25" customHeight="1"/>
-    <row r="489" ht="14.25" customHeight="1"/>
-    <row r="490" ht="14.25" customHeight="1"/>
-    <row r="491" ht="14.25" customHeight="1"/>
-    <row r="492" ht="14.25" customHeight="1"/>
-    <row r="493" ht="14.25" customHeight="1"/>
-    <row r="494" ht="14.25" customHeight="1"/>
-    <row r="495" ht="14.25" customHeight="1"/>
-    <row r="496" ht="14.25" customHeight="1"/>
-    <row r="497" ht="14.25" customHeight="1"/>
-    <row r="498" ht="14.25" customHeight="1"/>
-    <row r="499" ht="14.25" customHeight="1"/>
-    <row r="500" ht="14.25" customHeight="1"/>
-    <row r="501" ht="14.25" customHeight="1"/>
-    <row r="502" ht="14.25" customHeight="1"/>
-    <row r="503" ht="14.25" customHeight="1"/>
-    <row r="504" ht="14.25" customHeight="1"/>
-    <row r="505" ht="14.25" customHeight="1"/>
-    <row r="506" ht="14.25" customHeight="1"/>
-    <row r="507" ht="14.25" customHeight="1"/>
-    <row r="508" ht="14.25" customHeight="1"/>
-    <row r="509" ht="14.25" customHeight="1"/>
-    <row r="510" ht="14.25" customHeight="1"/>
-    <row r="511" ht="14.25" customHeight="1"/>
-    <row r="512" ht="14.25" customHeight="1"/>
-    <row r="513" ht="14.25" customHeight="1"/>
-    <row r="514" ht="14.25" customHeight="1"/>
-    <row r="515" ht="14.25" customHeight="1"/>
-    <row r="516" ht="14.25" customHeight="1"/>
-    <row r="517" ht="14.25" customHeight="1"/>
-    <row r="518" ht="14.25" customHeight="1"/>
-    <row r="519" ht="14.25" customHeight="1"/>
-    <row r="520" ht="14.25" customHeight="1"/>
-    <row r="521" ht="14.25" customHeight="1"/>
-    <row r="522" ht="14.25" customHeight="1"/>
-    <row r="523" ht="14.25" customHeight="1"/>
-    <row r="524" ht="14.25" customHeight="1"/>
-    <row r="525" ht="14.25" customHeight="1"/>
-    <row r="526" ht="14.25" customHeight="1"/>
-    <row r="527" ht="14.25" customHeight="1"/>
-    <row r="528" ht="14.25" customHeight="1"/>
-    <row r="529" ht="14.25" customHeight="1"/>
-    <row r="530" ht="14.25" customHeight="1"/>
-    <row r="531" ht="14.25" customHeight="1"/>
-    <row r="532" ht="14.25" customHeight="1"/>
-    <row r="533" ht="14.25" customHeight="1"/>
-    <row r="534" ht="14.25" customHeight="1"/>
-    <row r="535" ht="14.25" customHeight="1"/>
-    <row r="536" ht="14.25" customHeight="1"/>
-    <row r="537" ht="14.25" customHeight="1"/>
-    <row r="538" ht="14.25" customHeight="1"/>
-    <row r="539" ht="14.25" customHeight="1"/>
-    <row r="540" ht="14.25" customHeight="1"/>
-    <row r="541" ht="14.25" customHeight="1"/>
-    <row r="542" ht="14.25" customHeight="1"/>
-    <row r="543" ht="14.25" customHeight="1"/>
-    <row r="544" ht="14.25" customHeight="1"/>
-    <row r="545" ht="14.25" customHeight="1"/>
-    <row r="546" ht="14.25" customHeight="1"/>
-    <row r="547" ht="14.25" customHeight="1"/>
-    <row r="548" ht="14.25" customHeight="1"/>
-    <row r="549" ht="14.25" customHeight="1"/>
-    <row r="550" ht="14.25" customHeight="1"/>
-    <row r="551" ht="14.25" customHeight="1"/>
-    <row r="552" ht="14.25" customHeight="1"/>
-    <row r="553" ht="14.25" customHeight="1"/>
-    <row r="554" ht="14.25" customHeight="1"/>
-    <row r="555" ht="14.25" customHeight="1"/>
-    <row r="556" ht="14.25" customHeight="1"/>
-    <row r="557" ht="14.25" customHeight="1"/>
-    <row r="558" ht="14.25" customHeight="1"/>
-    <row r="559" ht="14.25" customHeight="1"/>
-    <row r="560" ht="14.25" customHeight="1"/>
-    <row r="561" ht="14.25" customHeight="1"/>
-    <row r="562" ht="14.25" customHeight="1"/>
-    <row r="563" ht="14.25" customHeight="1"/>
-    <row r="564" ht="14.25" customHeight="1"/>
-    <row r="565" ht="14.25" customHeight="1"/>
-    <row r="566" ht="14.25" customHeight="1"/>
-    <row r="567" ht="14.25" customHeight="1"/>
-    <row r="568" ht="14.25" customHeight="1"/>
-    <row r="569" ht="14.25" customHeight="1"/>
-    <row r="570" ht="14.25" customHeight="1"/>
-    <row r="571" ht="14.25" customHeight="1"/>
-    <row r="572" ht="14.25" customHeight="1"/>
-    <row r="573" ht="14.25" customHeight="1"/>
-    <row r="574" ht="14.25" customHeight="1"/>
-    <row r="575" ht="14.25" customHeight="1"/>
-    <row r="576" ht="14.25" customHeight="1"/>
-    <row r="577" ht="14.25" customHeight="1"/>
-    <row r="578" ht="14.25" customHeight="1"/>
-    <row r="579" ht="14.25" customHeight="1"/>
-    <row r="580" ht="14.25" customHeight="1"/>
-    <row r="581" ht="14.25" customHeight="1"/>
-    <row r="582" ht="14.25" customHeight="1"/>
-    <row r="583" ht="14.25" customHeight="1"/>
-    <row r="584" ht="14.25" customHeight="1"/>
-    <row r="585" ht="14.25" customHeight="1"/>
-    <row r="586" ht="14.25" customHeight="1"/>
-    <row r="587" ht="14.25" customHeight="1"/>
-    <row r="588" ht="14.25" customHeight="1"/>
-    <row r="589" ht="14.25" customHeight="1"/>
-    <row r="590" ht="14.25" customHeight="1"/>
-    <row r="591" ht="14.25" customHeight="1"/>
-    <row r="592" ht="14.25" customHeight="1"/>
-    <row r="593" ht="14.25" customHeight="1"/>
-    <row r="594" ht="14.25" customHeight="1"/>
-    <row r="595" ht="14.25" customHeight="1"/>
-    <row r="596" ht="14.25" customHeight="1"/>
-    <row r="597" ht="14.25" customHeight="1"/>
-    <row r="598" ht="14.25" customHeight="1"/>
-    <row r="599" ht="14.25" customHeight="1"/>
-    <row r="600" ht="14.25" customHeight="1"/>
-    <row r="601" ht="14.25" customHeight="1"/>
-    <row r="602" ht="14.25" customHeight="1"/>
-    <row r="603" ht="14.25" customHeight="1"/>
-    <row r="604" ht="14.25" customHeight="1"/>
-    <row r="605" ht="14.25" customHeight="1"/>
-    <row r="606" ht="14.25" customHeight="1"/>
-    <row r="607" ht="14.25" customHeight="1"/>
-    <row r="608" ht="14.25" customHeight="1"/>
-    <row r="609" ht="14.25" customHeight="1"/>
-    <row r="610" ht="14.25" customHeight="1"/>
-    <row r="611" ht="14.25" customHeight="1"/>
-    <row r="612" ht="14.25" customHeight="1"/>
-    <row r="613" ht="14.25" customHeight="1"/>
-    <row r="614" ht="14.25" customHeight="1"/>
-    <row r="615" ht="14.25" customHeight="1"/>
-    <row r="616" ht="14.25" customHeight="1"/>
-    <row r="617" ht="14.25" customHeight="1"/>
-    <row r="618" ht="14.25" customHeight="1"/>
-    <row r="619" ht="14.25" customHeight="1"/>
-    <row r="620" ht="14.25" customHeight="1"/>
-    <row r="621" ht="14.25" customHeight="1"/>
-    <row r="622" ht="14.25" customHeight="1"/>
-    <row r="623" ht="14.25" customHeight="1"/>
-    <row r="624" ht="14.25" customHeight="1"/>
-    <row r="625" ht="14.25" customHeight="1"/>
-    <row r="626" ht="14.25" customHeight="1"/>
-    <row r="627" ht="14.25" customHeight="1"/>
-    <row r="628" ht="14.25" customHeight="1"/>
-    <row r="629" ht="14.25" customHeight="1"/>
-    <row r="630" ht="14.25" customHeight="1"/>
-    <row r="631" ht="14.25" customHeight="1"/>
-    <row r="632" ht="14.25" customHeight="1"/>
-    <row r="633" ht="14.25" customHeight="1"/>
-    <row r="634" ht="14.25" customHeight="1"/>
-    <row r="635" ht="14.25" customHeight="1"/>
-    <row r="636" ht="14.25" customHeight="1"/>
-    <row r="637" ht="14.25" customHeight="1"/>
-    <row r="638" ht="14.25" customHeight="1"/>
-    <row r="639" ht="14.25" customHeight="1"/>
-    <row r="640" ht="14.25" customHeight="1"/>
-    <row r="641" ht="14.25" customHeight="1"/>
-    <row r="642" ht="14.25" customHeight="1"/>
-    <row r="643" ht="14.25" customHeight="1"/>
-    <row r="644" ht="14.25" customHeight="1"/>
-    <row r="645" ht="14.25" customHeight="1"/>
-    <row r="646" ht="14.25" customHeight="1"/>
-    <row r="647" ht="14.25" customHeight="1"/>
-    <row r="648" ht="14.25" customHeight="1"/>
-    <row r="649" ht="14.25" customHeight="1"/>
-    <row r="650" ht="14.25" customHeight="1"/>
-    <row r="651" ht="14.25" customHeight="1"/>
-    <row r="652" ht="14.25" customHeight="1"/>
-    <row r="653" ht="14.25" customHeight="1"/>
-    <row r="654" ht="14.25" customHeight="1"/>
-    <row r="655" ht="14.25" customHeight="1"/>
-    <row r="656" ht="14.25" customHeight="1"/>
-    <row r="657" ht="14.25" customHeight="1"/>
-    <row r="658" ht="14.25" customHeight="1"/>
-    <row r="659" ht="14.25" customHeight="1"/>
-    <row r="660" ht="14.25" customHeight="1"/>
-    <row r="661" ht="14.25" customHeight="1"/>
-    <row r="662" ht="14.25" customHeight="1"/>
-    <row r="663" ht="14.25" customHeight="1"/>
-    <row r="664" ht="14.25" customHeight="1"/>
-    <row r="665" ht="14.25" customHeight="1"/>
-    <row r="666" ht="14.25" customHeight="1"/>
-    <row r="667" ht="14.25" customHeight="1"/>
-    <row r="668" ht="14.25" customHeight="1"/>
-    <row r="669" ht="14.25" customHeight="1"/>
-    <row r="670" ht="14.25" customHeight="1"/>
-    <row r="671" ht="14.25" customHeight="1"/>
-    <row r="672" ht="14.25" customHeight="1"/>
-    <row r="673" ht="14.25" customHeight="1"/>
-    <row r="674" ht="14.25" customHeight="1"/>
-    <row r="675" ht="14.25" customHeight="1"/>
-    <row r="676" ht="14.25" customHeight="1"/>
-    <row r="677" ht="14.25" customHeight="1"/>
-    <row r="678" ht="14.25" customHeight="1"/>
-    <row r="679" ht="14.25" customHeight="1"/>
-    <row r="680" ht="14.25" customHeight="1"/>
-    <row r="681" ht="14.25" customHeight="1"/>
-    <row r="682" ht="14.25" customHeight="1"/>
-    <row r="683" ht="14.25" customHeight="1"/>
-    <row r="684" ht="14.25" customHeight="1"/>
-    <row r="685" ht="14.25" customHeight="1"/>
-    <row r="686" ht="14.25" customHeight="1"/>
-    <row r="687" ht="14.25" customHeight="1"/>
-    <row r="688" ht="14.25" customHeight="1"/>
-    <row r="689" ht="14.25" customHeight="1"/>
-    <row r="690" ht="14.25" customHeight="1"/>
-    <row r="691" ht="14.25" customHeight="1"/>
-    <row r="692" ht="14.25" customHeight="1"/>
-    <row r="693" ht="14.25" customHeight="1"/>
-    <row r="694" ht="14.25" customHeight="1"/>
-    <row r="695" ht="14.25" customHeight="1"/>
-    <row r="696" ht="14.25" customHeight="1"/>
-    <row r="697" ht="14.25" customHeight="1"/>
-    <row r="698" ht="14.25" customHeight="1"/>
-    <row r="699" ht="14.25" customHeight="1"/>
-    <row r="700" ht="14.25" customHeight="1"/>
-    <row r="701" ht="14.25" customHeight="1"/>
-    <row r="702" ht="14.25" customHeight="1"/>
-    <row r="703" ht="14.25" customHeight="1"/>
-    <row r="704" ht="14.25" customHeight="1"/>
-    <row r="705" ht="14.25" customHeight="1"/>
-    <row r="706" ht="14.25" customHeight="1"/>
-    <row r="707" ht="14.25" customHeight="1"/>
-    <row r="708" ht="14.25" customHeight="1"/>
-    <row r="709" ht="14.25" customHeight="1"/>
-    <row r="710" ht="14.25" customHeight="1"/>
-    <row r="711" ht="14.25" customHeight="1"/>
-    <row r="712" ht="14.25" customHeight="1"/>
-    <row r="713" ht="14.25" customHeight="1"/>
-    <row r="714" ht="14.25" customHeight="1"/>
-    <row r="715" ht="14.25" customHeight="1"/>
-    <row r="716" ht="14.25" customHeight="1"/>
-    <row r="717" ht="14.25" customHeight="1"/>
-    <row r="718" ht="14.25" customHeight="1"/>
-    <row r="719" ht="14.25" customHeight="1"/>
-    <row r="720" ht="14.25" customHeight="1"/>
-    <row r="721" ht="14.25" customHeight="1"/>
-    <row r="722" ht="14.25" customHeight="1"/>
-    <row r="723" ht="14.25" customHeight="1"/>
-    <row r="724" ht="14.25" customHeight="1"/>
-    <row r="725" ht="14.25" customHeight="1"/>
-    <row r="726" ht="14.25" customHeight="1"/>
-    <row r="727" ht="14.25" customHeight="1"/>
-    <row r="728" ht="14.25" customHeight="1"/>
-    <row r="729" ht="14.25" customHeight="1"/>
-    <row r="730" ht="14.25" customHeight="1"/>
-    <row r="731" ht="14.25" customHeight="1"/>
-    <row r="732" ht="14.25" customHeight="1"/>
-    <row r="733" ht="14.25" customHeight="1"/>
-    <row r="734" ht="14.25" customHeight="1"/>
-    <row r="735" ht="14.25" customHeight="1"/>
-    <row r="736" ht="14.25" customHeight="1"/>
-    <row r="737" ht="14.25" customHeight="1"/>
-    <row r="738" ht="14.25" customHeight="1"/>
-    <row r="739" ht="14.25" customHeight="1"/>
-    <row r="740" ht="14.25" customHeight="1"/>
-    <row r="741" ht="14.25" customHeight="1"/>
-    <row r="742" ht="14.25" customHeight="1"/>
-    <row r="743" ht="14.25" customHeight="1"/>
-    <row r="744" ht="14.25" customHeight="1"/>
-    <row r="745" ht="14.25" customHeight="1"/>
-    <row r="746" ht="14.25" customHeight="1"/>
-    <row r="747" ht="14.25" customHeight="1"/>
-    <row r="748" ht="14.25" customHeight="1"/>
-    <row r="749" ht="14.25" customHeight="1"/>
-    <row r="750" ht="14.25" customHeight="1"/>
-    <row r="751" ht="14.25" customHeight="1"/>
-    <row r="752" ht="14.25" customHeight="1"/>
-    <row r="753" ht="14.25" customHeight="1"/>
-    <row r="754" ht="14.25" customHeight="1"/>
-    <row r="755" ht="14.25" customHeight="1"/>
-    <row r="756" ht="14.25" customHeight="1"/>
-    <row r="757" ht="14.25" customHeight="1"/>
-    <row r="758" ht="14.25" customHeight="1"/>
-    <row r="759" ht="14.25" customHeight="1"/>
-    <row r="760" ht="14.25" customHeight="1"/>
-    <row r="761" ht="14.25" customHeight="1"/>
-    <row r="762" ht="14.25" customHeight="1"/>
-    <row r="763" ht="14.25" customHeight="1"/>
-    <row r="764" ht="14.25" customHeight="1"/>
-    <row r="765" ht="14.25" customHeight="1"/>
-    <row r="766" ht="14.25" customHeight="1"/>
-    <row r="767" ht="14.25" customHeight="1"/>
-    <row r="768" ht="14.25" customHeight="1"/>
-    <row r="769" ht="14.25" customHeight="1"/>
-    <row r="770" ht="14.25" customHeight="1"/>
-    <row r="771" ht="14.25" customHeight="1"/>
-    <row r="772" ht="14.25" customHeight="1"/>
-    <row r="773" ht="14.25" customHeight="1"/>
-    <row r="774" ht="14.25" customHeight="1"/>
-    <row r="775" ht="14.25" customHeight="1"/>
-    <row r="776" ht="14.25" customHeight="1"/>
-    <row r="777" ht="14.25" customHeight="1"/>
-    <row r="778" ht="14.25" customHeight="1"/>
-    <row r="779" ht="14.25" customHeight="1"/>
-    <row r="780" ht="14.25" customHeight="1"/>
-    <row r="781" ht="14.25" customHeight="1"/>
-    <row r="782" ht="14.25" customHeight="1"/>
-    <row r="783" ht="14.25" customHeight="1"/>
-    <row r="784" ht="14.25" customHeight="1"/>
-    <row r="785" ht="14.25" customHeight="1"/>
-    <row r="786" ht="14.25" customHeight="1"/>
-    <row r="787" ht="14.25" customHeight="1"/>
-    <row r="788" ht="14.25" customHeight="1"/>
-    <row r="789" ht="14.25" customHeight="1"/>
-    <row r="790" ht="14.25" customHeight="1"/>
-    <row r="791" ht="14.25" customHeight="1"/>
-    <row r="792" ht="14.25" customHeight="1"/>
-    <row r="793" ht="14.25" customHeight="1"/>
-    <row r="794" ht="14.25" customHeight="1"/>
-    <row r="795" ht="14.25" customHeight="1"/>
-    <row r="796" ht="14.25" customHeight="1"/>
-    <row r="797" ht="14.25" customHeight="1"/>
-    <row r="798" ht="14.25" customHeight="1"/>
-    <row r="799" ht="14.25" customHeight="1"/>
-    <row r="800" ht="14.25" customHeight="1"/>
-    <row r="801" ht="14.25" customHeight="1"/>
-    <row r="802" ht="14.25" customHeight="1"/>
-    <row r="803" ht="14.25" customHeight="1"/>
-    <row r="804" ht="14.25" customHeight="1"/>
-    <row r="805" ht="14.25" customHeight="1"/>
-    <row r="806" ht="14.25" customHeight="1"/>
-    <row r="807" ht="14.25" customHeight="1"/>
-    <row r="808" ht="14.25" customHeight="1"/>
-    <row r="809" ht="14.25" customHeight="1"/>
-    <row r="810" ht="14.25" customHeight="1"/>
-    <row r="811" ht="14.25" customHeight="1"/>
-    <row r="812" ht="14.25" customHeight="1"/>
-    <row r="813" ht="14.25" customHeight="1"/>
-    <row r="814" ht="14.25" customHeight="1"/>
-    <row r="815" ht="14.25" customHeight="1"/>
-    <row r="816" ht="14.25" customHeight="1"/>
-    <row r="817" ht="14.25" customHeight="1"/>
-    <row r="818" ht="14.25" customHeight="1"/>
-    <row r="819" ht="14.25" customHeight="1"/>
-    <row r="820" ht="14.25" customHeight="1"/>
-    <row r="821" ht="14.25" customHeight="1"/>
-    <row r="822" ht="14.25" customHeight="1"/>
-    <row r="823" ht="14.25" customHeight="1"/>
-    <row r="824" ht="14.25" customHeight="1"/>
-    <row r="825" ht="14.25" customHeight="1"/>
-    <row r="826" ht="14.25" customHeight="1"/>
-    <row r="827" ht="14.25" customHeight="1"/>
-    <row r="828" ht="14.25" customHeight="1"/>
-    <row r="829" ht="14.25" customHeight="1"/>
-    <row r="830" ht="14.25" customHeight="1"/>
-    <row r="831" ht="14.25" customHeight="1"/>
-    <row r="832" ht="14.25" customHeight="1"/>
-    <row r="833" ht="14.25" customHeight="1"/>
-    <row r="834" ht="14.25" customHeight="1"/>
-    <row r="835" ht="14.25" customHeight="1"/>
-    <row r="836" ht="14.25" customHeight="1"/>
-    <row r="837" ht="14.25" customHeight="1"/>
-    <row r="838" ht="14.25" customHeight="1"/>
-    <row r="839" ht="14.25" customHeight="1"/>
-    <row r="840" ht="14.25" customHeight="1"/>
-    <row r="841" ht="14.25" customHeight="1"/>
-    <row r="842" ht="14.25" customHeight="1"/>
-    <row r="843" ht="14.25" customHeight="1"/>
-    <row r="844" ht="14.25" customHeight="1"/>
-    <row r="845" ht="14.25" customHeight="1"/>
-    <row r="846" ht="14.25" customHeight="1"/>
-    <row r="847" ht="14.25" customHeight="1"/>
-    <row r="848" ht="14.25" customHeight="1"/>
-    <row r="849" ht="14.25" customHeight="1"/>
-    <row r="850" ht="14.25" customHeight="1"/>
-    <row r="851" ht="14.25" customHeight="1"/>
-    <row r="852" ht="14.25" customHeight="1"/>
-    <row r="853" ht="14.25" customHeight="1"/>
-    <row r="854" ht="14.25" customHeight="1"/>
-    <row r="855" ht="14.25" customHeight="1"/>
-    <row r="856" ht="14.25" customHeight="1"/>
-    <row r="857" ht="14.25" customHeight="1"/>
-    <row r="858" ht="14.25" customHeight="1"/>
-    <row r="859" ht="14.25" customHeight="1"/>
-    <row r="860" ht="14.25" customHeight="1"/>
-    <row r="861" ht="14.25" customHeight="1"/>
-    <row r="862" ht="14.25" customHeight="1"/>
-    <row r="863" ht="14.25" customHeight="1"/>
-    <row r="864" ht="14.25" customHeight="1"/>
-    <row r="865" ht="14.25" customHeight="1"/>
-    <row r="866" ht="14.25" customHeight="1"/>
-    <row r="867" ht="14.25" customHeight="1"/>
-    <row r="868" ht="14.25" customHeight="1"/>
-    <row r="869" ht="14.25" customHeight="1"/>
-    <row r="870" ht="14.25" customHeight="1"/>
-    <row r="871" ht="14.25" customHeight="1"/>
-    <row r="872" ht="14.25" customHeight="1"/>
-    <row r="873" ht="14.25" customHeight="1"/>
-    <row r="874" ht="14.25" customHeight="1"/>
-    <row r="875" ht="14.25" customHeight="1"/>
-    <row r="876" ht="14.25" customHeight="1"/>
-    <row r="877" ht="14.25" customHeight="1"/>
-    <row r="878" ht="14.25" customHeight="1"/>
-    <row r="879" ht="14.25" customHeight="1"/>
-    <row r="880" ht="14.25" customHeight="1"/>
-    <row r="881" ht="14.25" customHeight="1"/>
-    <row r="882" ht="14.25" customHeight="1"/>
-    <row r="883" ht="14.25" customHeight="1"/>
-    <row r="884" ht="14.25" customHeight="1"/>
-    <row r="885" ht="14.25" customHeight="1"/>
-    <row r="886" ht="14.25" customHeight="1"/>
-    <row r="887" ht="14.25" customHeight="1"/>
-    <row r="888" ht="14.25" customHeight="1"/>
-    <row r="889" ht="14.25" customHeight="1"/>
-    <row r="890" ht="14.25" customHeight="1"/>
-    <row r="891" ht="14.25" customHeight="1"/>
-    <row r="892" ht="14.25" customHeight="1"/>
-    <row r="893" ht="14.25" customHeight="1"/>
-    <row r="894" ht="14.25" customHeight="1"/>
-    <row r="895" ht="14.25" customHeight="1"/>
-    <row r="896" ht="14.25" customHeight="1"/>
-    <row r="897" ht="14.25" customHeight="1"/>
-    <row r="898" ht="14.25" customHeight="1"/>
-    <row r="899" ht="14.25" customHeight="1"/>
-    <row r="900" ht="14.25" customHeight="1"/>
-    <row r="901" ht="14.25" customHeight="1"/>
-    <row r="902" ht="14.25" customHeight="1"/>
-    <row r="903" ht="14.25" customHeight="1"/>
-    <row r="904" ht="14.25" customHeight="1"/>
-    <row r="905" ht="14.25" customHeight="1"/>
-    <row r="906" ht="14.25" customHeight="1"/>
-    <row r="907" ht="14.25" customHeight="1"/>
-    <row r="908" ht="14.25" customHeight="1"/>
-    <row r="909" ht="14.25" customHeight="1"/>
-    <row r="910" ht="14.25" customHeight="1"/>
-    <row r="911" ht="14.25" customHeight="1"/>
-    <row r="912" ht="14.25" customHeight="1"/>
-    <row r="913" ht="14.25" customHeight="1"/>
-    <row r="914" ht="14.25" customHeight="1"/>
-    <row r="915" ht="14.25" customHeight="1"/>
-    <row r="916" ht="14.25" customHeight="1"/>
-    <row r="917" ht="14.25" customHeight="1"/>
-    <row r="918" ht="14.25" customHeight="1"/>
-    <row r="919" ht="14.25" customHeight="1"/>
-    <row r="920" ht="14.25" customHeight="1"/>
-    <row r="921" ht="14.25" customHeight="1"/>
-    <row r="922" ht="14.25" customHeight="1"/>
-    <row r="923" ht="14.25" customHeight="1"/>
-    <row r="924" ht="14.25" customHeight="1"/>
-    <row r="925" ht="14.25" customHeight="1"/>
-    <row r="926" ht="14.25" customHeight="1"/>
-    <row r="927" ht="14.25" customHeight="1"/>
-    <row r="928" ht="14.25" customHeight="1"/>
-    <row r="929" ht="14.25" customHeight="1"/>
-    <row r="930" ht="14.25" customHeight="1"/>
-    <row r="931" ht="14.25" customHeight="1"/>
-    <row r="932" ht="14.25" customHeight="1"/>
-    <row r="933" ht="14.25" customHeight="1"/>
-    <row r="934" ht="14.25" customHeight="1"/>
-    <row r="935" ht="14.25" customHeight="1"/>
-    <row r="936" ht="14.25" customHeight="1"/>
-    <row r="937" ht="14.25" customHeight="1"/>
-    <row r="938" ht="14.25" customHeight="1"/>
-    <row r="939" ht="14.25" customHeight="1"/>
-    <row r="940" ht="14.25" customHeight="1"/>
-    <row r="941" ht="14.25" customHeight="1"/>
-    <row r="942" ht="14.25" customHeight="1"/>
-    <row r="943" ht="14.25" customHeight="1"/>
-    <row r="944" ht="14.25" customHeight="1"/>
-    <row r="945" ht="14.25" customHeight="1"/>
-    <row r="946" ht="14.25" customHeight="1"/>
-    <row r="947" ht="14.25" customHeight="1"/>
-    <row r="948" ht="14.25" customHeight="1"/>
-    <row r="949" ht="14.25" customHeight="1"/>
-    <row r="950" ht="14.25" customHeight="1"/>
-    <row r="951" ht="14.25" customHeight="1"/>
-    <row r="952" ht="14.25" customHeight="1"/>
-    <row r="953" ht="14.25" customHeight="1"/>
-    <row r="954" ht="14.25" customHeight="1"/>
-    <row r="955" ht="14.25" customHeight="1"/>
-    <row r="956" ht="14.25" customHeight="1"/>
-    <row r="957" ht="14.25" customHeight="1"/>
-    <row r="958" ht="14.25" customHeight="1"/>
-    <row r="959" ht="14.25" customHeight="1"/>
-    <row r="960" ht="14.25" customHeight="1"/>
-    <row r="961" ht="14.25" customHeight="1"/>
-    <row r="962" ht="14.25" customHeight="1"/>
-    <row r="963" ht="14.25" customHeight="1"/>
-    <row r="964" ht="14.25" customHeight="1"/>
-    <row r="965" ht="14.25" customHeight="1"/>
-    <row r="966" ht="14.25" customHeight="1"/>
-    <row r="967" ht="14.25" customHeight="1"/>
-    <row r="968" ht="14.25" customHeight="1"/>
-    <row r="969" ht="14.25" customHeight="1"/>
-    <row r="970" ht="14.25" customHeight="1"/>
-    <row r="971" ht="14.25" customHeight="1"/>
-    <row r="972" ht="14.25" customHeight="1"/>
-    <row r="973" ht="14.25" customHeight="1"/>
-    <row r="974" ht="14.25" customHeight="1"/>
-    <row r="975" ht="14.25" customHeight="1"/>
-    <row r="976" ht="14.25" customHeight="1"/>
-    <row r="977" ht="14.25" customHeight="1"/>
-    <row r="978" ht="14.25" customHeight="1"/>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
-    <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>573</v>
+      </c>
+      <c r="B18" t="s">
+        <v>587</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="23"/>
+  <phoneticPr fontId="24"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z22"/>
+  <dimension ref="A1:Z24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -4460,11 +3571,12 @@
       <c r="B2" t="s">
         <v>496</v>
       </c>
-      <c r="C2" t="s">
-        <v>538</v>
+      <c r="C2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
       <c r="D2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -4474,8 +3586,9 @@
       <c r="B3" t="s">
         <v>498</v>
       </c>
-      <c r="C3" t="s">
-        <v>538</v>
+      <c r="C3" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -4485,8 +3598,9 @@
       <c r="B4" t="s">
         <v>499</v>
       </c>
-      <c r="C4" t="s">
-        <v>538</v>
+      <c r="C4" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -4496,8 +3610,9 @@
       <c r="B5" t="s">
         <v>500</v>
       </c>
-      <c r="C5" t="s">
-        <v>538</v>
+      <c r="C5" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -4507,8 +3622,9 @@
       <c r="B6" t="s">
         <v>501</v>
       </c>
-      <c r="C6" t="s">
-        <v>538</v>
+      <c r="C6" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -4518,8 +3634,9 @@
       <c r="B7" t="s">
         <v>502</v>
       </c>
-      <c r="C7" t="s">
-        <v>538</v>
+      <c r="C7" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -4527,10 +3644,11 @@
         <v>101</v>
       </c>
       <c r="B8" t="s">
-        <v>531</v>
-      </c>
-      <c r="C8" t="s">
-        <v>538</v>
+        <v>530</v>
+      </c>
+      <c r="C8" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -4540,8 +3658,9 @@
       <c r="B9" t="s">
         <v>503</v>
       </c>
-      <c r="C9" t="s">
-        <v>538</v>
+      <c r="C9" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -4549,10 +3668,11 @@
         <v>520</v>
       </c>
       <c r="B10" t="s">
-        <v>523</v>
-      </c>
-      <c r="C10" t="s">
-        <v>538</v>
+        <v>522</v>
+      </c>
+      <c r="C10" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -4560,10 +3680,11 @@
         <v>521</v>
       </c>
       <c r="B11" t="s">
-        <v>524</v>
-      </c>
-      <c r="C11" t="s">
-        <v>538</v>
+        <v>523</v>
+      </c>
+      <c r="C11" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="12" spans="1:26">
@@ -4573,8 +3694,9 @@
       <c r="B12" t="s">
         <v>504</v>
       </c>
-      <c r="C12" t="s">
-        <v>538</v>
+      <c r="C12" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="13" spans="1:26">
@@ -4584,8 +3706,9 @@
       <c r="B13" t="s">
         <v>505</v>
       </c>
-      <c r="C13" t="s">
-        <v>538</v>
+      <c r="C13" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="14" spans="1:26">
@@ -4595,8 +3718,9 @@
       <c r="B14" t="s">
         <v>506</v>
       </c>
-      <c r="C14" t="s">
-        <v>538</v>
+      <c r="C14" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="15" spans="1:26">
@@ -4606,8 +3730,9 @@
       <c r="B15" t="s">
         <v>507</v>
       </c>
-      <c r="C15" t="s">
-        <v>538</v>
+      <c r="C15" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="16" spans="1:26">
@@ -4615,10 +3740,11 @@
         <v>310</v>
       </c>
       <c r="B16" t="s">
-        <v>525</v>
-      </c>
-      <c r="C16" t="s">
-        <v>538</v>
+        <v>524</v>
+      </c>
+      <c r="C16" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -4626,79 +3752,109 @@
         <v>311</v>
       </c>
       <c r="B17" t="s">
+        <v>525</v>
+      </c>
+      <c r="C17" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="27" t="s">
+        <v>579</v>
+      </c>
+      <c r="B18" t="s">
+        <v>580</v>
+      </c>
+      <c r="C18" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="27" t="s">
+        <v>581</v>
+      </c>
+      <c r="B19" t="s">
+        <v>582</v>
+      </c>
+      <c r="C19" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="21" t="s">
+        <v>508</v>
+      </c>
+      <c r="B20" t="s">
+        <v>509</v>
+      </c>
+      <c r="C20" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>372</v>
+      </c>
+      <c r="B21" t="s">
         <v>526</v>
       </c>
-      <c r="C17" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="21" t="s">
-        <v>508</v>
-      </c>
-      <c r="B18" t="s">
-        <v>509</v>
-      </c>
-      <c r="C18" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>372</v>
-      </c>
-      <c r="B19" t="s">
-        <v>527</v>
-      </c>
-      <c r="C19" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="26" t="s">
-        <v>373</v>
-      </c>
-      <c r="B20" t="s">
-        <v>528</v>
-      </c>
-      <c r="C20" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="B21" t="s">
-        <v>532</v>
-      </c>
-      <c r="C21" t="s">
-        <v>538</v>
+      <c r="C21" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="26" t="s">
+        <v>373</v>
+      </c>
+      <c r="B22" t="s">
+        <v>527</v>
+      </c>
+      <c r="C22" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="B23" t="s">
+        <v>531</v>
+      </c>
+      <c r="C23" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="26" t="s">
+        <v>566</v>
+      </c>
+      <c r="B24" t="s">
         <v>567</v>
       </c>
-      <c r="B22" t="s">
-        <v>568</v>
-      </c>
-      <c r="C22" t="s">
-        <v>538</v>
+      <c r="C24" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P002_090_PayCycleAfternoon")</f>
+        <v>PROD/P002_090_PayCycleAfternoon</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="23"/>
+  <phoneticPr fontId="24"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D9DC59-3960-42CB-B3EC-EFF452A90D4F}">
-  <dimension ref="A1:Z176"/>
+  <dimension ref="A1:Z180"/>
   <sheetViews>
-    <sheetView topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="B115" sqref="B115"/>
+    <sheetView topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4800,407 +3956,407 @@
     </row>
     <row r="9" spans="1:26">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>583</v>
       </c>
       <c r="B9" t="s">
-        <v>97</v>
+        <v>584</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>585</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>586</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" t="s">
-        <v>142</v>
+        <v>93</v>
       </c>
       <c r="B11" t="s">
-        <v>145</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" t="s">
-        <v>561</v>
+        <v>94</v>
       </c>
       <c r="B12" t="s">
-        <v>565</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" t="s">
-        <v>562</v>
+        <v>142</v>
       </c>
       <c r="B13" t="s">
-        <v>566</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="B14" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" t="s">
-        <v>147</v>
+        <v>561</v>
       </c>
       <c r="B15" t="s">
-        <v>152</v>
+        <v>565</v>
       </c>
     </row>
     <row r="16" spans="1:26">
       <c r="A16" t="s">
-        <v>148</v>
+        <v>562</v>
       </c>
       <c r="B16" t="s">
-        <v>151</v>
+        <v>565</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>564</v>
+        <v>147</v>
       </c>
       <c r="B17" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>150</v>
+        <v>563</v>
       </c>
       <c r="B19" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="B20" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="B22" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="B23" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B24" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B25" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="B26" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B27" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B28" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="B29" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B30" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>482</v>
+        <v>175</v>
       </c>
       <c r="B31" t="s">
-        <v>483</v>
+        <v>174</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B32" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>181</v>
+        <v>482</v>
       </c>
       <c r="B33" t="s">
-        <v>182</v>
+        <v>483</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B34" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B35" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B36" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B37" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B38" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B39" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B40" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>169</v>
+        <v>190</v>
       </c>
       <c r="B41" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="B42" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B43" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="B44" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>359</v>
+        <v>171</v>
       </c>
       <c r="B45" t="s">
-        <v>360</v>
+        <v>197</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>354</v>
+        <v>200</v>
       </c>
       <c r="B46" t="s">
-        <v>361</v>
+        <v>199</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="B47" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B48" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B49" t="s">
-        <v>432</v>
+        <v>362</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B50" t="s">
-        <v>432</v>
+        <v>363</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>206</v>
+        <v>357</v>
       </c>
       <c r="B51" t="s">
-        <v>364</v>
+        <v>432</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>207</v>
+        <v>358</v>
       </c>
       <c r="B52" t="s">
-        <v>364</v>
+        <v>432</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="B53" t="s">
-        <v>208</v>
+        <v>364</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="B54" t="s">
-        <v>209</v>
+        <v>364</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="B55" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="B56" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="B57" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B58" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B59" t="s">
         <v>216</v>
@@ -5208,26 +4364,26 @@
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="B60" t="s">
-        <v>365</v>
+        <v>221</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>544</v>
+        <v>219</v>
       </c>
       <c r="B61" t="s">
-        <v>542</v>
+        <v>216</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>545</v>
+        <v>229</v>
       </c>
       <c r="B62" t="s">
-        <v>542</v>
+        <v>365</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -5235,911 +4391,943 @@
         <v>543</v>
       </c>
       <c r="B63" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>368</v>
+        <v>544</v>
       </c>
       <c r="B64" t="s">
-        <v>370</v>
+        <v>541</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>463</v>
+        <v>542</v>
       </c>
       <c r="B65" t="s">
-        <v>464</v>
+        <v>545</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B66" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>211</v>
+        <v>463</v>
       </c>
       <c r="B67" t="s">
-        <v>214</v>
+        <v>464</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>212</v>
+        <v>369</v>
       </c>
       <c r="B68" t="s">
-        <v>215</v>
+        <v>371</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="B69" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="B70" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B71" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B72" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B73" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>446</v>
+        <v>229</v>
       </c>
       <c r="B74" t="s">
-        <v>445</v>
+        <v>230</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B75" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>237</v>
+        <v>446</v>
       </c>
       <c r="B76" t="s">
-        <v>235</v>
+        <v>445</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B77" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B78" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B79" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B80" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="B81" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>555</v>
+        <v>242</v>
       </c>
       <c r="B82" t="s">
-        <v>554</v>
+        <v>244</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B83" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>252</v>
+        <v>554</v>
       </c>
       <c r="B84" t="s">
-        <v>253</v>
+        <v>553</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>514</v>
+        <v>251</v>
       </c>
       <c r="B85" t="s">
-        <v>515</v>
+        <v>250</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>556</v>
+        <v>252</v>
       </c>
       <c r="B86" t="s">
-        <v>559</v>
+        <v>253</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>557</v>
+        <v>514</v>
       </c>
       <c r="B87" t="s">
-        <v>560</v>
+        <v>515</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
+        <v>555</v>
+      </c>
+      <c r="B88" t="s">
         <v>558</v>
-      </c>
-      <c r="B88" t="s">
-        <v>560</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>245</v>
+        <v>556</v>
       </c>
       <c r="B89" t="s">
-        <v>247</v>
+        <v>559</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>246</v>
+        <v>557</v>
       </c>
       <c r="B90" t="s">
-        <v>254</v>
+        <v>559</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>473</v>
+        <v>245</v>
       </c>
       <c r="B91" t="s">
-        <v>486</v>
+        <v>247</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="B92" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>262</v>
+        <v>473</v>
       </c>
       <c r="B93" t="s">
-        <v>467</v>
+        <v>486</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>469</v>
+        <v>261</v>
       </c>
       <c r="B94" t="s">
-        <v>470</v>
+        <v>260</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>466</v>
+        <v>262</v>
       </c>
       <c r="B95" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>271</v>
+        <v>469</v>
       </c>
       <c r="B96" t="s">
-        <v>270</v>
+        <v>470</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>273</v>
+        <v>466</v>
       </c>
       <c r="B97" t="s">
-        <v>272</v>
+        <v>468</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>516</v>
+        <v>569</v>
       </c>
       <c r="B98" t="s">
-        <v>517</v>
+        <v>570</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>474</v>
+        <v>271</v>
       </c>
       <c r="B99" t="s">
-        <v>487</v>
+        <v>270</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>475</v>
+        <v>273</v>
       </c>
       <c r="B100" t="s">
-        <v>488</v>
+        <v>272</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>476</v>
+        <v>516</v>
       </c>
       <c r="B101" t="s">
-        <v>489</v>
+        <v>517</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>276</v>
+        <v>474</v>
       </c>
       <c r="B102" t="s">
-        <v>279</v>
+        <v>487</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>283</v>
+        <v>475</v>
       </c>
       <c r="B103" t="s">
-        <v>282</v>
+        <v>488</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>284</v>
+        <v>476</v>
       </c>
       <c r="B104" t="s">
-        <v>451</v>
+        <v>489</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>450</v>
+        <v>276</v>
       </c>
       <c r="B105" t="s">
-        <v>451</v>
+        <v>279</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>453</v>
+        <v>283</v>
       </c>
       <c r="B106" t="s">
-        <v>452</v>
+        <v>282</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>454</v>
+        <v>284</v>
       </c>
       <c r="B107" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>277</v>
+        <v>450</v>
       </c>
       <c r="B108" t="s">
-        <v>280</v>
+        <v>451</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>278</v>
+        <v>453</v>
       </c>
       <c r="B109" t="s">
-        <v>281</v>
+        <v>452</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>108</v>
+        <v>454</v>
       </c>
       <c r="B110" t="s">
-        <v>107</v>
+        <v>455</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>112</v>
+        <v>277</v>
       </c>
       <c r="B111" t="s">
-        <v>113</v>
+        <v>280</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="B112" t="s">
-        <v>114</v>
+        <v>281</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B113" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B115" t="s">
-        <v>569</v>
+        <v>114</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B116" t="s">
-        <v>425</v>
+        <v>111</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B117" t="s">
-        <v>424</v>
+        <v>116</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>120</v>
+        <v>568</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>352</v>
+        <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>353</v>
+        <v>425</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>126</v>
+        <v>424</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B121" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>128</v>
+        <v>352</v>
       </c>
       <c r="B122" t="s">
-        <v>129</v>
+        <v>353</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B123" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B124" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B125" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B126" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="B127" t="s">
-        <v>286</v>
+        <v>133</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="B128" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="B129" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>322</v>
+        <v>122</v>
       </c>
       <c r="B130" t="s">
-        <v>323</v>
+        <v>286</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>426</v>
+        <v>123</v>
       </c>
       <c r="B131" t="s">
-        <v>428</v>
+        <v>138</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>427</v>
+        <v>124</v>
       </c>
       <c r="B132" t="s">
-        <v>429</v>
+        <v>137</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B133" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>326</v>
+        <v>426</v>
       </c>
       <c r="B134" t="s">
-        <v>327</v>
+        <v>428</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>376</v>
+        <v>427</v>
       </c>
       <c r="B135" t="s">
-        <v>383</v>
+        <v>429</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>379</v>
+        <v>324</v>
       </c>
       <c r="B136" t="s">
-        <v>387</v>
+        <v>325</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>380</v>
+        <v>326</v>
       </c>
       <c r="B137" t="s">
-        <v>386</v>
+        <v>327</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="B138" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B139" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="B140" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="B141" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="B142" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B143" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="B144" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>398</v>
+        <v>378</v>
       </c>
       <c r="B145" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="B146" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B147" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="B148" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B149" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>536</v>
+        <v>395</v>
       </c>
       <c r="B150" t="s">
-        <v>533</v>
+        <v>393</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>407</v>
+        <v>396</v>
       </c>
       <c r="B151" t="s">
-        <v>534</v>
+        <v>394</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="B152" t="s">
-        <v>535</v>
+        <v>403</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>406</v>
+        <v>535</v>
       </c>
       <c r="B153" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B154" t="s">
-        <v>412</v>
+        <v>533</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B155" t="s">
-        <v>413</v>
+        <v>534</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="B156" t="s">
-        <v>416</v>
+        <v>536</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="B157" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>418</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>419</v>
+        <v>411</v>
+      </c>
+      <c r="B158" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="159" spans="1:2">
-      <c r="A159" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="B159" s="2" t="s">
-        <v>449</v>
+      <c r="A159" t="s">
+        <v>414</v>
+      </c>
+      <c r="B159" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>401</v>
+        <v>415</v>
       </c>
       <c r="B160" t="s">
-        <v>404</v>
+        <v>417</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>402</v>
-      </c>
-      <c r="B161" t="s">
-        <v>405</v>
+        <v>418</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="162" spans="1:2">
-      <c r="A162" t="s">
-        <v>256</v>
-      </c>
-      <c r="B162" t="s">
-        <v>255</v>
+      <c r="A162" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>433</v>
+        <v>401</v>
       </c>
       <c r="B163" t="s">
-        <v>361</v>
+        <v>404</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>434</v>
+        <v>402</v>
       </c>
       <c r="B164" t="s">
-        <v>362</v>
+        <v>405</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>435</v>
+        <v>256</v>
       </c>
       <c r="B165" t="s">
-        <v>363</v>
+        <v>255</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B166" t="s">
-        <v>432</v>
+        <v>361</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B167" t="s">
-        <v>432</v>
+        <v>362</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B168" t="s">
-        <v>441</v>
+        <v>363</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B169" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B170" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>268</v>
+        <v>438</v>
       </c>
       <c r="B171" t="s">
-        <v>485</v>
+        <v>441</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>477</v>
+        <v>439</v>
       </c>
       <c r="B172" t="s">
-        <v>480</v>
+        <v>442</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
-        <v>478</v>
+        <v>440</v>
       </c>
       <c r="B173" t="s">
-        <v>481</v>
+        <v>442</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" t="s">
-        <v>479</v>
+        <v>268</v>
       </c>
       <c r="B174" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" t="s">
-        <v>257</v>
+        <v>477</v>
       </c>
       <c r="B175" t="s">
-        <v>274</v>
+        <v>480</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" t="s">
+        <v>478</v>
+      </c>
+      <c r="B176" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="A177" t="s">
+        <v>479</v>
+      </c>
+      <c r="B177" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="A178" t="s">
+        <v>257</v>
+      </c>
+      <c r="B178" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="A179" t="s">
         <v>258</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B179" t="s">
         <v>275</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2">
+      <c r="A180" t="s">
+        <v>571</v>
+      </c>
+      <c r="B180" t="s">
+        <v>572</v>
       </c>
     </row>
   </sheetData>

</xml_diff>